<commit_message>
se agregan criterios de aceptacion para el modelo de autorizacion
</commit_message>
<xml_diff>
--- a/src/test/resources/data_driven/EstructuraServicio.xlsx
+++ b/src/test/resources/data_driven/EstructuraServicio.xlsx
@@ -380,7 +380,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="208">
   <si>
     <t>Buscar Auxiliares de expedición asociados al parámetro + Su ubicación física de acuerdo al código de oficina</t>
   </si>
@@ -1000,16 +1000,16 @@
     <t>11868</t>
   </si>
   <si>
-    <t>Valor Asegurado</t>
-  </si>
-  <si>
     <t>Maria Angelica</t>
   </si>
   <si>
     <t>Luis Saldarriaga</t>
   </si>
   <si>
-    <t>Paola Rosa</t>
+    <t>valor asegurado</t>
+  </si>
+  <si>
+    <t>CAROLINA MARTINEZ MOLINA</t>
   </si>
 </sst>
 </file>
@@ -1088,7 +1088,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1146,6 +1146,15 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -1212,9 +1221,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -3812,48 +3819,49 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="B1" t="s">
         <v>204</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="B2" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="7" t="s">
+      <c r="B3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C3" t="s">
-        <v>207</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:A3"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agregan criterios de aceptacion para la automatización del modelo de autorizaciones
</commit_message>
<xml_diff>
--- a/src/test/resources/data_driven/EstructuraServicio.xlsx
+++ b/src/test/resources/data_driven/EstructuraServicio.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="465" windowWidth="19875" windowHeight="6630" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="525" windowWidth="19875" windowHeight="6570" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Estructura" sheetId="1" r:id="rId1"/>
@@ -380,7 +380,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="226">
   <si>
     <t>Buscar Auxiliares de expedición asociados al parámetro + Su ubicación física de acuerdo al código de oficina</t>
   </si>
@@ -1006,10 +1006,64 @@
     <t>Luis Saldarriaga</t>
   </si>
   <si>
-    <t>valor asegurado</t>
-  </si>
-  <si>
     <t>CAROLINA MARTINEZ MOLINA</t>
+  </si>
+  <si>
+    <t>El valor asegurado del vehículo ($405.000.000,00) supera el límite máximo permitido por políticas. El aseguramiento de este carro así como la oferta presentada al cliente, deben ser avalados previamente por el Comité de Riesgo No Estándar Autos</t>
+  </si>
+  <si>
+    <t>NATALIA MOLINA GRANADOS</t>
+  </si>
+  <si>
+    <t>El Valor del vehiculo no se encuentra en los rangos estimados por Suramericana</t>
+  </si>
+  <si>
+    <t>CRISTIAN FRANCISCO RODRIGUEZ RAMIREZ</t>
+  </si>
+  <si>
+    <t>Por política de la compañía este vehículo no puede ser asegurado.</t>
+  </si>
+  <si>
+    <t>ANA MARIA CANO GALLEGO</t>
+  </si>
+  <si>
+    <t>El valor de los accesorios es mayor al 20% del valor Asegurado</t>
+  </si>
+  <si>
+    <t>MAYRA ALEJANDRA PEREZ GRAJALES</t>
+  </si>
+  <si>
+    <t>El valor de los accesorios especiales es mayor al valor Asegurado del vehículo. Por favor verifique.</t>
+  </si>
+  <si>
+    <t>La placa DAG64F está asegurada en la póliza 800000018775, por favor verifique.</t>
+  </si>
+  <si>
+    <t>JAISA ZAPATA MENDEZ</t>
+  </si>
+  <si>
+    <t>JUAN DIEGO CANO RAMIREZ</t>
+  </si>
+  <si>
+    <t>4029</t>
+  </si>
+  <si>
+    <t>PAOLA ANDREA RODRIGUEZ SALAZAR</t>
+  </si>
+  <si>
+    <t>USURIO PRUEBA SCRIPT PROVISIONAMIENTO</t>
+  </si>
+  <si>
+    <t>ANA JULIETA VELASQUEZ HENAO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANA JULIETA VELASQUEZ HENAO </t>
+  </si>
+  <si>
+    <t>LUIS FERNANDO SALDARRIAGA DIAZ</t>
+  </si>
+  <si>
+    <t>eliajiar</t>
   </si>
 </sst>
 </file>
@@ -1162,7 +1216,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1188,6 +1242,22 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1221,7 +1291,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1530,7 +1599,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="59.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1544,28 +1613,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="11"/>
+      <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
       <c r="E2" s="2" t="s">
         <v>27</v>
       </c>
@@ -1774,8 +1843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F134"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C24" sqref="B8:C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1808,10 +1877,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="19">
+      <c r="B2" s="27">
         <v>4029</v>
       </c>
       <c r="C2" s="6">
@@ -1828,8 +1897,8 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
-      <c r="B3" s="19"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="27"/>
       <c r="C3" s="6">
         <v>70129463</v>
       </c>
@@ -1844,8 +1913,8 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
-      <c r="B4" s="19"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="27"/>
       <c r="C4" s="6">
         <v>43596238</v>
       </c>
@@ -1860,8 +1929,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="19">
+      <c r="A5" s="28"/>
+      <c r="B5" s="27">
         <v>2527</v>
       </c>
       <c r="C5" s="8">
@@ -1876,8 +1945,8 @@
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="19"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="27"/>
       <c r="C6" s="8">
         <v>71526214</v>
       </c>
@@ -1890,8 +1959,8 @@
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
-      <c r="B7" s="19"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="27"/>
       <c r="C7" s="8">
         <v>43287144</v>
       </c>
@@ -1904,19 +1973,19 @@
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="27">
         <v>4029</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="24">
         <v>43628391</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="29" t="s">
         <v>52</v>
       </c>
       <c r="F8" s="8" t="s">
@@ -1924,99 +1993,99 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="17"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="25"/>
       <c r="D9" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="E9" s="21"/>
+      <c r="E9" s="29"/>
       <c r="F9" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="17"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="25"/>
       <c r="D10" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="21"/>
+      <c r="E10" s="29"/>
       <c r="F10" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="17"/>
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="25"/>
       <c r="D11" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="E11" s="21"/>
+      <c r="E11" s="29"/>
       <c r="F11" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="17"/>
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="25"/>
       <c r="D12" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="E12" s="21"/>
+      <c r="E12" s="29"/>
       <c r="F12" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="17"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="25"/>
       <c r="D13" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="E13" s="21"/>
+      <c r="E13" s="29"/>
       <c r="F13" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="19"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="17"/>
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="25"/>
       <c r="D14" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="E14" s="21"/>
+      <c r="E14" s="29"/>
       <c r="F14" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="18"/>
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="26"/>
       <c r="D15" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="E15" s="21"/>
+      <c r="E15" s="29"/>
       <c r="F15" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="16">
+      <c r="A16" s="27"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="24">
         <v>43618716</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="E16" s="21" t="s">
+      <c r="E16" s="29" t="s">
         <v>53</v>
       </c>
       <c r="F16" s="8" t="s">
@@ -2024,99 +2093,99 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="17"/>
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="25"/>
       <c r="D17" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="E17" s="21"/>
+      <c r="E17" s="29"/>
       <c r="F17" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="19"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="17"/>
+      <c r="A18" s="27"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="25"/>
       <c r="D18" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="E18" s="21"/>
+      <c r="E18" s="29"/>
       <c r="F18" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="19"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="17"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="25"/>
       <c r="D19" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="21"/>
+      <c r="E19" s="29"/>
       <c r="F19" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="17"/>
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="25"/>
       <c r="D20" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="E20" s="21"/>
+      <c r="E20" s="29"/>
       <c r="F20" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="17"/>
+      <c r="A21" s="27"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="25"/>
       <c r="D21" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="E21" s="21"/>
+      <c r="E21" s="29"/>
       <c r="F21" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="19"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="17"/>
+      <c r="A22" s="27"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="25"/>
       <c r="D22" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="E22" s="21"/>
+      <c r="E22" s="29"/>
       <c r="F22" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="19"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="18"/>
+      <c r="A23" s="27"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="26"/>
       <c r="D23" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="E23" s="21"/>
+      <c r="E23" s="29"/>
       <c r="F23" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="19"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="16">
+      <c r="A24" s="27"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="24">
         <v>71698481</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="E24" s="21" t="s">
+      <c r="E24" s="29" t="s">
         <v>54</v>
       </c>
       <c r="F24" s="8" t="s">
@@ -2124,99 +2193,99 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="19"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="17"/>
+      <c r="A25" s="27"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="25"/>
       <c r="D25" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="E25" s="21"/>
+      <c r="E25" s="29"/>
       <c r="F25" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="19"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="17"/>
+      <c r="A26" s="27"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="25"/>
       <c r="D26" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="E26" s="21"/>
+      <c r="E26" s="29"/>
       <c r="F26" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="19"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="17"/>
+      <c r="A27" s="27"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="25"/>
       <c r="D27" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="E27" s="21"/>
+      <c r="E27" s="29"/>
       <c r="F27" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="19"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="17"/>
+      <c r="A28" s="27"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="25"/>
       <c r="D28" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="E28" s="21"/>
+      <c r="E28" s="29"/>
       <c r="F28" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="19"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="17"/>
+      <c r="A29" s="27"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="25"/>
       <c r="D29" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="E29" s="21"/>
+      <c r="E29" s="29"/>
       <c r="F29" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="19"/>
-      <c r="B30" s="19"/>
-      <c r="C30" s="17"/>
+      <c r="A30" s="27"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="25"/>
       <c r="D30" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="E30" s="21"/>
+      <c r="E30" s="29"/>
       <c r="F30" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="19"/>
-      <c r="B31" s="19"/>
-      <c r="C31" s="18"/>
+      <c r="A31" s="27"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="26"/>
       <c r="D31" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="E31" s="21"/>
+      <c r="E31" s="29"/>
       <c r="F31" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="19"/>
-      <c r="B32" s="19"/>
-      <c r="C32" s="16">
+      <c r="A32" s="27"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="24">
         <v>43520997</v>
       </c>
       <c r="D32" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="E32" s="21" t="s">
+      <c r="E32" s="29" t="s">
         <v>55</v>
       </c>
       <c r="F32" s="8" t="s">
@@ -2224,99 +2293,99 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="19"/>
-      <c r="B33" s="19"/>
-      <c r="C33" s="17"/>
+      <c r="A33" s="27"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="25"/>
       <c r="D33" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="E33" s="21"/>
+      <c r="E33" s="29"/>
       <c r="F33" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="19"/>
-      <c r="B34" s="19"/>
-      <c r="C34" s="17"/>
+      <c r="A34" s="27"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="25"/>
       <c r="D34" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="E34" s="21"/>
+      <c r="E34" s="29"/>
       <c r="F34" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="19"/>
-      <c r="B35" s="19"/>
-      <c r="C35" s="17"/>
+      <c r="A35" s="27"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="25"/>
       <c r="D35" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="E35" s="21"/>
+      <c r="E35" s="29"/>
       <c r="F35" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="19"/>
-      <c r="B36" s="19"/>
-      <c r="C36" s="17"/>
+      <c r="A36" s="27"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="25"/>
       <c r="D36" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="E36" s="21"/>
+      <c r="E36" s="29"/>
       <c r="F36" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="19"/>
-      <c r="B37" s="19"/>
-      <c r="C37" s="17"/>
+      <c r="A37" s="27"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="25"/>
       <c r="D37" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E37" s="21"/>
+      <c r="E37" s="29"/>
       <c r="F37" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="19"/>
-      <c r="B38" s="19"/>
-      <c r="C38" s="17"/>
+      <c r="A38" s="27"/>
+      <c r="B38" s="27"/>
+      <c r="C38" s="25"/>
       <c r="D38" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="E38" s="21"/>
+      <c r="E38" s="29"/>
       <c r="F38" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="19"/>
-      <c r="B39" s="19"/>
-      <c r="C39" s="18"/>
+      <c r="A39" s="27"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="26"/>
       <c r="D39" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="E39" s="21"/>
+      <c r="E39" s="29"/>
       <c r="F39" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="19"/>
-      <c r="B40" s="19"/>
-      <c r="C40" s="16">
+      <c r="A40" s="27"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="24">
         <v>43527460</v>
       </c>
       <c r="D40" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="E40" s="21" t="s">
+      <c r="E40" s="29" t="s">
         <v>56</v>
       </c>
       <c r="F40" s="8" t="s">
@@ -2324,101 +2393,101 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="19"/>
-      <c r="B41" s="19"/>
-      <c r="C41" s="17"/>
+      <c r="A41" s="27"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="25"/>
       <c r="D41" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="E41" s="21"/>
+      <c r="E41" s="29"/>
       <c r="F41" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="19"/>
-      <c r="B42" s="19"/>
-      <c r="C42" s="17"/>
+      <c r="A42" s="27"/>
+      <c r="B42" s="27"/>
+      <c r="C42" s="25"/>
       <c r="D42" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="E42" s="21"/>
+      <c r="E42" s="29"/>
       <c r="F42" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="19"/>
-      <c r="B43" s="19"/>
-      <c r="C43" s="17"/>
+      <c r="A43" s="27"/>
+      <c r="B43" s="27"/>
+      <c r="C43" s="25"/>
       <c r="D43" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="E43" s="21"/>
+      <c r="E43" s="29"/>
       <c r="F43" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="19"/>
-      <c r="B44" s="19"/>
-      <c r="C44" s="17"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="25"/>
       <c r="D44" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="E44" s="21"/>
+      <c r="E44" s="29"/>
       <c r="F44" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="19"/>
-      <c r="B45" s="19"/>
-      <c r="C45" s="17"/>
+      <c r="A45" s="27"/>
+      <c r="B45" s="27"/>
+      <c r="C45" s="25"/>
       <c r="D45" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="E45" s="21"/>
+      <c r="E45" s="29"/>
       <c r="F45" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="19"/>
-      <c r="B46" s="19"/>
-      <c r="C46" s="17"/>
+      <c r="A46" s="27"/>
+      <c r="B46" s="27"/>
+      <c r="C46" s="25"/>
       <c r="D46" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="E46" s="21"/>
+      <c r="E46" s="29"/>
       <c r="F46" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="19"/>
-      <c r="B47" s="19"/>
-      <c r="C47" s="18"/>
+      <c r="A47" s="27"/>
+      <c r="B47" s="27"/>
+      <c r="C47" s="26"/>
       <c r="D47" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="E47" s="21"/>
+      <c r="E47" s="29"/>
       <c r="F47" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="19"/>
-      <c r="B48" s="19">
+      <c r="A48" s="27"/>
+      <c r="B48" s="27">
         <v>2527</v>
       </c>
-      <c r="C48" s="20">
+      <c r="C48" s="28">
         <v>32143454</v>
       </c>
       <c r="D48" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="E48" s="20" t="s">
+      <c r="E48" s="28" t="s">
         <v>97</v>
       </c>
       <c r="F48" s="8" t="s">
@@ -2426,99 +2495,99 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="19"/>
-      <c r="B49" s="19"/>
-      <c r="C49" s="20"/>
+      <c r="A49" s="27"/>
+      <c r="B49" s="27"/>
+      <c r="C49" s="28"/>
       <c r="D49" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="E49" s="20"/>
+      <c r="E49" s="28"/>
       <c r="F49" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="19"/>
-      <c r="B50" s="19"/>
-      <c r="C50" s="20"/>
+      <c r="A50" s="27"/>
+      <c r="B50" s="27"/>
+      <c r="C50" s="28"/>
       <c r="D50" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="E50" s="20"/>
+      <c r="E50" s="28"/>
       <c r="F50" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="19"/>
-      <c r="B51" s="19"/>
-      <c r="C51" s="20"/>
+      <c r="A51" s="27"/>
+      <c r="B51" s="27"/>
+      <c r="C51" s="28"/>
       <c r="D51" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="E51" s="20"/>
+      <c r="E51" s="28"/>
       <c r="F51" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="19"/>
-      <c r="B52" s="19"/>
-      <c r="C52" s="20"/>
+      <c r="A52" s="27"/>
+      <c r="B52" s="27"/>
+      <c r="C52" s="28"/>
       <c r="D52" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="E52" s="20"/>
+      <c r="E52" s="28"/>
       <c r="F52" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="19"/>
-      <c r="B53" s="19"/>
-      <c r="C53" s="20"/>
+      <c r="A53" s="27"/>
+      <c r="B53" s="27"/>
+      <c r="C53" s="28"/>
       <c r="D53" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="E53" s="20"/>
+      <c r="E53" s="28"/>
       <c r="F53" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="19"/>
-      <c r="B54" s="19"/>
-      <c r="C54" s="20"/>
+      <c r="A54" s="27"/>
+      <c r="B54" s="27"/>
+      <c r="C54" s="28"/>
       <c r="D54" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="E54" s="20"/>
+      <c r="E54" s="28"/>
       <c r="F54" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="19"/>
-      <c r="B55" s="19"/>
-      <c r="C55" s="20"/>
+      <c r="A55" s="27"/>
+      <c r="B55" s="27"/>
+      <c r="C55" s="28"/>
       <c r="D55" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="E55" s="20"/>
+      <c r="E55" s="28"/>
       <c r="F55" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="19"/>
-      <c r="B56" s="19"/>
-      <c r="C56" s="20">
+      <c r="A56" s="27"/>
+      <c r="B56" s="27"/>
+      <c r="C56" s="28">
         <v>42790786</v>
       </c>
       <c r="D56" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="E56" s="20" t="s">
+      <c r="E56" s="28" t="s">
         <v>98</v>
       </c>
       <c r="F56" s="8" t="s">
@@ -2526,91 +2595,91 @@
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="19"/>
-      <c r="B57" s="19"/>
-      <c r="C57" s="20"/>
+      <c r="A57" s="27"/>
+      <c r="B57" s="27"/>
+      <c r="C57" s="28"/>
       <c r="D57" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="E57" s="20"/>
+      <c r="E57" s="28"/>
       <c r="F57" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="19"/>
-      <c r="B58" s="19"/>
-      <c r="C58" s="20"/>
+      <c r="A58" s="27"/>
+      <c r="B58" s="27"/>
+      <c r="C58" s="28"/>
       <c r="D58" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="E58" s="20"/>
+      <c r="E58" s="28"/>
       <c r="F58" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="19"/>
-      <c r="B59" s="19"/>
-      <c r="C59" s="20"/>
+      <c r="A59" s="27"/>
+      <c r="B59" s="27"/>
+      <c r="C59" s="28"/>
       <c r="D59" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="E59" s="20"/>
+      <c r="E59" s="28"/>
       <c r="F59" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="19"/>
-      <c r="B60" s="19"/>
-      <c r="C60" s="20"/>
+      <c r="A60" s="27"/>
+      <c r="B60" s="27"/>
+      <c r="C60" s="28"/>
       <c r="D60" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="E60" s="20"/>
+      <c r="E60" s="28"/>
       <c r="F60" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="19"/>
-      <c r="B61" s="19"/>
-      <c r="C61" s="20"/>
+      <c r="A61" s="27"/>
+      <c r="B61" s="27"/>
+      <c r="C61" s="28"/>
       <c r="D61" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="E61" s="20"/>
+      <c r="E61" s="28"/>
       <c r="F61" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="19"/>
-      <c r="B62" s="19"/>
-      <c r="C62" s="20"/>
+      <c r="A62" s="27"/>
+      <c r="B62" s="27"/>
+      <c r="C62" s="28"/>
       <c r="D62" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="E62" s="20"/>
+      <c r="E62" s="28"/>
       <c r="F62" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="19"/>
-      <c r="B63" s="19"/>
-      <c r="C63" s="20"/>
+      <c r="A63" s="27"/>
+      <c r="B63" s="27"/>
+      <c r="C63" s="28"/>
       <c r="D63" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="E63" s="20"/>
+      <c r="E63" s="28"/>
       <c r="F63" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="19" t="s">
+      <c r="A64" s="27" t="s">
         <v>34</v>
       </c>
       <c r="B64" s="4">
@@ -2630,7 +2699,7 @@
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="19"/>
+      <c r="A65" s="27"/>
       <c r="B65" s="4">
         <v>2527</v>
       </c>
@@ -2648,10 +2717,10 @@
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="19" t="s">
+      <c r="A66" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="B66" s="19" t="s">
+      <c r="B66" s="27" t="s">
         <v>51</v>
       </c>
       <c r="C66" s="8" t="s">
@@ -2668,8 +2737,8 @@
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="19"/>
-      <c r="B67" s="19"/>
+      <c r="A67" s="27"/>
+      <c r="B67" s="27"/>
       <c r="C67" s="8" t="s">
         <v>117</v>
       </c>
@@ -2684,8 +2753,8 @@
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="19"/>
-      <c r="B68" s="19"/>
+      <c r="A68" s="27"/>
+      <c r="B68" s="27"/>
       <c r="C68" s="8" t="s">
         <v>118</v>
       </c>
@@ -2700,8 +2769,8 @@
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="19"/>
-      <c r="B69" s="19"/>
+      <c r="A69" s="27"/>
+      <c r="B69" s="27"/>
       <c r="C69" s="8" t="s">
         <v>119</v>
       </c>
@@ -2716,8 +2785,8 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="19"/>
-      <c r="B70" s="19"/>
+      <c r="A70" s="27"/>
+      <c r="B70" s="27"/>
       <c r="C70" s="8" t="s">
         <v>120</v>
       </c>
@@ -2732,8 +2801,8 @@
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="19"/>
-      <c r="B71" s="19"/>
+      <c r="A71" s="27"/>
+      <c r="B71" s="27"/>
       <c r="C71" s="8" t="s">
         <v>121</v>
       </c>
@@ -2748,8 +2817,8 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="19"/>
-      <c r="B72" s="19"/>
+      <c r="A72" s="27"/>
+      <c r="B72" s="27"/>
       <c r="C72" s="8" t="s">
         <v>122</v>
       </c>
@@ -2764,8 +2833,8 @@
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="19"/>
-      <c r="B73" s="19"/>
+      <c r="A73" s="27"/>
+      <c r="B73" s="27"/>
       <c r="C73" s="8" t="s">
         <v>123</v>
       </c>
@@ -2780,8 +2849,8 @@
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="19"/>
-      <c r="B74" s="19"/>
+      <c r="A74" s="27"/>
+      <c r="B74" s="27"/>
       <c r="C74" s="8" t="s">
         <v>124</v>
       </c>
@@ -2796,8 +2865,8 @@
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="19"/>
-      <c r="B75" s="19"/>
+      <c r="A75" s="27"/>
+      <c r="B75" s="27"/>
       <c r="C75" s="8" t="s">
         <v>125</v>
       </c>
@@ -2812,8 +2881,8 @@
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="19"/>
-      <c r="B76" s="19"/>
+      <c r="A76" s="27"/>
+      <c r="B76" s="27"/>
       <c r="C76" s="8" t="s">
         <v>126</v>
       </c>
@@ -2828,8 +2897,8 @@
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="19"/>
-      <c r="B77" s="19"/>
+      <c r="A77" s="27"/>
+      <c r="B77" s="27"/>
       <c r="C77" s="8" t="s">
         <v>127</v>
       </c>
@@ -2844,8 +2913,8 @@
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="19"/>
-      <c r="B78" s="19"/>
+      <c r="A78" s="27"/>
+      <c r="B78" s="27"/>
       <c r="C78" s="8" t="s">
         <v>128</v>
       </c>
@@ -2860,10 +2929,10 @@
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="19" t="s">
+      <c r="A79" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="B79" s="19">
+      <c r="B79" s="27">
         <v>4029</v>
       </c>
       <c r="C79" s="8" t="s">
@@ -2880,8 +2949,8 @@
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="19"/>
-      <c r="B80" s="19"/>
+      <c r="A80" s="27"/>
+      <c r="B80" s="27"/>
       <c r="C80" s="8" t="s">
         <v>146</v>
       </c>
@@ -2896,8 +2965,8 @@
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="19"/>
-      <c r="B81" s="19"/>
+      <c r="A81" s="27"/>
+      <c r="B81" s="27"/>
       <c r="C81" s="8" t="s">
         <v>147</v>
       </c>
@@ -2912,8 +2981,8 @@
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="19"/>
-      <c r="B82" s="19"/>
+      <c r="A82" s="27"/>
+      <c r="B82" s="27"/>
       <c r="C82" s="8" t="s">
         <v>148</v>
       </c>
@@ -2928,8 +2997,8 @@
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="19"/>
-      <c r="B83" s="19"/>
+      <c r="A83" s="27"/>
+      <c r="B83" s="27"/>
       <c r="C83" s="8" t="s">
         <v>149</v>
       </c>
@@ -2944,8 +3013,8 @@
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="19"/>
-      <c r="B84" s="19"/>
+      <c r="A84" s="27"/>
+      <c r="B84" s="27"/>
       <c r="C84" s="8" t="s">
         <v>150</v>
       </c>
@@ -2960,8 +3029,8 @@
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="19"/>
-      <c r="B85" s="19"/>
+      <c r="A85" s="27"/>
+      <c r="B85" s="27"/>
       <c r="C85" s="8" t="s">
         <v>151</v>
       </c>
@@ -2976,7 +3045,7 @@
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="19" t="s">
+      <c r="A86" s="27" t="s">
         <v>37</v>
       </c>
       <c r="B86" s="4">
@@ -2996,7 +3065,7 @@
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="19"/>
+      <c r="A87" s="27"/>
       <c r="B87" s="4">
         <v>3108</v>
       </c>
@@ -3014,7 +3083,7 @@
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="19" t="s">
+      <c r="A88" s="27" t="s">
         <v>39</v>
       </c>
       <c r="B88" s="4">
@@ -3034,7 +3103,7 @@
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="19"/>
+      <c r="A89" s="27"/>
       <c r="B89" s="4">
         <v>3152</v>
       </c>
@@ -3052,7 +3121,7 @@
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="19"/>
+      <c r="A90" s="27"/>
       <c r="B90" s="4">
         <v>3152</v>
       </c>
@@ -3070,7 +3139,7 @@
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="19" t="s">
+      <c r="A91" s="27" t="s">
         <v>38</v>
       </c>
       <c r="B91" s="4">
@@ -3090,7 +3159,7 @@
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="19"/>
+      <c r="A92" s="27"/>
       <c r="B92" s="4">
         <v>3152</v>
       </c>
@@ -3108,7 +3177,7 @@
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="19"/>
+      <c r="A93" s="27"/>
       <c r="B93" s="4">
         <v>3152</v>
       </c>
@@ -3126,7 +3195,7 @@
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="19"/>
+      <c r="A94" s="27"/>
       <c r="B94" s="4">
         <v>3152</v>
       </c>
@@ -3144,7 +3213,7 @@
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="19"/>
+      <c r="A95" s="27"/>
       <c r="B95" s="4">
         <v>3152</v>
       </c>
@@ -3162,7 +3231,7 @@
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="19"/>
+      <c r="A96" s="27"/>
       <c r="B96" s="4">
         <v>3152</v>
       </c>
@@ -3180,7 +3249,7 @@
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="19"/>
+      <c r="A97" s="27"/>
       <c r="B97" s="4">
         <v>3152</v>
       </c>
@@ -3198,7 +3267,7 @@
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="19"/>
+      <c r="A98" s="27"/>
       <c r="B98" s="4">
         <v>3152</v>
       </c>
@@ -3216,7 +3285,7 @@
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="19"/>
+      <c r="A99" s="27"/>
       <c r="B99" s="4">
         <v>3152</v>
       </c>
@@ -3234,7 +3303,7 @@
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="19"/>
+      <c r="A100" s="27"/>
       <c r="B100" s="4">
         <v>3152</v>
       </c>
@@ -3252,7 +3321,7 @@
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="19"/>
+      <c r="A101" s="27"/>
       <c r="B101" s="4">
         <v>3152</v>
       </c>
@@ -3270,7 +3339,7 @@
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" s="19"/>
+      <c r="A102" s="27"/>
       <c r="B102" s="4">
         <v>3152</v>
       </c>
@@ -3288,7 +3357,7 @@
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="19"/>
+      <c r="A103" s="27"/>
       <c r="B103" s="4">
         <v>3108</v>
       </c>
@@ -3306,7 +3375,7 @@
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" s="19"/>
+      <c r="A104" s="27"/>
       <c r="B104" s="4">
         <v>3108</v>
       </c>
@@ -3324,7 +3393,7 @@
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="19"/>
+      <c r="A105" s="27"/>
       <c r="B105" s="4">
         <v>3108</v>
       </c>
@@ -3342,7 +3411,7 @@
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" s="19"/>
+      <c r="A106" s="27"/>
       <c r="B106" s="4">
         <v>3108</v>
       </c>
@@ -3360,7 +3429,7 @@
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107" s="19"/>
+      <c r="A107" s="27"/>
       <c r="B107" s="4">
         <v>3108</v>
       </c>
@@ -3378,7 +3447,7 @@
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A108" s="19"/>
+      <c r="A108" s="27"/>
       <c r="B108" s="4">
         <v>3108</v>
       </c>
@@ -3396,13 +3465,13 @@
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109" s="16" t="s">
+      <c r="A109" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="B109" s="16">
+      <c r="B109" s="24">
         <v>4029</v>
       </c>
-      <c r="C109" s="13">
+      <c r="C109" s="21">
         <v>1128271593</v>
       </c>
       <c r="D109" s="4" t="s">
@@ -3416,9 +3485,9 @@
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A110" s="17"/>
-      <c r="B110" s="17"/>
-      <c r="C110" s="14"/>
+      <c r="A110" s="25"/>
+      <c r="B110" s="25"/>
+      <c r="C110" s="22"/>
       <c r="D110" s="4" t="s">
         <v>189</v>
       </c>
@@ -3430,9 +3499,9 @@
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A111" s="17"/>
-      <c r="B111" s="17"/>
-      <c r="C111" s="14"/>
+      <c r="A111" s="25"/>
+      <c r="B111" s="25"/>
+      <c r="C111" s="22"/>
       <c r="D111" s="4" t="s">
         <v>190</v>
       </c>
@@ -3444,9 +3513,9 @@
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A112" s="17"/>
-      <c r="B112" s="17"/>
-      <c r="C112" s="14"/>
+      <c r="A112" s="25"/>
+      <c r="B112" s="25"/>
+      <c r="C112" s="22"/>
       <c r="D112" s="4" t="s">
         <v>191</v>
       </c>
@@ -3458,9 +3527,9 @@
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A113" s="17"/>
-      <c r="B113" s="17"/>
-      <c r="C113" s="14"/>
+      <c r="A113" s="25"/>
+      <c r="B113" s="25"/>
+      <c r="C113" s="22"/>
       <c r="D113" s="4" t="s">
         <v>192</v>
       </c>
@@ -3472,9 +3541,9 @@
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A114" s="17"/>
-      <c r="B114" s="17"/>
-      <c r="C114" s="14"/>
+      <c r="A114" s="25"/>
+      <c r="B114" s="25"/>
+      <c r="C114" s="22"/>
       <c r="D114" s="4" t="s">
         <v>193</v>
       </c>
@@ -3486,9 +3555,9 @@
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A115" s="17"/>
-      <c r="B115" s="17"/>
-      <c r="C115" s="14"/>
+      <c r="A115" s="25"/>
+      <c r="B115" s="25"/>
+      <c r="C115" s="22"/>
       <c r="D115" s="4" t="s">
         <v>194</v>
       </c>
@@ -3500,9 +3569,9 @@
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A116" s="17"/>
-      <c r="B116" s="17"/>
-      <c r="C116" s="14"/>
+      <c r="A116" s="25"/>
+      <c r="B116" s="25"/>
+      <c r="C116" s="22"/>
       <c r="D116" s="4" t="s">
         <v>195</v>
       </c>
@@ -3514,9 +3583,9 @@
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A117" s="17"/>
-      <c r="B117" s="17"/>
-      <c r="C117" s="14"/>
+      <c r="A117" s="25"/>
+      <c r="B117" s="25"/>
+      <c r="C117" s="22"/>
       <c r="D117" s="4" t="s">
         <v>196</v>
       </c>
@@ -3528,9 +3597,9 @@
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A118" s="17"/>
-      <c r="B118" s="17"/>
-      <c r="C118" s="15"/>
+      <c r="A118" s="25"/>
+      <c r="B118" s="25"/>
+      <c r="C118" s="23"/>
       <c r="D118" s="4" t="s">
         <v>197</v>
       </c>
@@ -3542,9 +3611,9 @@
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A119" s="17"/>
-      <c r="B119" s="17"/>
-      <c r="C119" s="16">
+      <c r="A119" s="25"/>
+      <c r="B119" s="25"/>
+      <c r="C119" s="24">
         <v>43504265</v>
       </c>
       <c r="D119" s="4" t="s">
@@ -3558,9 +3627,9 @@
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A120" s="17"/>
-      <c r="B120" s="17"/>
-      <c r="C120" s="17"/>
+      <c r="A120" s="25"/>
+      <c r="B120" s="25"/>
+      <c r="C120" s="25"/>
       <c r="D120" s="4" t="s">
         <v>199</v>
       </c>
@@ -3572,9 +3641,9 @@
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A121" s="17"/>
-      <c r="B121" s="17"/>
-      <c r="C121" s="17"/>
+      <c r="A121" s="25"/>
+      <c r="B121" s="25"/>
+      <c r="C121" s="25"/>
       <c r="D121" s="4" t="s">
         <v>70</v>
       </c>
@@ -3586,9 +3655,9 @@
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A122" s="17"/>
-      <c r="B122" s="17"/>
-      <c r="C122" s="17"/>
+      <c r="A122" s="25"/>
+      <c r="B122" s="25"/>
+      <c r="C122" s="25"/>
       <c r="D122" s="4" t="s">
         <v>200</v>
       </c>
@@ -3600,9 +3669,9 @@
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A123" s="17"/>
-      <c r="B123" s="17"/>
-      <c r="C123" s="17"/>
+      <c r="A123" s="25"/>
+      <c r="B123" s="25"/>
+      <c r="C123" s="25"/>
       <c r="D123" s="4" t="s">
         <v>71</v>
       </c>
@@ -3614,9 +3683,9 @@
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A124" s="17"/>
-      <c r="B124" s="17"/>
-      <c r="C124" s="17"/>
+      <c r="A124" s="25"/>
+      <c r="B124" s="25"/>
+      <c r="C124" s="25"/>
       <c r="D124" s="4" t="s">
         <v>201</v>
       </c>
@@ -3628,9 +3697,9 @@
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A125" s="17"/>
-      <c r="B125" s="17"/>
-      <c r="C125" s="17"/>
+      <c r="A125" s="25"/>
+      <c r="B125" s="25"/>
+      <c r="C125" s="25"/>
       <c r="D125" s="4" t="s">
         <v>202</v>
       </c>
@@ -3642,9 +3711,9 @@
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A126" s="17"/>
-      <c r="B126" s="18"/>
-      <c r="C126" s="18"/>
+      <c r="A126" s="25"/>
+      <c r="B126" s="26"/>
+      <c r="C126" s="26"/>
       <c r="D126" s="4" t="s">
         <v>72</v>
       </c>
@@ -3656,11 +3725,11 @@
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A127" s="17"/>
-      <c r="B127" s="16">
+      <c r="A127" s="25"/>
+      <c r="B127" s="24">
         <v>2597</v>
       </c>
-      <c r="C127" s="16">
+      <c r="C127" s="24">
         <v>1128278017</v>
       </c>
       <c r="D127" s="4" t="s">
@@ -3674,9 +3743,9 @@
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A128" s="17"/>
-      <c r="B128" s="17"/>
-      <c r="C128" s="17"/>
+      <c r="A128" s="25"/>
+      <c r="B128" s="25"/>
+      <c r="C128" s="25"/>
       <c r="D128" s="4" t="s">
         <v>109</v>
       </c>
@@ -3688,9 +3757,9 @@
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A129" s="17"/>
-      <c r="B129" s="17"/>
-      <c r="C129" s="17"/>
+      <c r="A129" s="25"/>
+      <c r="B129" s="25"/>
+      <c r="C129" s="25"/>
       <c r="D129" s="4" t="s">
         <v>110</v>
       </c>
@@ -3702,9 +3771,9 @@
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A130" s="17"/>
-      <c r="B130" s="17"/>
-      <c r="C130" s="17"/>
+      <c r="A130" s="25"/>
+      <c r="B130" s="25"/>
+      <c r="C130" s="25"/>
       <c r="D130" s="4" t="s">
         <v>203</v>
       </c>
@@ -3716,9 +3785,9 @@
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A131" s="17"/>
-      <c r="B131" s="17"/>
-      <c r="C131" s="17"/>
+      <c r="A131" s="25"/>
+      <c r="B131" s="25"/>
+      <c r="C131" s="25"/>
       <c r="D131" s="4" t="s">
         <v>111</v>
       </c>
@@ -3730,9 +3799,9 @@
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A132" s="17"/>
-      <c r="B132" s="17"/>
-      <c r="C132" s="17"/>
+      <c r="A132" s="25"/>
+      <c r="B132" s="25"/>
+      <c r="C132" s="25"/>
       <c r="D132" s="4" t="s">
         <v>112</v>
       </c>
@@ -3744,9 +3813,9 @@
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A133" s="17"/>
-      <c r="B133" s="17"/>
-      <c r="C133" s="17"/>
+      <c r="A133" s="25"/>
+      <c r="B133" s="25"/>
+      <c r="C133" s="25"/>
       <c r="D133" s="4" t="s">
         <v>113</v>
       </c>
@@ -3758,9 +3827,9 @@
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A134" s="18"/>
-      <c r="B134" s="18"/>
-      <c r="C134" s="18"/>
+      <c r="A134" s="26"/>
+      <c r="B134" s="26"/>
+      <c r="C134" s="26"/>
       <c r="D134" s="4" t="s">
         <v>114</v>
       </c>
@@ -3816,52 +3885,568 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="G5" sqref="G1:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="94.5703125" customWidth="1"/>
     <col min="2" max="2" width="42.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="B1" t="s">
         <v>206</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="B3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="B4" t="s">
         <v>204</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
-        <v>206</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C4" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="B11" t="s">
+        <v>210</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="B12" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
-        <v>206</v>
-      </c>
-      <c r="B3" t="s">
-        <v>207</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>46</v>
+      <c r="C12" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="B13" t="s">
+        <v>210</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="B14" t="s">
+        <v>212</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="B15" t="s">
+        <v>212</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="B25" t="s">
+        <v>212</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="B32" t="s">
+        <v>212</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D32" s="18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D34" s="18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D35" s="18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D38" s="18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="B39" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D39" s="18" t="s">
+        <v>219</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Criterios de aceptacion modelo de autorizaciones
</commit_message>
<xml_diff>
--- a/src/test/resources/data_driven/EstructuraServicio.xlsx
+++ b/src/test/resources/data_driven/EstructuraServicio.xlsx
@@ -380,7 +380,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="247">
   <si>
     <t>Buscar Auxiliares de expedición asociados al parámetro + Su ubicación física de acuerdo al código de oficina</t>
   </si>
@@ -1003,9 +1003,6 @@
     <t>Maria Angelica</t>
   </si>
   <si>
-    <t>Luis Saldarriaga</t>
-  </si>
-  <si>
     <t>CAROLINA MARTINEZ MOLINA</t>
   </si>
   <si>
@@ -1064,13 +1061,79 @@
   </si>
   <si>
     <t>eliajiar</t>
+  </si>
+  <si>
+    <t>El vehículo es importado por terceros, debe ser autorizado</t>
+  </si>
+  <si>
+    <t>Por política de la compañía no esta permitido asegurar vehículos que circulen en esta zona.</t>
+  </si>
+  <si>
+    <t>caromamo</t>
+  </si>
+  <si>
+    <t>anamcagl</t>
+  </si>
+  <si>
+    <t>luissadi</t>
+  </si>
+  <si>
+    <t>natamogn</t>
+  </si>
+  <si>
+    <t>mayrpegr</t>
+  </si>
+  <si>
+    <t>juancara</t>
+  </si>
+  <si>
+    <t>anajvehe</t>
+  </si>
+  <si>
+    <t>crisrora</t>
+  </si>
+  <si>
+    <t>jaiszame</t>
+  </si>
+  <si>
+    <t>paolrosa</t>
+  </si>
+  <si>
+    <t>Valor para campo transporta combustible no permitido. Por favor verifique.</t>
+  </si>
+  <si>
+    <t>ELIANA MARIA JIMENEZ ARISTIZABAL</t>
+  </si>
+  <si>
+    <t>El modelo es superior al máximo permitido por este canal. Por favor verifique</t>
+  </si>
+  <si>
+    <t>El valor del vehículo es inferior al tope mínimo. Por favor verifique.</t>
+  </si>
+  <si>
+    <t>Placa extranjera debe ser autorizada.</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>JESUS ANTONIO GOMEZ CAÑIZARES CQLII, El tomador es un riesgo no estándar y no es posible gestionar la solicitud por este canal. Diríjase a análisis de riesgos para solicitar aprobación.</t>
+  </si>
+  <si>
+    <t>JESUS ANTONIO GOMEZ CAÑIZARES CQLII, El tomador es un riesgo PEPS y no es posible gestionar la solicitud por este canal. Diríjase a análisis de riesgos para solicitar aprobación.</t>
+  </si>
+  <si>
+    <t>BIBIANA BARBOSA MORENO</t>
+  </si>
+  <si>
+    <t>bibibamo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1120,6 +1183,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF232323"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1216,7 +1285,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1258,19 +1327,28 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1282,13 +1360,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1613,28 +1691,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="19"/>
+      <c r="F1" s="24"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
       <c r="E2" s="2" t="s">
         <v>27</v>
       </c>
@@ -1877,10 +1955,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="27">
+      <c r="B2" s="26">
         <v>4029</v>
       </c>
       <c r="C2" s="6">
@@ -1897,8 +1975,8 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
-      <c r="B3" s="27"/>
+      <c r="A3" s="27"/>
+      <c r="B3" s="26"/>
       <c r="C3" s="6">
         <v>70129463</v>
       </c>
@@ -1913,8 +1991,8 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="27"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="26"/>
       <c r="C4" s="6">
         <v>43596238</v>
       </c>
@@ -1929,8 +2007,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
-      <c r="B5" s="27">
+      <c r="A5" s="27"/>
+      <c r="B5" s="26">
         <v>2527</v>
       </c>
       <c r="C5" s="8">
@@ -1945,8 +2023,8 @@
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="27"/>
+      <c r="A6" s="27"/>
+      <c r="B6" s="26"/>
       <c r="C6" s="8">
         <v>71526214</v>
       </c>
@@ -1959,8 +2037,8 @@
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
-      <c r="B7" s="27"/>
+      <c r="A7" s="27"/>
+      <c r="B7" s="26"/>
       <c r="C7" s="8">
         <v>43287144</v>
       </c>
@@ -1973,19 +2051,19 @@
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="27">
+      <c r="B8" s="26">
         <v>4029</v>
       </c>
-      <c r="C8" s="24">
+      <c r="C8" s="29">
         <v>43628391</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="29" t="s">
+      <c r="E8" s="28" t="s">
         <v>52</v>
       </c>
       <c r="F8" s="8" t="s">
@@ -1993,99 +2071,99 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="25"/>
+      <c r="A9" s="26"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="30"/>
       <c r="D9" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="E9" s="29"/>
+      <c r="E9" s="28"/>
       <c r="F9" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="25"/>
+      <c r="A10" s="26"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="30"/>
       <c r="D10" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="29"/>
+      <c r="E10" s="28"/>
       <c r="F10" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="27"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="25"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="30"/>
       <c r="D11" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="E11" s="29"/>
+      <c r="E11" s="28"/>
       <c r="F11" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="25"/>
+      <c r="A12" s="26"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="30"/>
       <c r="D12" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="E12" s="29"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="25"/>
+      <c r="A13" s="26"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="30"/>
       <c r="D13" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="E13" s="29"/>
+      <c r="E13" s="28"/>
       <c r="F13" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="27"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="25"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="30"/>
       <c r="D14" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="E14" s="29"/>
+      <c r="E14" s="28"/>
       <c r="F14" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="27"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="26"/>
+      <c r="A15" s="26"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="31"/>
       <c r="D15" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="E15" s="29"/>
+      <c r="E15" s="28"/>
       <c r="F15" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="27"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="24">
+      <c r="A16" s="26"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="29">
         <v>43618716</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="E16" s="29" t="s">
+      <c r="E16" s="28" t="s">
         <v>53</v>
       </c>
       <c r="F16" s="8" t="s">
@@ -2093,99 +2171,99 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="27"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="25"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="30"/>
       <c r="D17" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="E17" s="29"/>
+      <c r="E17" s="28"/>
       <c r="F17" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="27"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="25"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="30"/>
       <c r="D18" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="E18" s="29"/>
+      <c r="E18" s="28"/>
       <c r="F18" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="27"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="25"/>
+      <c r="A19" s="26"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="30"/>
       <c r="D19" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="29"/>
+      <c r="E19" s="28"/>
       <c r="F19" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
-      <c r="B20" s="27"/>
-      <c r="C20" s="25"/>
+      <c r="A20" s="26"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="30"/>
       <c r="D20" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="E20" s="29"/>
+      <c r="E20" s="28"/>
       <c r="F20" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="27"/>
-      <c r="B21" s="27"/>
-      <c r="C21" s="25"/>
+      <c r="A21" s="26"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="30"/>
       <c r="D21" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="E21" s="29"/>
+      <c r="E21" s="28"/>
       <c r="F21" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="27"/>
-      <c r="B22" s="27"/>
-      <c r="C22" s="25"/>
+      <c r="A22" s="26"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="30"/>
       <c r="D22" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="E22" s="29"/>
+      <c r="E22" s="28"/>
       <c r="F22" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="27"/>
-      <c r="B23" s="27"/>
-      <c r="C23" s="26"/>
+      <c r="A23" s="26"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="31"/>
       <c r="D23" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="E23" s="29"/>
+      <c r="E23" s="28"/>
       <c r="F23" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="24">
+      <c r="A24" s="26"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="29">
         <v>71698481</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="E24" s="29" t="s">
+      <c r="E24" s="28" t="s">
         <v>54</v>
       </c>
       <c r="F24" s="8" t="s">
@@ -2193,99 +2271,99 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="27"/>
-      <c r="B25" s="27"/>
-      <c r="C25" s="25"/>
+      <c r="A25" s="26"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="30"/>
       <c r="D25" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="E25" s="29"/>
+      <c r="E25" s="28"/>
       <c r="F25" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="27"/>
-      <c r="B26" s="27"/>
-      <c r="C26" s="25"/>
+      <c r="A26" s="26"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="30"/>
       <c r="D26" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="E26" s="29"/>
+      <c r="E26" s="28"/>
       <c r="F26" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="27"/>
-      <c r="B27" s="27"/>
-      <c r="C27" s="25"/>
+      <c r="A27" s="26"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="30"/>
       <c r="D27" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="E27" s="29"/>
+      <c r="E27" s="28"/>
       <c r="F27" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="27"/>
-      <c r="B28" s="27"/>
-      <c r="C28" s="25"/>
+      <c r="A28" s="26"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="30"/>
       <c r="D28" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="E28" s="29"/>
+      <c r="E28" s="28"/>
       <c r="F28" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="27"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="25"/>
+      <c r="A29" s="26"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="30"/>
       <c r="D29" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="E29" s="29"/>
+      <c r="E29" s="28"/>
       <c r="F29" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="27"/>
-      <c r="B30" s="27"/>
-      <c r="C30" s="25"/>
+      <c r="A30" s="26"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="30"/>
       <c r="D30" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="E30" s="29"/>
+      <c r="E30" s="28"/>
       <c r="F30" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="27"/>
-      <c r="B31" s="27"/>
-      <c r="C31" s="26"/>
+      <c r="A31" s="26"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="31"/>
       <c r="D31" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="E31" s="29"/>
+      <c r="E31" s="28"/>
       <c r="F31" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="27"/>
-      <c r="B32" s="27"/>
-      <c r="C32" s="24">
+      <c r="A32" s="26"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="29">
         <v>43520997</v>
       </c>
       <c r="D32" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="E32" s="29" t="s">
+      <c r="E32" s="28" t="s">
         <v>55</v>
       </c>
       <c r="F32" s="8" t="s">
@@ -2293,99 +2371,99 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="27"/>
-      <c r="B33" s="27"/>
-      <c r="C33" s="25"/>
+      <c r="A33" s="26"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="30"/>
       <c r="D33" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="E33" s="29"/>
+      <c r="E33" s="28"/>
       <c r="F33" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="27"/>
-      <c r="B34" s="27"/>
-      <c r="C34" s="25"/>
+      <c r="A34" s="26"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="30"/>
       <c r="D34" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="E34" s="29"/>
+      <c r="E34" s="28"/>
       <c r="F34" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="27"/>
-      <c r="B35" s="27"/>
-      <c r="C35" s="25"/>
+      <c r="A35" s="26"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="30"/>
       <c r="D35" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="E35" s="29"/>
+      <c r="E35" s="28"/>
       <c r="F35" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="27"/>
-      <c r="B36" s="27"/>
-      <c r="C36" s="25"/>
+      <c r="A36" s="26"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="30"/>
       <c r="D36" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="E36" s="29"/>
+      <c r="E36" s="28"/>
       <c r="F36" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="27"/>
-      <c r="B37" s="27"/>
-      <c r="C37" s="25"/>
+      <c r="A37" s="26"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="30"/>
       <c r="D37" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E37" s="29"/>
+      <c r="E37" s="28"/>
       <c r="F37" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="27"/>
-      <c r="B38" s="27"/>
-      <c r="C38" s="25"/>
+      <c r="A38" s="26"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="30"/>
       <c r="D38" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="E38" s="29"/>
+      <c r="E38" s="28"/>
       <c r="F38" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="27"/>
-      <c r="B39" s="27"/>
-      <c r="C39" s="26"/>
+      <c r="A39" s="26"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="31"/>
       <c r="D39" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="E39" s="29"/>
+      <c r="E39" s="28"/>
       <c r="F39" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="27"/>
-      <c r="B40" s="27"/>
-      <c r="C40" s="24">
+      <c r="A40" s="26"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="29">
         <v>43527460</v>
       </c>
       <c r="D40" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="E40" s="29" t="s">
+      <c r="E40" s="28" t="s">
         <v>56</v>
       </c>
       <c r="F40" s="8" t="s">
@@ -2393,101 +2471,101 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="27"/>
-      <c r="B41" s="27"/>
-      <c r="C41" s="25"/>
+      <c r="A41" s="26"/>
+      <c r="B41" s="26"/>
+      <c r="C41" s="30"/>
       <c r="D41" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="E41" s="29"/>
+      <c r="E41" s="28"/>
       <c r="F41" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="27"/>
-      <c r="B42" s="27"/>
-      <c r="C42" s="25"/>
+      <c r="A42" s="26"/>
+      <c r="B42" s="26"/>
+      <c r="C42" s="30"/>
       <c r="D42" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="E42" s="29"/>
+      <c r="E42" s="28"/>
       <c r="F42" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="27"/>
-      <c r="B43" s="27"/>
-      <c r="C43" s="25"/>
+      <c r="A43" s="26"/>
+      <c r="B43" s="26"/>
+      <c r="C43" s="30"/>
       <c r="D43" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="E43" s="29"/>
+      <c r="E43" s="28"/>
       <c r="F43" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="27"/>
-      <c r="B44" s="27"/>
-      <c r="C44" s="25"/>
+      <c r="A44" s="26"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="30"/>
       <c r="D44" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="E44" s="29"/>
+      <c r="E44" s="28"/>
       <c r="F44" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="27"/>
-      <c r="B45" s="27"/>
-      <c r="C45" s="25"/>
+      <c r="A45" s="26"/>
+      <c r="B45" s="26"/>
+      <c r="C45" s="30"/>
       <c r="D45" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="E45" s="29"/>
+      <c r="E45" s="28"/>
       <c r="F45" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="27"/>
-      <c r="B46" s="27"/>
-      <c r="C46" s="25"/>
+      <c r="A46" s="26"/>
+      <c r="B46" s="26"/>
+      <c r="C46" s="30"/>
       <c r="D46" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="E46" s="29"/>
+      <c r="E46" s="28"/>
       <c r="F46" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="27"/>
-      <c r="B47" s="27"/>
-      <c r="C47" s="26"/>
+      <c r="A47" s="26"/>
+      <c r="B47" s="26"/>
+      <c r="C47" s="31"/>
       <c r="D47" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="E47" s="29"/>
+      <c r="E47" s="28"/>
       <c r="F47" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="27"/>
-      <c r="B48" s="27">
+      <c r="A48" s="26"/>
+      <c r="B48" s="26">
         <v>2527</v>
       </c>
-      <c r="C48" s="28">
+      <c r="C48" s="27">
         <v>32143454</v>
       </c>
       <c r="D48" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="E48" s="28" t="s">
+      <c r="E48" s="27" t="s">
         <v>97</v>
       </c>
       <c r="F48" s="8" t="s">
@@ -2495,99 +2573,99 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="27"/>
-      <c r="B49" s="27"/>
-      <c r="C49" s="28"/>
+      <c r="A49" s="26"/>
+      <c r="B49" s="26"/>
+      <c r="C49" s="27"/>
       <c r="D49" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="E49" s="28"/>
+      <c r="E49" s="27"/>
       <c r="F49" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="27"/>
-      <c r="B50" s="27"/>
-      <c r="C50" s="28"/>
+      <c r="A50" s="26"/>
+      <c r="B50" s="26"/>
+      <c r="C50" s="27"/>
       <c r="D50" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="E50" s="28"/>
+      <c r="E50" s="27"/>
       <c r="F50" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="27"/>
-      <c r="B51" s="27"/>
-      <c r="C51" s="28"/>
+      <c r="A51" s="26"/>
+      <c r="B51" s="26"/>
+      <c r="C51" s="27"/>
       <c r="D51" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="E51" s="28"/>
+      <c r="E51" s="27"/>
       <c r="F51" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="27"/>
-      <c r="B52" s="27"/>
-      <c r="C52" s="28"/>
+      <c r="A52" s="26"/>
+      <c r="B52" s="26"/>
+      <c r="C52" s="27"/>
       <c r="D52" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="E52" s="28"/>
+      <c r="E52" s="27"/>
       <c r="F52" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="27"/>
-      <c r="B53" s="27"/>
-      <c r="C53" s="28"/>
+      <c r="A53" s="26"/>
+      <c r="B53" s="26"/>
+      <c r="C53" s="27"/>
       <c r="D53" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="E53" s="28"/>
+      <c r="E53" s="27"/>
       <c r="F53" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="27"/>
-      <c r="B54" s="27"/>
-      <c r="C54" s="28"/>
+      <c r="A54" s="26"/>
+      <c r="B54" s="26"/>
+      <c r="C54" s="27"/>
       <c r="D54" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="E54" s="28"/>
+      <c r="E54" s="27"/>
       <c r="F54" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="27"/>
-      <c r="B55" s="27"/>
-      <c r="C55" s="28"/>
+      <c r="A55" s="26"/>
+      <c r="B55" s="26"/>
+      <c r="C55" s="27"/>
       <c r="D55" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="E55" s="28"/>
+      <c r="E55" s="27"/>
       <c r="F55" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="27"/>
-      <c r="B56" s="27"/>
-      <c r="C56" s="28">
+      <c r="A56" s="26"/>
+      <c r="B56" s="26"/>
+      <c r="C56" s="27">
         <v>42790786</v>
       </c>
       <c r="D56" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="E56" s="28" t="s">
+      <c r="E56" s="27" t="s">
         <v>98</v>
       </c>
       <c r="F56" s="8" t="s">
@@ -2595,91 +2673,91 @@
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="27"/>
-      <c r="B57" s="27"/>
-      <c r="C57" s="28"/>
+      <c r="A57" s="26"/>
+      <c r="B57" s="26"/>
+      <c r="C57" s="27"/>
       <c r="D57" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="E57" s="28"/>
+      <c r="E57" s="27"/>
       <c r="F57" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="27"/>
-      <c r="B58" s="27"/>
-      <c r="C58" s="28"/>
+      <c r="A58" s="26"/>
+      <c r="B58" s="26"/>
+      <c r="C58" s="27"/>
       <c r="D58" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="E58" s="28"/>
+      <c r="E58" s="27"/>
       <c r="F58" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="27"/>
-      <c r="B59" s="27"/>
-      <c r="C59" s="28"/>
+      <c r="A59" s="26"/>
+      <c r="B59" s="26"/>
+      <c r="C59" s="27"/>
       <c r="D59" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="E59" s="28"/>
+      <c r="E59" s="27"/>
       <c r="F59" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="27"/>
-      <c r="B60" s="27"/>
-      <c r="C60" s="28"/>
+      <c r="A60" s="26"/>
+      <c r="B60" s="26"/>
+      <c r="C60" s="27"/>
       <c r="D60" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="E60" s="28"/>
+      <c r="E60" s="27"/>
       <c r="F60" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="27"/>
-      <c r="B61" s="27"/>
-      <c r="C61" s="28"/>
+      <c r="A61" s="26"/>
+      <c r="B61" s="26"/>
+      <c r="C61" s="27"/>
       <c r="D61" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="E61" s="28"/>
+      <c r="E61" s="27"/>
       <c r="F61" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="27"/>
-      <c r="B62" s="27"/>
-      <c r="C62" s="28"/>
+      <c r="A62" s="26"/>
+      <c r="B62" s="26"/>
+      <c r="C62" s="27"/>
       <c r="D62" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="E62" s="28"/>
+      <c r="E62" s="27"/>
       <c r="F62" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="27"/>
-      <c r="B63" s="27"/>
-      <c r="C63" s="28"/>
+      <c r="A63" s="26"/>
+      <c r="B63" s="26"/>
+      <c r="C63" s="27"/>
       <c r="D63" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="E63" s="28"/>
+      <c r="E63" s="27"/>
       <c r="F63" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="27" t="s">
+      <c r="A64" s="26" t="s">
         <v>34</v>
       </c>
       <c r="B64" s="4">
@@ -2699,7 +2777,7 @@
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="27"/>
+      <c r="A65" s="26"/>
       <c r="B65" s="4">
         <v>2527</v>
       </c>
@@ -2717,10 +2795,10 @@
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="27" t="s">
+      <c r="A66" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="B66" s="27" t="s">
+      <c r="B66" s="26" t="s">
         <v>51</v>
       </c>
       <c r="C66" s="8" t="s">
@@ -2737,8 +2815,8 @@
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="27"/>
-      <c r="B67" s="27"/>
+      <c r="A67" s="26"/>
+      <c r="B67" s="26"/>
       <c r="C67" s="8" t="s">
         <v>117</v>
       </c>
@@ -2753,8 +2831,8 @@
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="27"/>
-      <c r="B68" s="27"/>
+      <c r="A68" s="26"/>
+      <c r="B68" s="26"/>
       <c r="C68" s="8" t="s">
         <v>118</v>
       </c>
@@ -2769,8 +2847,8 @@
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="27"/>
-      <c r="B69" s="27"/>
+      <c r="A69" s="26"/>
+      <c r="B69" s="26"/>
       <c r="C69" s="8" t="s">
         <v>119</v>
       </c>
@@ -2785,8 +2863,8 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="27"/>
-      <c r="B70" s="27"/>
+      <c r="A70" s="26"/>
+      <c r="B70" s="26"/>
       <c r="C70" s="8" t="s">
         <v>120</v>
       </c>
@@ -2801,8 +2879,8 @@
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="27"/>
-      <c r="B71" s="27"/>
+      <c r="A71" s="26"/>
+      <c r="B71" s="26"/>
       <c r="C71" s="8" t="s">
         <v>121</v>
       </c>
@@ -2817,8 +2895,8 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="27"/>
-      <c r="B72" s="27"/>
+      <c r="A72" s="26"/>
+      <c r="B72" s="26"/>
       <c r="C72" s="8" t="s">
         <v>122</v>
       </c>
@@ -2833,8 +2911,8 @@
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="27"/>
-      <c r="B73" s="27"/>
+      <c r="A73" s="26"/>
+      <c r="B73" s="26"/>
       <c r="C73" s="8" t="s">
         <v>123</v>
       </c>
@@ -2849,8 +2927,8 @@
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="27"/>
-      <c r="B74" s="27"/>
+      <c r="A74" s="26"/>
+      <c r="B74" s="26"/>
       <c r="C74" s="8" t="s">
         <v>124</v>
       </c>
@@ -2865,8 +2943,8 @@
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="27"/>
-      <c r="B75" s="27"/>
+      <c r="A75" s="26"/>
+      <c r="B75" s="26"/>
       <c r="C75" s="8" t="s">
         <v>125</v>
       </c>
@@ -2881,8 +2959,8 @@
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="27"/>
-      <c r="B76" s="27"/>
+      <c r="A76" s="26"/>
+      <c r="B76" s="26"/>
       <c r="C76" s="8" t="s">
         <v>126</v>
       </c>
@@ -2897,8 +2975,8 @@
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="27"/>
-      <c r="B77" s="27"/>
+      <c r="A77" s="26"/>
+      <c r="B77" s="26"/>
       <c r="C77" s="8" t="s">
         <v>127</v>
       </c>
@@ -2913,8 +2991,8 @@
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="27"/>
-      <c r="B78" s="27"/>
+      <c r="A78" s="26"/>
+      <c r="B78" s="26"/>
       <c r="C78" s="8" t="s">
         <v>128</v>
       </c>
@@ -2929,10 +3007,10 @@
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="27" t="s">
+      <c r="A79" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="B79" s="27">
+      <c r="B79" s="26">
         <v>4029</v>
       </c>
       <c r="C79" s="8" t="s">
@@ -2949,8 +3027,8 @@
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="27"/>
-      <c r="B80" s="27"/>
+      <c r="A80" s="26"/>
+      <c r="B80" s="26"/>
       <c r="C80" s="8" t="s">
         <v>146</v>
       </c>
@@ -2965,8 +3043,8 @@
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="27"/>
-      <c r="B81" s="27"/>
+      <c r="A81" s="26"/>
+      <c r="B81" s="26"/>
       <c r="C81" s="8" t="s">
         <v>147</v>
       </c>
@@ -2981,8 +3059,8 @@
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="27"/>
-      <c r="B82" s="27"/>
+      <c r="A82" s="26"/>
+      <c r="B82" s="26"/>
       <c r="C82" s="8" t="s">
         <v>148</v>
       </c>
@@ -2997,8 +3075,8 @@
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="27"/>
-      <c r="B83" s="27"/>
+      <c r="A83" s="26"/>
+      <c r="B83" s="26"/>
       <c r="C83" s="8" t="s">
         <v>149</v>
       </c>
@@ -3013,8 +3091,8 @@
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="27"/>
-      <c r="B84" s="27"/>
+      <c r="A84" s="26"/>
+      <c r="B84" s="26"/>
       <c r="C84" s="8" t="s">
         <v>150</v>
       </c>
@@ -3029,8 +3107,8 @@
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="27"/>
-      <c r="B85" s="27"/>
+      <c r="A85" s="26"/>
+      <c r="B85" s="26"/>
       <c r="C85" s="8" t="s">
         <v>151</v>
       </c>
@@ -3045,7 +3123,7 @@
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="27" t="s">
+      <c r="A86" s="26" t="s">
         <v>37</v>
       </c>
       <c r="B86" s="4">
@@ -3065,7 +3143,7 @@
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="27"/>
+      <c r="A87" s="26"/>
       <c r="B87" s="4">
         <v>3108</v>
       </c>
@@ -3083,7 +3161,7 @@
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="27" t="s">
+      <c r="A88" s="26" t="s">
         <v>39</v>
       </c>
       <c r="B88" s="4">
@@ -3103,7 +3181,7 @@
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="27"/>
+      <c r="A89" s="26"/>
       <c r="B89" s="4">
         <v>3152</v>
       </c>
@@ -3121,7 +3199,7 @@
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="27"/>
+      <c r="A90" s="26"/>
       <c r="B90" s="4">
         <v>3152</v>
       </c>
@@ -3139,7 +3217,7 @@
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="27" t="s">
+      <c r="A91" s="26" t="s">
         <v>38</v>
       </c>
       <c r="B91" s="4">
@@ -3159,7 +3237,7 @@
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="27"/>
+      <c r="A92" s="26"/>
       <c r="B92" s="4">
         <v>3152</v>
       </c>
@@ -3177,7 +3255,7 @@
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="27"/>
+      <c r="A93" s="26"/>
       <c r="B93" s="4">
         <v>3152</v>
       </c>
@@ -3195,7 +3273,7 @@
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="27"/>
+      <c r="A94" s="26"/>
       <c r="B94" s="4">
         <v>3152</v>
       </c>
@@ -3213,7 +3291,7 @@
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="27"/>
+      <c r="A95" s="26"/>
       <c r="B95" s="4">
         <v>3152</v>
       </c>
@@ -3231,7 +3309,7 @@
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="27"/>
+      <c r="A96" s="26"/>
       <c r="B96" s="4">
         <v>3152</v>
       </c>
@@ -3249,7 +3327,7 @@
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="27"/>
+      <c r="A97" s="26"/>
       <c r="B97" s="4">
         <v>3152</v>
       </c>
@@ -3267,7 +3345,7 @@
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="27"/>
+      <c r="A98" s="26"/>
       <c r="B98" s="4">
         <v>3152</v>
       </c>
@@ -3285,7 +3363,7 @@
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="27"/>
+      <c r="A99" s="26"/>
       <c r="B99" s="4">
         <v>3152</v>
       </c>
@@ -3303,7 +3381,7 @@
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="27"/>
+      <c r="A100" s="26"/>
       <c r="B100" s="4">
         <v>3152</v>
       </c>
@@ -3321,7 +3399,7 @@
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="27"/>
+      <c r="A101" s="26"/>
       <c r="B101" s="4">
         <v>3152</v>
       </c>
@@ -3339,7 +3417,7 @@
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" s="27"/>
+      <c r="A102" s="26"/>
       <c r="B102" s="4">
         <v>3152</v>
       </c>
@@ -3357,7 +3435,7 @@
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="27"/>
+      <c r="A103" s="26"/>
       <c r="B103" s="4">
         <v>3108</v>
       </c>
@@ -3375,7 +3453,7 @@
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" s="27"/>
+      <c r="A104" s="26"/>
       <c r="B104" s="4">
         <v>3108</v>
       </c>
@@ -3393,7 +3471,7 @@
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="27"/>
+      <c r="A105" s="26"/>
       <c r="B105" s="4">
         <v>3108</v>
       </c>
@@ -3411,7 +3489,7 @@
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" s="27"/>
+      <c r="A106" s="26"/>
       <c r="B106" s="4">
         <v>3108</v>
       </c>
@@ -3429,7 +3507,7 @@
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107" s="27"/>
+      <c r="A107" s="26"/>
       <c r="B107" s="4">
         <v>3108</v>
       </c>
@@ -3447,7 +3525,7 @@
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A108" s="27"/>
+      <c r="A108" s="26"/>
       <c r="B108" s="4">
         <v>3108</v>
       </c>
@@ -3465,13 +3543,13 @@
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109" s="24" t="s">
+      <c r="A109" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="B109" s="24">
+      <c r="B109" s="29">
         <v>4029</v>
       </c>
-      <c r="C109" s="21">
+      <c r="C109" s="32">
         <v>1128271593</v>
       </c>
       <c r="D109" s="4" t="s">
@@ -3485,9 +3563,9 @@
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A110" s="25"/>
-      <c r="B110" s="25"/>
-      <c r="C110" s="22"/>
+      <c r="A110" s="30"/>
+      <c r="B110" s="30"/>
+      <c r="C110" s="33"/>
       <c r="D110" s="4" t="s">
         <v>189</v>
       </c>
@@ -3499,9 +3577,9 @@
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A111" s="25"/>
-      <c r="B111" s="25"/>
-      <c r="C111" s="22"/>
+      <c r="A111" s="30"/>
+      <c r="B111" s="30"/>
+      <c r="C111" s="33"/>
       <c r="D111" s="4" t="s">
         <v>190</v>
       </c>
@@ -3513,9 +3591,9 @@
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A112" s="25"/>
-      <c r="B112" s="25"/>
-      <c r="C112" s="22"/>
+      <c r="A112" s="30"/>
+      <c r="B112" s="30"/>
+      <c r="C112" s="33"/>
       <c r="D112" s="4" t="s">
         <v>191</v>
       </c>
@@ -3527,9 +3605,9 @@
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A113" s="25"/>
-      <c r="B113" s="25"/>
-      <c r="C113" s="22"/>
+      <c r="A113" s="30"/>
+      <c r="B113" s="30"/>
+      <c r="C113" s="33"/>
       <c r="D113" s="4" t="s">
         <v>192</v>
       </c>
@@ -3541,9 +3619,9 @@
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A114" s="25"/>
-      <c r="B114" s="25"/>
-      <c r="C114" s="22"/>
+      <c r="A114" s="30"/>
+      <c r="B114" s="30"/>
+      <c r="C114" s="33"/>
       <c r="D114" s="4" t="s">
         <v>193</v>
       </c>
@@ -3555,9 +3633,9 @@
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A115" s="25"/>
-      <c r="B115" s="25"/>
-      <c r="C115" s="22"/>
+      <c r="A115" s="30"/>
+      <c r="B115" s="30"/>
+      <c r="C115" s="33"/>
       <c r="D115" s="4" t="s">
         <v>194</v>
       </c>
@@ -3569,9 +3647,9 @@
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A116" s="25"/>
-      <c r="B116" s="25"/>
-      <c r="C116" s="22"/>
+      <c r="A116" s="30"/>
+      <c r="B116" s="30"/>
+      <c r="C116" s="33"/>
       <c r="D116" s="4" t="s">
         <v>195</v>
       </c>
@@ -3583,9 +3661,9 @@
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A117" s="25"/>
-      <c r="B117" s="25"/>
-      <c r="C117" s="22"/>
+      <c r="A117" s="30"/>
+      <c r="B117" s="30"/>
+      <c r="C117" s="33"/>
       <c r="D117" s="4" t="s">
         <v>196</v>
       </c>
@@ -3597,9 +3675,9 @@
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A118" s="25"/>
-      <c r="B118" s="25"/>
-      <c r="C118" s="23"/>
+      <c r="A118" s="30"/>
+      <c r="B118" s="30"/>
+      <c r="C118" s="34"/>
       <c r="D118" s="4" t="s">
         <v>197</v>
       </c>
@@ -3611,9 +3689,9 @@
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A119" s="25"/>
-      <c r="B119" s="25"/>
-      <c r="C119" s="24">
+      <c r="A119" s="30"/>
+      <c r="B119" s="30"/>
+      <c r="C119" s="29">
         <v>43504265</v>
       </c>
       <c r="D119" s="4" t="s">
@@ -3627,9 +3705,9 @@
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A120" s="25"/>
-      <c r="B120" s="25"/>
-      <c r="C120" s="25"/>
+      <c r="A120" s="30"/>
+      <c r="B120" s="30"/>
+      <c r="C120" s="30"/>
       <c r="D120" s="4" t="s">
         <v>199</v>
       </c>
@@ -3641,9 +3719,9 @@
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A121" s="25"/>
-      <c r="B121" s="25"/>
-      <c r="C121" s="25"/>
+      <c r="A121" s="30"/>
+      <c r="B121" s="30"/>
+      <c r="C121" s="30"/>
       <c r="D121" s="4" t="s">
         <v>70</v>
       </c>
@@ -3655,9 +3733,9 @@
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A122" s="25"/>
-      <c r="B122" s="25"/>
-      <c r="C122" s="25"/>
+      <c r="A122" s="30"/>
+      <c r="B122" s="30"/>
+      <c r="C122" s="30"/>
       <c r="D122" s="4" t="s">
         <v>200</v>
       </c>
@@ -3669,9 +3747,9 @@
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A123" s="25"/>
-      <c r="B123" s="25"/>
-      <c r="C123" s="25"/>
+      <c r="A123" s="30"/>
+      <c r="B123" s="30"/>
+      <c r="C123" s="30"/>
       <c r="D123" s="4" t="s">
         <v>71</v>
       </c>
@@ -3683,9 +3761,9 @@
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A124" s="25"/>
-      <c r="B124" s="25"/>
-      <c r="C124" s="25"/>
+      <c r="A124" s="30"/>
+      <c r="B124" s="30"/>
+      <c r="C124" s="30"/>
       <c r="D124" s="4" t="s">
         <v>201</v>
       </c>
@@ -3697,9 +3775,9 @@
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A125" s="25"/>
-      <c r="B125" s="25"/>
-      <c r="C125" s="25"/>
+      <c r="A125" s="30"/>
+      <c r="B125" s="30"/>
+      <c r="C125" s="30"/>
       <c r="D125" s="4" t="s">
         <v>202</v>
       </c>
@@ -3711,9 +3789,9 @@
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A126" s="25"/>
-      <c r="B126" s="26"/>
-      <c r="C126" s="26"/>
+      <c r="A126" s="30"/>
+      <c r="B126" s="31"/>
+      <c r="C126" s="31"/>
       <c r="D126" s="4" t="s">
         <v>72</v>
       </c>
@@ -3725,11 +3803,11 @@
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A127" s="25"/>
-      <c r="B127" s="24">
+      <c r="A127" s="30"/>
+      <c r="B127" s="29">
         <v>2597</v>
       </c>
-      <c r="C127" s="24">
+      <c r="C127" s="29">
         <v>1128278017</v>
       </c>
       <c r="D127" s="4" t="s">
@@ -3743,9 +3821,9 @@
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A128" s="25"/>
-      <c r="B128" s="25"/>
-      <c r="C128" s="25"/>
+      <c r="A128" s="30"/>
+      <c r="B128" s="30"/>
+      <c r="C128" s="30"/>
       <c r="D128" s="4" t="s">
         <v>109</v>
       </c>
@@ -3757,9 +3835,9 @@
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A129" s="25"/>
-      <c r="B129" s="25"/>
-      <c r="C129" s="25"/>
+      <c r="A129" s="30"/>
+      <c r="B129" s="30"/>
+      <c r="C129" s="30"/>
       <c r="D129" s="4" t="s">
         <v>110</v>
       </c>
@@ -3771,9 +3849,9 @@
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A130" s="25"/>
-      <c r="B130" s="25"/>
-      <c r="C130" s="25"/>
+      <c r="A130" s="30"/>
+      <c r="B130" s="30"/>
+      <c r="C130" s="30"/>
       <c r="D130" s="4" t="s">
         <v>203</v>
       </c>
@@ -3785,9 +3863,9 @@
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A131" s="25"/>
-      <c r="B131" s="25"/>
-      <c r="C131" s="25"/>
+      <c r="A131" s="30"/>
+      <c r="B131" s="30"/>
+      <c r="C131" s="30"/>
       <c r="D131" s="4" t="s">
         <v>111</v>
       </c>
@@ -3799,9 +3877,9 @@
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A132" s="25"/>
-      <c r="B132" s="25"/>
-      <c r="C132" s="25"/>
+      <c r="A132" s="30"/>
+      <c r="B132" s="30"/>
+      <c r="C132" s="30"/>
       <c r="D132" s="4" t="s">
         <v>112</v>
       </c>
@@ -3813,9 +3891,9 @@
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A133" s="25"/>
-      <c r="B133" s="25"/>
-      <c r="C133" s="25"/>
+      <c r="A133" s="30"/>
+      <c r="B133" s="30"/>
+      <c r="C133" s="30"/>
       <c r="D133" s="4" t="s">
         <v>113</v>
       </c>
@@ -3827,9 +3905,9 @@
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A134" s="26"/>
-      <c r="B134" s="26"/>
-      <c r="C134" s="26"/>
+      <c r="A134" s="31"/>
+      <c r="B134" s="31"/>
+      <c r="C134" s="31"/>
       <c r="D134" s="4" t="s">
         <v>114</v>
       </c>
@@ -3842,6 +3920,31 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="C109:C118"/>
+    <mergeCell ref="B109:B126"/>
+    <mergeCell ref="C119:C126"/>
+    <mergeCell ref="C127:C134"/>
+    <mergeCell ref="B127:B134"/>
+    <mergeCell ref="A109:A134"/>
+    <mergeCell ref="A79:A85"/>
+    <mergeCell ref="B79:B85"/>
+    <mergeCell ref="A86:A87"/>
+    <mergeCell ref="A88:A90"/>
+    <mergeCell ref="A91:A108"/>
+    <mergeCell ref="A64:A65"/>
+    <mergeCell ref="A66:A78"/>
+    <mergeCell ref="B66:B78"/>
+    <mergeCell ref="A8:A63"/>
+    <mergeCell ref="C56:C63"/>
+    <mergeCell ref="B48:B63"/>
+    <mergeCell ref="C8:C15"/>
+    <mergeCell ref="E56:E63"/>
+    <mergeCell ref="C32:C39"/>
+    <mergeCell ref="E32:E39"/>
+    <mergeCell ref="C40:C47"/>
+    <mergeCell ref="E40:E47"/>
+    <mergeCell ref="C48:C55"/>
+    <mergeCell ref="E48:E55"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="A2:A7"/>
@@ -3851,31 +3954,6 @@
     <mergeCell ref="E16:E23"/>
     <mergeCell ref="C24:C31"/>
     <mergeCell ref="E24:E31"/>
-    <mergeCell ref="E56:E63"/>
-    <mergeCell ref="C32:C39"/>
-    <mergeCell ref="E32:E39"/>
-    <mergeCell ref="C40:C47"/>
-    <mergeCell ref="E40:E47"/>
-    <mergeCell ref="C48:C55"/>
-    <mergeCell ref="E48:E55"/>
-    <mergeCell ref="A64:A65"/>
-    <mergeCell ref="A66:A78"/>
-    <mergeCell ref="B66:B78"/>
-    <mergeCell ref="A8:A63"/>
-    <mergeCell ref="C56:C63"/>
-    <mergeCell ref="B48:B63"/>
-    <mergeCell ref="C8:C15"/>
-    <mergeCell ref="A109:A134"/>
-    <mergeCell ref="A79:A85"/>
-    <mergeCell ref="B79:B85"/>
-    <mergeCell ref="A86:A87"/>
-    <mergeCell ref="A88:A90"/>
-    <mergeCell ref="A91:A108"/>
-    <mergeCell ref="C109:C118"/>
-    <mergeCell ref="B109:B126"/>
-    <mergeCell ref="C119:C126"/>
-    <mergeCell ref="C127:C134"/>
-    <mergeCell ref="B127:B134"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3885,15 +3963,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G1:G5"/>
+    <sheetView tabSelected="1" topLeftCell="B30" workbookViewId="0">
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="94.5703125" customWidth="1"/>
+    <col min="1" max="1" width="162.7109375" customWidth="1"/>
     <col min="2" max="2" width="42.140625" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" style="18"/>
@@ -3901,548 +3979,798 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="B3" t="s">
         <v>207</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>207</v>
-      </c>
-      <c r="B3" t="s">
-        <v>208</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>225</v>
+      <c r="C3" s="20" t="s">
+        <v>230</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B4" t="s">
         <v>204</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>225</v>
+        <v>236</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>225</v>
+        <v>235</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="B11" t="s">
         <v>209</v>
       </c>
-      <c r="B11" t="s">
-        <v>210</v>
-      </c>
       <c r="C11" s="7" t="s">
-        <v>225</v>
+        <v>234</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>205</v>
+        <v>223</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B13" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>225</v>
+        <v>234</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
+        <v>210</v>
+      </c>
+      <c r="B14" t="s">
         <v>211</v>
       </c>
-      <c r="B14" t="s">
-        <v>212</v>
-      </c>
       <c r="C14" s="7" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B15" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>225</v>
+        <v>235</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>225</v>
+        <v>236</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="B22" s="14" t="s">
         <v>213</v>
       </c>
-      <c r="B22" s="14" t="s">
-        <v>214</v>
-      </c>
       <c r="C22" s="7" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B25" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>225</v>
+        <v>234</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>225</v>
+        <v>235</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>225</v>
+        <v>236</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B32" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="B33" s="14" t="s">
         <v>216</v>
       </c>
-      <c r="B33" s="14" t="s">
-        <v>217</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>225</v>
+      <c r="C33" s="21" t="s">
+        <v>235</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>225</v>
+        <v>234</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A38" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="C38" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="D38" s="18" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A39" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="B39" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="C39" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="D39" s="18" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>225</v>
+      </c>
+      <c r="B40" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="C40" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="D40" s="18" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>237</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>238</v>
+      </c>
+      <c r="C41" s="19" t="s">
+        <v>224</v>
+      </c>
+      <c r="D41" s="18" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="15" t="s">
+        <v>226</v>
+      </c>
+      <c r="B42" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="C42" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="D42" s="18" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B43" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C43" s="23" t="s">
+        <v>236</v>
+      </c>
+      <c r="D43" s="18" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B44" s="22" t="s">
+        <v>213</v>
+      </c>
+      <c r="C44" s="23" t="s">
+        <v>231</v>
+      </c>
+      <c r="D44" s="18" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B45" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C45" s="23" t="s">
+        <v>236</v>
+      </c>
+      <c r="D45" s="18" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B46" s="22" t="s">
+        <v>209</v>
+      </c>
+      <c r="C46" s="23" t="s">
+        <v>234</v>
+      </c>
+      <c r="D46" s="18" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B47" s="22" t="s">
+        <v>245</v>
+      </c>
+      <c r="C47" s="23" t="s">
+        <v>246</v>
+      </c>
+      <c r="D47" s="18" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B48" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="C48" s="23" t="s">
+        <v>229</v>
+      </c>
+      <c r="D48" s="18" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B49" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C49" s="23" t="s">
+        <v>233</v>
+      </c>
+      <c r="D49" s="18" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B50" s="22" t="s">
         <v>216</v>
       </c>
-      <c r="B37" s="17" t="s">
+      <c r="C50" s="23" t="s">
+        <v>235</v>
+      </c>
+      <c r="D50" s="18" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B51" s="22" t="s">
+        <v>217</v>
+      </c>
+      <c r="C51" s="23" t="s">
+        <v>232</v>
+      </c>
+      <c r="D51" s="18" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B52" s="22" t="s">
+        <v>220</v>
+      </c>
+      <c r="C52" s="23" t="s">
         <v>224</v>
       </c>
-      <c r="C37" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="D37" s="18" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="15" t="s">
-        <v>216</v>
-      </c>
-      <c r="B38" s="17" t="s">
-        <v>218</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="D38" s="18" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="15" t="s">
-        <v>216</v>
-      </c>
-      <c r="B39" s="17" t="s">
-        <v>214</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="D39" s="18" t="s">
-        <v>219</v>
+      <c r="D52" s="18" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A53" s="20" t="s">
+        <v>240</v>
+      </c>
+      <c r="B53" s="22"/>
+      <c r="C53" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="D53" s="18" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A54" s="20" t="s">
+        <v>240</v>
+      </c>
+      <c r="B54" s="22" t="s">
+        <v>242</v>
+      </c>
+      <c r="C54" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="D54" s="18" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B55" s="22" t="s">
+        <v>238</v>
+      </c>
+      <c r="C55" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="D55" s="18" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>243</v>
+      </c>
+      <c r="B56" s="22" t="s">
+        <v>238</v>
+      </c>
+      <c r="C56" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="D56" s="18" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>244</v>
+      </c>
+      <c r="B57" s="22" t="s">
+        <v>238</v>
+      </c>
+      <c r="C57" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="D57" s="18" t="s">
+        <v>218</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Estabilizacion pruebas cancelacion autorizacion
</commit_message>
<xml_diff>
--- a/src/test/resources/data_driven/EstructuraServicio.xlsx
+++ b/src/test/resources/data_driven/EstructuraServicio.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SURA\BDDCoreSuraPolicy\src\test\resources\data_driven\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="885" windowWidth="19875" windowHeight="6210" activeTab="2"/>
   </bookViews>
@@ -21,7 +26,7 @@
     <author>Jenifer Mora Sanchez</author>
   </authors>
   <commentList>
-    <comment ref="D3" authorId="0">
+    <comment ref="D3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -55,7 +60,7 @@
     <author>Jenifer Mora Sanchez</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0">
+    <comment ref="B2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -79,7 +84,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B86" authorId="0">
+    <comment ref="B86" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -103,7 +108,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B87" authorId="0">
+    <comment ref="B87" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -128,7 +133,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B88" authorId="0">
+    <comment ref="B88" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -153,7 +158,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B89" authorId="0">
+    <comment ref="B89" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -177,7 +182,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B90" authorId="0">
+    <comment ref="B90" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -201,7 +206,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B91" authorId="0">
+    <comment ref="B91" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -225,7 +230,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B103" authorId="0">
+    <comment ref="B103" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -250,7 +255,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B104" authorId="0">
+    <comment ref="B104" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -275,7 +280,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B105" authorId="0">
+    <comment ref="B105" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -300,7 +305,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B106" authorId="0">
+    <comment ref="B106" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -325,7 +330,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B107" authorId="0">
+    <comment ref="B107" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -350,7 +355,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B108" authorId="0">
+    <comment ref="B108" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -380,7 +385,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="291">
   <si>
     <t>Buscar Auxiliares de expedición asociados al parámetro + Su ubicación física de acuerdo al código de oficina</t>
   </si>
@@ -1483,13 +1488,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1501,13 +1506,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1571,7 +1576,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1606,7 +1611,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2096,10 +2101,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="33">
+      <c r="B2" s="27">
         <v>4029</v>
       </c>
       <c r="C2" s="6">
@@ -2116,8 +2121,8 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="34"/>
-      <c r="B3" s="33"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="27"/>
       <c r="C3" s="6">
         <v>70129463</v>
       </c>
@@ -2132,8 +2137,8 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="34"/>
-      <c r="B4" s="33"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="27"/>
       <c r="C4" s="6">
         <v>43596238</v>
       </c>
@@ -2148,8 +2153,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="34"/>
-      <c r="B5" s="33">
+      <c r="A5" s="28"/>
+      <c r="B5" s="27">
         <v>2527</v>
       </c>
       <c r="C5" s="8">
@@ -2164,8 +2169,8 @@
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="34"/>
-      <c r="B6" s="33"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="27"/>
       <c r="C6" s="8">
         <v>71526214</v>
       </c>
@@ -2178,8 +2183,8 @@
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="34"/>
-      <c r="B7" s="33"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="27"/>
       <c r="C7" s="8">
         <v>43287144</v>
       </c>
@@ -2192,10 +2197,10 @@
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="33">
+      <c r="B8" s="27">
         <v>4029</v>
       </c>
       <c r="C8" s="30">
@@ -2204,7 +2209,7 @@
       <c r="D8" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="35" t="s">
+      <c r="E8" s="29" t="s">
         <v>52</v>
       </c>
       <c r="F8" s="8" t="s">
@@ -2212,99 +2217,99 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="33"/>
-      <c r="B9" s="33"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
       <c r="C9" s="31"/>
       <c r="D9" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="E9" s="35"/>
+      <c r="E9" s="29"/>
       <c r="F9" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="33"/>
-      <c r="B10" s="33"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
       <c r="C10" s="31"/>
       <c r="D10" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="35"/>
+      <c r="E10" s="29"/>
       <c r="F10" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="33"/>
-      <c r="B11" s="33"/>
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
       <c r="C11" s="31"/>
       <c r="D11" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="E11" s="35"/>
+      <c r="E11" s="29"/>
       <c r="F11" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="33"/>
-      <c r="B12" s="33"/>
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
       <c r="C12" s="31"/>
       <c r="D12" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="E12" s="35"/>
+      <c r="E12" s="29"/>
       <c r="F12" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="33"/>
-      <c r="B13" s="33"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
       <c r="C13" s="31"/>
       <c r="D13" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="E13" s="35"/>
+      <c r="E13" s="29"/>
       <c r="F13" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="33"/>
-      <c r="B14" s="33"/>
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
       <c r="C14" s="31"/>
       <c r="D14" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="E14" s="35"/>
+      <c r="E14" s="29"/>
       <c r="F14" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="33"/>
-      <c r="B15" s="33"/>
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
       <c r="C15" s="32"/>
       <c r="D15" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="E15" s="35"/>
+      <c r="E15" s="29"/>
       <c r="F15" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="33"/>
-      <c r="B16" s="33"/>
+      <c r="A16" s="27"/>
+      <c r="B16" s="27"/>
       <c r="C16" s="30">
         <v>43618716</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="E16" s="35" t="s">
+      <c r="E16" s="29" t="s">
         <v>53</v>
       </c>
       <c r="F16" s="8" t="s">
@@ -2312,99 +2317,99 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
       <c r="C17" s="31"/>
       <c r="D17" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="E17" s="35"/>
+      <c r="E17" s="29"/>
       <c r="F17" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="27"/>
+      <c r="B18" s="27"/>
       <c r="C18" s="31"/>
       <c r="D18" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="E18" s="35"/>
+      <c r="E18" s="29"/>
       <c r="F18" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="33"/>
-      <c r="B19" s="33"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
       <c r="C19" s="31"/>
       <c r="D19" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="35"/>
+      <c r="E19" s="29"/>
       <c r="F19" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="33"/>
-      <c r="B20" s="33"/>
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
       <c r="C20" s="31"/>
       <c r="D20" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="E20" s="35"/>
+      <c r="E20" s="29"/>
       <c r="F20" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="33"/>
-      <c r="B21" s="33"/>
+      <c r="A21" s="27"/>
+      <c r="B21" s="27"/>
       <c r="C21" s="31"/>
       <c r="D21" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="E21" s="35"/>
+      <c r="E21" s="29"/>
       <c r="F21" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="33"/>
-      <c r="B22" s="33"/>
+      <c r="A22" s="27"/>
+      <c r="B22" s="27"/>
       <c r="C22" s="31"/>
       <c r="D22" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="E22" s="35"/>
+      <c r="E22" s="29"/>
       <c r="F22" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="33"/>
-      <c r="B23" s="33"/>
+      <c r="A23" s="27"/>
+      <c r="B23" s="27"/>
       <c r="C23" s="32"/>
       <c r="D23" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="E23" s="35"/>
+      <c r="E23" s="29"/>
       <c r="F23" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="33"/>
-      <c r="B24" s="33"/>
+      <c r="A24" s="27"/>
+      <c r="B24" s="27"/>
       <c r="C24" s="30">
         <v>71698481</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="E24" s="35" t="s">
+      <c r="E24" s="29" t="s">
         <v>54</v>
       </c>
       <c r="F24" s="8" t="s">
@@ -2412,99 +2417,99 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="33"/>
-      <c r="B25" s="33"/>
+      <c r="A25" s="27"/>
+      <c r="B25" s="27"/>
       <c r="C25" s="31"/>
       <c r="D25" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="E25" s="35"/>
+      <c r="E25" s="29"/>
       <c r="F25" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="33"/>
-      <c r="B26" s="33"/>
+      <c r="A26" s="27"/>
+      <c r="B26" s="27"/>
       <c r="C26" s="31"/>
       <c r="D26" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="E26" s="35"/>
+      <c r="E26" s="29"/>
       <c r="F26" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="33"/>
-      <c r="B27" s="33"/>
+      <c r="A27" s="27"/>
+      <c r="B27" s="27"/>
       <c r="C27" s="31"/>
       <c r="D27" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="E27" s="35"/>
+      <c r="E27" s="29"/>
       <c r="F27" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="33"/>
-      <c r="B28" s="33"/>
+      <c r="A28" s="27"/>
+      <c r="B28" s="27"/>
       <c r="C28" s="31"/>
       <c r="D28" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="E28" s="35"/>
+      <c r="E28" s="29"/>
       <c r="F28" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="33"/>
-      <c r="B29" s="33"/>
+      <c r="A29" s="27"/>
+      <c r="B29" s="27"/>
       <c r="C29" s="31"/>
       <c r="D29" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="E29" s="35"/>
+      <c r="E29" s="29"/>
       <c r="F29" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="33"/>
-      <c r="B30" s="33"/>
+      <c r="A30" s="27"/>
+      <c r="B30" s="27"/>
       <c r="C30" s="31"/>
       <c r="D30" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="E30" s="35"/>
+      <c r="E30" s="29"/>
       <c r="F30" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="33"/>
-      <c r="B31" s="33"/>
+      <c r="A31" s="27"/>
+      <c r="B31" s="27"/>
       <c r="C31" s="32"/>
       <c r="D31" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="E31" s="35"/>
+      <c r="E31" s="29"/>
       <c r="F31" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="33"/>
-      <c r="B32" s="33"/>
+      <c r="A32" s="27"/>
+      <c r="B32" s="27"/>
       <c r="C32" s="30">
         <v>43520997</v>
       </c>
       <c r="D32" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="E32" s="35" t="s">
+      <c r="E32" s="29" t="s">
         <v>55</v>
       </c>
       <c r="F32" s="8" t="s">
@@ -2512,99 +2517,99 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="33"/>
-      <c r="B33" s="33"/>
+      <c r="A33" s="27"/>
+      <c r="B33" s="27"/>
       <c r="C33" s="31"/>
       <c r="D33" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="E33" s="35"/>
+      <c r="E33" s="29"/>
       <c r="F33" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="33"/>
-      <c r="B34" s="33"/>
+      <c r="A34" s="27"/>
+      <c r="B34" s="27"/>
       <c r="C34" s="31"/>
       <c r="D34" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="E34" s="35"/>
+      <c r="E34" s="29"/>
       <c r="F34" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="33"/>
-      <c r="B35" s="33"/>
+      <c r="A35" s="27"/>
+      <c r="B35" s="27"/>
       <c r="C35" s="31"/>
       <c r="D35" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="E35" s="35"/>
+      <c r="E35" s="29"/>
       <c r="F35" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="33"/>
-      <c r="B36" s="33"/>
+      <c r="A36" s="27"/>
+      <c r="B36" s="27"/>
       <c r="C36" s="31"/>
       <c r="D36" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="E36" s="35"/>
+      <c r="E36" s="29"/>
       <c r="F36" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="33"/>
-      <c r="B37" s="33"/>
+      <c r="A37" s="27"/>
+      <c r="B37" s="27"/>
       <c r="C37" s="31"/>
       <c r="D37" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E37" s="35"/>
+      <c r="E37" s="29"/>
       <c r="F37" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="33"/>
-      <c r="B38" s="33"/>
+      <c r="A38" s="27"/>
+      <c r="B38" s="27"/>
       <c r="C38" s="31"/>
       <c r="D38" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="E38" s="35"/>
+      <c r="E38" s="29"/>
       <c r="F38" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="33"/>
-      <c r="B39" s="33"/>
+      <c r="A39" s="27"/>
+      <c r="B39" s="27"/>
       <c r="C39" s="32"/>
       <c r="D39" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="E39" s="35"/>
+      <c r="E39" s="29"/>
       <c r="F39" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="33"/>
-      <c r="B40" s="33"/>
+      <c r="A40" s="27"/>
+      <c r="B40" s="27"/>
       <c r="C40" s="30">
         <v>43527460</v>
       </c>
       <c r="D40" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="E40" s="35" t="s">
+      <c r="E40" s="29" t="s">
         <v>56</v>
       </c>
       <c r="F40" s="8" t="s">
@@ -2612,101 +2617,101 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="33"/>
-      <c r="B41" s="33"/>
+      <c r="A41" s="27"/>
+      <c r="B41" s="27"/>
       <c r="C41" s="31"/>
       <c r="D41" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="E41" s="35"/>
+      <c r="E41" s="29"/>
       <c r="F41" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="33"/>
-      <c r="B42" s="33"/>
+      <c r="A42" s="27"/>
+      <c r="B42" s="27"/>
       <c r="C42" s="31"/>
       <c r="D42" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="E42" s="35"/>
+      <c r="E42" s="29"/>
       <c r="F42" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="33"/>
-      <c r="B43" s="33"/>
+      <c r="A43" s="27"/>
+      <c r="B43" s="27"/>
       <c r="C43" s="31"/>
       <c r="D43" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="E43" s="35"/>
+      <c r="E43" s="29"/>
       <c r="F43" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="33"/>
-      <c r="B44" s="33"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="27"/>
       <c r="C44" s="31"/>
       <c r="D44" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="E44" s="35"/>
+      <c r="E44" s="29"/>
       <c r="F44" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="33"/>
-      <c r="B45" s="33"/>
+      <c r="A45" s="27"/>
+      <c r="B45" s="27"/>
       <c r="C45" s="31"/>
       <c r="D45" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="E45" s="35"/>
+      <c r="E45" s="29"/>
       <c r="F45" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="33"/>
-      <c r="B46" s="33"/>
+      <c r="A46" s="27"/>
+      <c r="B46" s="27"/>
       <c r="C46" s="31"/>
       <c r="D46" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="E46" s="35"/>
+      <c r="E46" s="29"/>
       <c r="F46" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="33"/>
-      <c r="B47" s="33"/>
+      <c r="A47" s="27"/>
+      <c r="B47" s="27"/>
       <c r="C47" s="32"/>
       <c r="D47" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="E47" s="35"/>
+      <c r="E47" s="29"/>
       <c r="F47" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="33"/>
-      <c r="B48" s="33">
+      <c r="A48" s="27"/>
+      <c r="B48" s="27">
         <v>2527</v>
       </c>
-      <c r="C48" s="34">
+      <c r="C48" s="28">
         <v>32143454</v>
       </c>
       <c r="D48" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="E48" s="34" t="s">
+      <c r="E48" s="28" t="s">
         <v>97</v>
       </c>
       <c r="F48" s="8" t="s">
@@ -2714,99 +2719,99 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="33"/>
-      <c r="B49" s="33"/>
-      <c r="C49" s="34"/>
+      <c r="A49" s="27"/>
+      <c r="B49" s="27"/>
+      <c r="C49" s="28"/>
       <c r="D49" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="E49" s="34"/>
+      <c r="E49" s="28"/>
       <c r="F49" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="33"/>
-      <c r="B50" s="33"/>
-      <c r="C50" s="34"/>
+      <c r="A50" s="27"/>
+      <c r="B50" s="27"/>
+      <c r="C50" s="28"/>
       <c r="D50" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="E50" s="34"/>
+      <c r="E50" s="28"/>
       <c r="F50" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="33"/>
-      <c r="B51" s="33"/>
-      <c r="C51" s="34"/>
+      <c r="A51" s="27"/>
+      <c r="B51" s="27"/>
+      <c r="C51" s="28"/>
       <c r="D51" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="E51" s="34"/>
+      <c r="E51" s="28"/>
       <c r="F51" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="33"/>
-      <c r="B52" s="33"/>
-      <c r="C52" s="34"/>
+      <c r="A52" s="27"/>
+      <c r="B52" s="27"/>
+      <c r="C52" s="28"/>
       <c r="D52" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="E52" s="34"/>
+      <c r="E52" s="28"/>
       <c r="F52" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="33"/>
-      <c r="B53" s="33"/>
-      <c r="C53" s="34"/>
+      <c r="A53" s="27"/>
+      <c r="B53" s="27"/>
+      <c r="C53" s="28"/>
       <c r="D53" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="E53" s="34"/>
+      <c r="E53" s="28"/>
       <c r="F53" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="33"/>
-      <c r="B54" s="33"/>
-      <c r="C54" s="34"/>
+      <c r="A54" s="27"/>
+      <c r="B54" s="27"/>
+      <c r="C54" s="28"/>
       <c r="D54" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="E54" s="34"/>
+      <c r="E54" s="28"/>
       <c r="F54" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="33"/>
-      <c r="B55" s="33"/>
-      <c r="C55" s="34"/>
+      <c r="A55" s="27"/>
+      <c r="B55" s="27"/>
+      <c r="C55" s="28"/>
       <c r="D55" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="E55" s="34"/>
+      <c r="E55" s="28"/>
       <c r="F55" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="33"/>
-      <c r="B56" s="33"/>
-      <c r="C56" s="34">
+      <c r="A56" s="27"/>
+      <c r="B56" s="27"/>
+      <c r="C56" s="28">
         <v>42790786</v>
       </c>
       <c r="D56" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="E56" s="34" t="s">
+      <c r="E56" s="28" t="s">
         <v>98</v>
       </c>
       <c r="F56" s="8" t="s">
@@ -2814,91 +2819,91 @@
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="33"/>
-      <c r="B57" s="33"/>
-      <c r="C57" s="34"/>
+      <c r="A57" s="27"/>
+      <c r="B57" s="27"/>
+      <c r="C57" s="28"/>
       <c r="D57" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="E57" s="34"/>
+      <c r="E57" s="28"/>
       <c r="F57" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="33"/>
-      <c r="B58" s="33"/>
-      <c r="C58" s="34"/>
+      <c r="A58" s="27"/>
+      <c r="B58" s="27"/>
+      <c r="C58" s="28"/>
       <c r="D58" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="E58" s="34"/>
+      <c r="E58" s="28"/>
       <c r="F58" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="33"/>
-      <c r="B59" s="33"/>
-      <c r="C59" s="34"/>
+      <c r="A59" s="27"/>
+      <c r="B59" s="27"/>
+      <c r="C59" s="28"/>
       <c r="D59" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="E59" s="34"/>
+      <c r="E59" s="28"/>
       <c r="F59" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="33"/>
-      <c r="B60" s="33"/>
-      <c r="C60" s="34"/>
+      <c r="A60" s="27"/>
+      <c r="B60" s="27"/>
+      <c r="C60" s="28"/>
       <c r="D60" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="E60" s="34"/>
+      <c r="E60" s="28"/>
       <c r="F60" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="33"/>
-      <c r="B61" s="33"/>
-      <c r="C61" s="34"/>
+      <c r="A61" s="27"/>
+      <c r="B61" s="27"/>
+      <c r="C61" s="28"/>
       <c r="D61" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="E61" s="34"/>
+      <c r="E61" s="28"/>
       <c r="F61" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="33"/>
-      <c r="B62" s="33"/>
-      <c r="C62" s="34"/>
+      <c r="A62" s="27"/>
+      <c r="B62" s="27"/>
+      <c r="C62" s="28"/>
       <c r="D62" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="E62" s="34"/>
+      <c r="E62" s="28"/>
       <c r="F62" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="33"/>
-      <c r="B63" s="33"/>
-      <c r="C63" s="34"/>
+      <c r="A63" s="27"/>
+      <c r="B63" s="27"/>
+      <c r="C63" s="28"/>
       <c r="D63" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="E63" s="34"/>
+      <c r="E63" s="28"/>
       <c r="F63" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="33" t="s">
+      <c r="A64" s="27" t="s">
         <v>34</v>
       </c>
       <c r="B64" s="4">
@@ -2918,7 +2923,7 @@
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="33"/>
+      <c r="A65" s="27"/>
       <c r="B65" s="4">
         <v>2527</v>
       </c>
@@ -2936,10 +2941,10 @@
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="33" t="s">
+      <c r="A66" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="B66" s="33" t="s">
+      <c r="B66" s="27" t="s">
         <v>51</v>
       </c>
       <c r="C66" s="8" t="s">
@@ -2956,8 +2961,8 @@
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="33"/>
-      <c r="B67" s="33"/>
+      <c r="A67" s="27"/>
+      <c r="B67" s="27"/>
       <c r="C67" s="8" t="s">
         <v>117</v>
       </c>
@@ -2972,8 +2977,8 @@
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="33"/>
-      <c r="B68" s="33"/>
+      <c r="A68" s="27"/>
+      <c r="B68" s="27"/>
       <c r="C68" s="8" t="s">
         <v>118</v>
       </c>
@@ -2988,8 +2993,8 @@
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="33"/>
-      <c r="B69" s="33"/>
+      <c r="A69" s="27"/>
+      <c r="B69" s="27"/>
       <c r="C69" s="8" t="s">
         <v>119</v>
       </c>
@@ -3004,8 +3009,8 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="33"/>
-      <c r="B70" s="33"/>
+      <c r="A70" s="27"/>
+      <c r="B70" s="27"/>
       <c r="C70" s="8" t="s">
         <v>120</v>
       </c>
@@ -3020,8 +3025,8 @@
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="33"/>
-      <c r="B71" s="33"/>
+      <c r="A71" s="27"/>
+      <c r="B71" s="27"/>
       <c r="C71" s="8" t="s">
         <v>121</v>
       </c>
@@ -3036,8 +3041,8 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="33"/>
-      <c r="B72" s="33"/>
+      <c r="A72" s="27"/>
+      <c r="B72" s="27"/>
       <c r="C72" s="8" t="s">
         <v>122</v>
       </c>
@@ -3052,8 +3057,8 @@
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="33"/>
-      <c r="B73" s="33"/>
+      <c r="A73" s="27"/>
+      <c r="B73" s="27"/>
       <c r="C73" s="8" t="s">
         <v>123</v>
       </c>
@@ -3068,8 +3073,8 @@
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="33"/>
-      <c r="B74" s="33"/>
+      <c r="A74" s="27"/>
+      <c r="B74" s="27"/>
       <c r="C74" s="8" t="s">
         <v>124</v>
       </c>
@@ -3084,8 +3089,8 @@
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="33"/>
-      <c r="B75" s="33"/>
+      <c r="A75" s="27"/>
+      <c r="B75" s="27"/>
       <c r="C75" s="8" t="s">
         <v>125</v>
       </c>
@@ -3100,8 +3105,8 @@
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="33"/>
-      <c r="B76" s="33"/>
+      <c r="A76" s="27"/>
+      <c r="B76" s="27"/>
       <c r="C76" s="8" t="s">
         <v>126</v>
       </c>
@@ -3116,8 +3121,8 @@
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="33"/>
-      <c r="B77" s="33"/>
+      <c r="A77" s="27"/>
+      <c r="B77" s="27"/>
       <c r="C77" s="8" t="s">
         <v>127</v>
       </c>
@@ -3132,8 +3137,8 @@
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="33"/>
-      <c r="B78" s="33"/>
+      <c r="A78" s="27"/>
+      <c r="B78" s="27"/>
       <c r="C78" s="8" t="s">
         <v>128</v>
       </c>
@@ -3148,10 +3153,10 @@
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="33" t="s">
+      <c r="A79" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="B79" s="33">
+      <c r="B79" s="27">
         <v>4029</v>
       </c>
       <c r="C79" s="8" t="s">
@@ -3168,8 +3173,8 @@
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="33"/>
-      <c r="B80" s="33"/>
+      <c r="A80" s="27"/>
+      <c r="B80" s="27"/>
       <c r="C80" s="8" t="s">
         <v>146</v>
       </c>
@@ -3184,8 +3189,8 @@
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="33"/>
-      <c r="B81" s="33"/>
+      <c r="A81" s="27"/>
+      <c r="B81" s="27"/>
       <c r="C81" s="8" t="s">
         <v>147</v>
       </c>
@@ -3200,8 +3205,8 @@
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="33"/>
-      <c r="B82" s="33"/>
+      <c r="A82" s="27"/>
+      <c r="B82" s="27"/>
       <c r="C82" s="8" t="s">
         <v>148</v>
       </c>
@@ -3216,8 +3221,8 @@
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="33"/>
-      <c r="B83" s="33"/>
+      <c r="A83" s="27"/>
+      <c r="B83" s="27"/>
       <c r="C83" s="8" t="s">
         <v>149</v>
       </c>
@@ -3232,8 +3237,8 @@
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="33"/>
-      <c r="B84" s="33"/>
+      <c r="A84" s="27"/>
+      <c r="B84" s="27"/>
       <c r="C84" s="8" t="s">
         <v>150</v>
       </c>
@@ -3248,8 +3253,8 @@
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="33"/>
-      <c r="B85" s="33"/>
+      <c r="A85" s="27"/>
+      <c r="B85" s="27"/>
       <c r="C85" s="8" t="s">
         <v>151</v>
       </c>
@@ -3264,7 +3269,7 @@
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="33" t="s">
+      <c r="A86" s="27" t="s">
         <v>37</v>
       </c>
       <c r="B86" s="4">
@@ -3284,7 +3289,7 @@
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="33"/>
+      <c r="A87" s="27"/>
       <c r="B87" s="4">
         <v>3108</v>
       </c>
@@ -3302,7 +3307,7 @@
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="33" t="s">
+      <c r="A88" s="27" t="s">
         <v>39</v>
       </c>
       <c r="B88" s="4">
@@ -3322,7 +3327,7 @@
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="33"/>
+      <c r="A89" s="27"/>
       <c r="B89" s="4">
         <v>3152</v>
       </c>
@@ -3340,7 +3345,7 @@
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="33"/>
+      <c r="A90" s="27"/>
       <c r="B90" s="4">
         <v>3152</v>
       </c>
@@ -3358,7 +3363,7 @@
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="33" t="s">
+      <c r="A91" s="27" t="s">
         <v>38</v>
       </c>
       <c r="B91" s="4">
@@ -3378,7 +3383,7 @@
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="33"/>
+      <c r="A92" s="27"/>
       <c r="B92" s="4">
         <v>3152</v>
       </c>
@@ -3396,7 +3401,7 @@
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="33"/>
+      <c r="A93" s="27"/>
       <c r="B93" s="4">
         <v>3152</v>
       </c>
@@ -3414,7 +3419,7 @@
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="33"/>
+      <c r="A94" s="27"/>
       <c r="B94" s="4">
         <v>3152</v>
       </c>
@@ -3432,7 +3437,7 @@
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="33"/>
+      <c r="A95" s="27"/>
       <c r="B95" s="4">
         <v>3152</v>
       </c>
@@ -3450,7 +3455,7 @@
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="33"/>
+      <c r="A96" s="27"/>
       <c r="B96" s="4">
         <v>3152</v>
       </c>
@@ -3468,7 +3473,7 @@
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="33"/>
+      <c r="A97" s="27"/>
       <c r="B97" s="4">
         <v>3152</v>
       </c>
@@ -3486,7 +3491,7 @@
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="33"/>
+      <c r="A98" s="27"/>
       <c r="B98" s="4">
         <v>3152</v>
       </c>
@@ -3504,7 +3509,7 @@
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="33"/>
+      <c r="A99" s="27"/>
       <c r="B99" s="4">
         <v>3152</v>
       </c>
@@ -3522,7 +3527,7 @@
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="33"/>
+      <c r="A100" s="27"/>
       <c r="B100" s="4">
         <v>3152</v>
       </c>
@@ -3540,7 +3545,7 @@
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="33"/>
+      <c r="A101" s="27"/>
       <c r="B101" s="4">
         <v>3152</v>
       </c>
@@ -3558,7 +3563,7 @@
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" s="33"/>
+      <c r="A102" s="27"/>
       <c r="B102" s="4">
         <v>3152</v>
       </c>
@@ -3576,7 +3581,7 @@
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="33"/>
+      <c r="A103" s="27"/>
       <c r="B103" s="4">
         <v>3108</v>
       </c>
@@ -3594,7 +3599,7 @@
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" s="33"/>
+      <c r="A104" s="27"/>
       <c r="B104" s="4">
         <v>3108</v>
       </c>
@@ -3612,7 +3617,7 @@
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="33"/>
+      <c r="A105" s="27"/>
       <c r="B105" s="4">
         <v>3108</v>
       </c>
@@ -3630,7 +3635,7 @@
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" s="33"/>
+      <c r="A106" s="27"/>
       <c r="B106" s="4">
         <v>3108</v>
       </c>
@@ -3648,7 +3653,7 @@
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107" s="33"/>
+      <c r="A107" s="27"/>
       <c r="B107" s="4">
         <v>3108</v>
       </c>
@@ -3666,7 +3671,7 @@
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A108" s="33"/>
+      <c r="A108" s="27"/>
       <c r="B108" s="4">
         <v>3108</v>
       </c>
@@ -3690,7 +3695,7 @@
       <c r="B109" s="30">
         <v>4029</v>
       </c>
-      <c r="C109" s="27">
+      <c r="C109" s="33">
         <v>1128271593</v>
       </c>
       <c r="D109" s="4" t="s">
@@ -3706,7 +3711,7 @@
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="31"/>
       <c r="B110" s="31"/>
-      <c r="C110" s="28"/>
+      <c r="C110" s="34"/>
       <c r="D110" s="4" t="s">
         <v>189</v>
       </c>
@@ -3720,7 +3725,7 @@
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="31"/>
       <c r="B111" s="31"/>
-      <c r="C111" s="28"/>
+      <c r="C111" s="34"/>
       <c r="D111" s="4" t="s">
         <v>190</v>
       </c>
@@ -3734,7 +3739,7 @@
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="31"/>
       <c r="B112" s="31"/>
-      <c r="C112" s="28"/>
+      <c r="C112" s="34"/>
       <c r="D112" s="4" t="s">
         <v>191</v>
       </c>
@@ -3748,7 +3753,7 @@
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="31"/>
       <c r="B113" s="31"/>
-      <c r="C113" s="28"/>
+      <c r="C113" s="34"/>
       <c r="D113" s="4" t="s">
         <v>192</v>
       </c>
@@ -3762,7 +3767,7 @@
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="31"/>
       <c r="B114" s="31"/>
-      <c r="C114" s="28"/>
+      <c r="C114" s="34"/>
       <c r="D114" s="4" t="s">
         <v>193</v>
       </c>
@@ -3776,7 +3781,7 @@
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="31"/>
       <c r="B115" s="31"/>
-      <c r="C115" s="28"/>
+      <c r="C115" s="34"/>
       <c r="D115" s="4" t="s">
         <v>194</v>
       </c>
@@ -3790,7 +3795,7 @@
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="31"/>
       <c r="B116" s="31"/>
-      <c r="C116" s="28"/>
+      <c r="C116" s="34"/>
       <c r="D116" s="4" t="s">
         <v>195</v>
       </c>
@@ -3804,7 +3809,7 @@
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="31"/>
       <c r="B117" s="31"/>
-      <c r="C117" s="28"/>
+      <c r="C117" s="34"/>
       <c r="D117" s="4" t="s">
         <v>196</v>
       </c>
@@ -3818,7 +3823,7 @@
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="31"/>
       <c r="B118" s="31"/>
-      <c r="C118" s="29"/>
+      <c r="C118" s="35"/>
       <c r="D118" s="4" t="s">
         <v>197</v>
       </c>
@@ -4061,6 +4066,31 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="C109:C118"/>
+    <mergeCell ref="B109:B126"/>
+    <mergeCell ref="C119:C126"/>
+    <mergeCell ref="C127:C134"/>
+    <mergeCell ref="B127:B134"/>
+    <mergeCell ref="A109:A134"/>
+    <mergeCell ref="A79:A85"/>
+    <mergeCell ref="B79:B85"/>
+    <mergeCell ref="A86:A87"/>
+    <mergeCell ref="A88:A90"/>
+    <mergeCell ref="A91:A108"/>
+    <mergeCell ref="A64:A65"/>
+    <mergeCell ref="A66:A78"/>
+    <mergeCell ref="B66:B78"/>
+    <mergeCell ref="A8:A63"/>
+    <mergeCell ref="C56:C63"/>
+    <mergeCell ref="B48:B63"/>
+    <mergeCell ref="C8:C15"/>
+    <mergeCell ref="E56:E63"/>
+    <mergeCell ref="C32:C39"/>
+    <mergeCell ref="E32:E39"/>
+    <mergeCell ref="C40:C47"/>
+    <mergeCell ref="E40:E47"/>
+    <mergeCell ref="C48:C55"/>
+    <mergeCell ref="E48:E55"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="A2:A7"/>
@@ -4070,31 +4100,6 @@
     <mergeCell ref="E16:E23"/>
     <mergeCell ref="C24:C31"/>
     <mergeCell ref="E24:E31"/>
-    <mergeCell ref="E56:E63"/>
-    <mergeCell ref="C32:C39"/>
-    <mergeCell ref="E32:E39"/>
-    <mergeCell ref="C40:C47"/>
-    <mergeCell ref="E40:E47"/>
-    <mergeCell ref="C48:C55"/>
-    <mergeCell ref="E48:E55"/>
-    <mergeCell ref="A64:A65"/>
-    <mergeCell ref="A66:A78"/>
-    <mergeCell ref="B66:B78"/>
-    <mergeCell ref="A8:A63"/>
-    <mergeCell ref="C56:C63"/>
-    <mergeCell ref="B48:B63"/>
-    <mergeCell ref="C8:C15"/>
-    <mergeCell ref="A109:A134"/>
-    <mergeCell ref="A79:A85"/>
-    <mergeCell ref="B79:B85"/>
-    <mergeCell ref="A86:A87"/>
-    <mergeCell ref="A88:A90"/>
-    <mergeCell ref="A91:A108"/>
-    <mergeCell ref="C109:C118"/>
-    <mergeCell ref="B109:B126"/>
-    <mergeCell ref="C119:C126"/>
-    <mergeCell ref="C127:C134"/>
-    <mergeCell ref="B127:B134"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4104,10 +4109,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D125"/>
+  <dimension ref="A1:D126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40:C70"/>
+    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="A126" sqref="A126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5866,6 +5871,11 @@
         <v>216</v>
       </c>
     </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>252</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Ajustes automatizacion modelo de autorizaciones
</commit_message>
<xml_diff>
--- a/src/test/resources/data_driven/EstructuraServicio.xlsx
+++ b/src/test/resources/data_driven/EstructuraServicio.xlsx
@@ -1516,13 +1516,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1534,13 +1534,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -2129,10 +2129,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="36">
+      <c r="B2" s="30">
         <v>4029</v>
       </c>
       <c r="C2" s="6">
@@ -2149,8 +2149,8 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="37"/>
-      <c r="B3" s="36"/>
+      <c r="A3" s="31"/>
+      <c r="B3" s="30"/>
       <c r="C3" s="6">
         <v>70129463</v>
       </c>
@@ -2165,8 +2165,8 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="37"/>
-      <c r="B4" s="36"/>
+      <c r="A4" s="31"/>
+      <c r="B4" s="30"/>
       <c r="C4" s="6">
         <v>43596238</v>
       </c>
@@ -2181,8 +2181,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="37"/>
-      <c r="B5" s="36">
+      <c r="A5" s="31"/>
+      <c r="B5" s="30">
         <v>2527</v>
       </c>
       <c r="C5" s="8">
@@ -2197,8 +2197,8 @@
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="37"/>
-      <c r="B6" s="36"/>
+      <c r="A6" s="31"/>
+      <c r="B6" s="30"/>
       <c r="C6" s="8">
         <v>71526214</v>
       </c>
@@ -2211,8 +2211,8 @@
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="37"/>
-      <c r="B7" s="36"/>
+      <c r="A7" s="31"/>
+      <c r="B7" s="30"/>
       <c r="C7" s="8">
         <v>43287144</v>
       </c>
@@ -2225,10 +2225,10 @@
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="36">
+      <c r="B8" s="30">
         <v>4029</v>
       </c>
       <c r="C8" s="33">
@@ -2237,7 +2237,7 @@
       <c r="D8" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="38" t="s">
+      <c r="E8" s="32" t="s">
         <v>52</v>
       </c>
       <c r="F8" s="8" t="s">
@@ -2245,99 +2245,99 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="36"/>
-      <c r="B9" s="36"/>
+      <c r="A9" s="30"/>
+      <c r="B9" s="30"/>
       <c r="C9" s="34"/>
       <c r="D9" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="E9" s="38"/>
+      <c r="E9" s="32"/>
       <c r="F9" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="36"/>
-      <c r="B10" s="36"/>
+      <c r="A10" s="30"/>
+      <c r="B10" s="30"/>
       <c r="C10" s="34"/>
       <c r="D10" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="38"/>
+      <c r="E10" s="32"/>
       <c r="F10" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="36"/>
-      <c r="B11" s="36"/>
+      <c r="A11" s="30"/>
+      <c r="B11" s="30"/>
       <c r="C11" s="34"/>
       <c r="D11" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="E11" s="38"/>
+      <c r="E11" s="32"/>
       <c r="F11" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="36"/>
-      <c r="B12" s="36"/>
+      <c r="A12" s="30"/>
+      <c r="B12" s="30"/>
       <c r="C12" s="34"/>
       <c r="D12" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="E12" s="38"/>
+      <c r="E12" s="32"/>
       <c r="F12" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="36"/>
-      <c r="B13" s="36"/>
+      <c r="A13" s="30"/>
+      <c r="B13" s="30"/>
       <c r="C13" s="34"/>
       <c r="D13" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="E13" s="38"/>
+      <c r="E13" s="32"/>
       <c r="F13" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="36"/>
-      <c r="B14" s="36"/>
+      <c r="A14" s="30"/>
+      <c r="B14" s="30"/>
       <c r="C14" s="34"/>
       <c r="D14" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="E14" s="38"/>
+      <c r="E14" s="32"/>
       <c r="F14" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="36"/>
-      <c r="B15" s="36"/>
+      <c r="A15" s="30"/>
+      <c r="B15" s="30"/>
       <c r="C15" s="35"/>
       <c r="D15" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="E15" s="38"/>
+      <c r="E15" s="32"/>
       <c r="F15" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="36"/>
-      <c r="B16" s="36"/>
+      <c r="A16" s="30"/>
+      <c r="B16" s="30"/>
       <c r="C16" s="33">
         <v>43618716</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="E16" s="38" t="s">
+      <c r="E16" s="32" t="s">
         <v>53</v>
       </c>
       <c r="F16" s="8" t="s">
@@ -2345,99 +2345,99 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="36"/>
-      <c r="B17" s="36"/>
+      <c r="A17" s="30"/>
+      <c r="B17" s="30"/>
       <c r="C17" s="34"/>
       <c r="D17" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="E17" s="38"/>
+      <c r="E17" s="32"/>
       <c r="F17" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="36"/>
-      <c r="B18" s="36"/>
+      <c r="A18" s="30"/>
+      <c r="B18" s="30"/>
       <c r="C18" s="34"/>
       <c r="D18" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="E18" s="38"/>
+      <c r="E18" s="32"/>
       <c r="F18" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
+      <c r="A19" s="30"/>
+      <c r="B19" s="30"/>
       <c r="C19" s="34"/>
       <c r="D19" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="38"/>
+      <c r="E19" s="32"/>
       <c r="F19" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="36"/>
-      <c r="B20" s="36"/>
+      <c r="A20" s="30"/>
+      <c r="B20" s="30"/>
       <c r="C20" s="34"/>
       <c r="D20" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="E20" s="38"/>
+      <c r="E20" s="32"/>
       <c r="F20" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="36"/>
-      <c r="B21" s="36"/>
+      <c r="A21" s="30"/>
+      <c r="B21" s="30"/>
       <c r="C21" s="34"/>
       <c r="D21" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="E21" s="38"/>
+      <c r="E21" s="32"/>
       <c r="F21" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="36"/>
-      <c r="B22" s="36"/>
+      <c r="A22" s="30"/>
+      <c r="B22" s="30"/>
       <c r="C22" s="34"/>
       <c r="D22" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="E22" s="38"/>
+      <c r="E22" s="32"/>
       <c r="F22" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="36"/>
-      <c r="B23" s="36"/>
+      <c r="A23" s="30"/>
+      <c r="B23" s="30"/>
       <c r="C23" s="35"/>
       <c r="D23" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="E23" s="38"/>
+      <c r="E23" s="32"/>
       <c r="F23" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="36"/>
-      <c r="B24" s="36"/>
+      <c r="A24" s="30"/>
+      <c r="B24" s="30"/>
       <c r="C24" s="33">
         <v>71698481</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="E24" s="38" t="s">
+      <c r="E24" s="32" t="s">
         <v>54</v>
       </c>
       <c r="F24" s="8" t="s">
@@ -2445,99 +2445,99 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="36"/>
-      <c r="B25" s="36"/>
+      <c r="A25" s="30"/>
+      <c r="B25" s="30"/>
       <c r="C25" s="34"/>
       <c r="D25" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="E25" s="38"/>
+      <c r="E25" s="32"/>
       <c r="F25" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="36"/>
-      <c r="B26" s="36"/>
+      <c r="A26" s="30"/>
+      <c r="B26" s="30"/>
       <c r="C26" s="34"/>
       <c r="D26" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="E26" s="38"/>
+      <c r="E26" s="32"/>
       <c r="F26" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="36"/>
-      <c r="B27" s="36"/>
+      <c r="A27" s="30"/>
+      <c r="B27" s="30"/>
       <c r="C27" s="34"/>
       <c r="D27" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="E27" s="38"/>
+      <c r="E27" s="32"/>
       <c r="F27" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="36"/>
-      <c r="B28" s="36"/>
+      <c r="A28" s="30"/>
+      <c r="B28" s="30"/>
       <c r="C28" s="34"/>
       <c r="D28" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="E28" s="38"/>
+      <c r="E28" s="32"/>
       <c r="F28" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="36"/>
-      <c r="B29" s="36"/>
+      <c r="A29" s="30"/>
+      <c r="B29" s="30"/>
       <c r="C29" s="34"/>
       <c r="D29" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="E29" s="38"/>
+      <c r="E29" s="32"/>
       <c r="F29" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="36"/>
-      <c r="B30" s="36"/>
+      <c r="A30" s="30"/>
+      <c r="B30" s="30"/>
       <c r="C30" s="34"/>
       <c r="D30" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="E30" s="38"/>
+      <c r="E30" s="32"/>
       <c r="F30" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="36"/>
-      <c r="B31" s="36"/>
+      <c r="A31" s="30"/>
+      <c r="B31" s="30"/>
       <c r="C31" s="35"/>
       <c r="D31" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="E31" s="38"/>
+      <c r="E31" s="32"/>
       <c r="F31" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="36"/>
-      <c r="B32" s="36"/>
+      <c r="A32" s="30"/>
+      <c r="B32" s="30"/>
       <c r="C32" s="33">
         <v>43520997</v>
       </c>
       <c r="D32" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="E32" s="38" t="s">
+      <c r="E32" s="32" t="s">
         <v>55</v>
       </c>
       <c r="F32" s="8" t="s">
@@ -2545,99 +2545,99 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="36"/>
-      <c r="B33" s="36"/>
+      <c r="A33" s="30"/>
+      <c r="B33" s="30"/>
       <c r="C33" s="34"/>
       <c r="D33" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="E33" s="38"/>
+      <c r="E33" s="32"/>
       <c r="F33" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="36"/>
-      <c r="B34" s="36"/>
+      <c r="A34" s="30"/>
+      <c r="B34" s="30"/>
       <c r="C34" s="34"/>
       <c r="D34" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="E34" s="38"/>
+      <c r="E34" s="32"/>
       <c r="F34" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="36"/>
-      <c r="B35" s="36"/>
+      <c r="A35" s="30"/>
+      <c r="B35" s="30"/>
       <c r="C35" s="34"/>
       <c r="D35" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="E35" s="38"/>
+      <c r="E35" s="32"/>
       <c r="F35" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="36"/>
-      <c r="B36" s="36"/>
+      <c r="A36" s="30"/>
+      <c r="B36" s="30"/>
       <c r="C36" s="34"/>
       <c r="D36" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="E36" s="38"/>
+      <c r="E36" s="32"/>
       <c r="F36" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="36"/>
-      <c r="B37" s="36"/>
+      <c r="A37" s="30"/>
+      <c r="B37" s="30"/>
       <c r="C37" s="34"/>
       <c r="D37" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E37" s="38"/>
+      <c r="E37" s="32"/>
       <c r="F37" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="36"/>
-      <c r="B38" s="36"/>
+      <c r="A38" s="30"/>
+      <c r="B38" s="30"/>
       <c r="C38" s="34"/>
       <c r="D38" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="E38" s="38"/>
+      <c r="E38" s="32"/>
       <c r="F38" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="36"/>
-      <c r="B39" s="36"/>
+      <c r="A39" s="30"/>
+      <c r="B39" s="30"/>
       <c r="C39" s="35"/>
       <c r="D39" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="E39" s="38"/>
+      <c r="E39" s="32"/>
       <c r="F39" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="36"/>
-      <c r="B40" s="36"/>
+      <c r="A40" s="30"/>
+      <c r="B40" s="30"/>
       <c r="C40" s="33">
         <v>43527460</v>
       </c>
       <c r="D40" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="E40" s="38" t="s">
+      <c r="E40" s="32" t="s">
         <v>56</v>
       </c>
       <c r="F40" s="8" t="s">
@@ -2645,101 +2645,101 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="36"/>
-      <c r="B41" s="36"/>
+      <c r="A41" s="30"/>
+      <c r="B41" s="30"/>
       <c r="C41" s="34"/>
       <c r="D41" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="E41" s="38"/>
+      <c r="E41" s="32"/>
       <c r="F41" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="36"/>
-      <c r="B42" s="36"/>
+      <c r="A42" s="30"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="34"/>
       <c r="D42" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="E42" s="38"/>
+      <c r="E42" s="32"/>
       <c r="F42" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="36"/>
-      <c r="B43" s="36"/>
+      <c r="A43" s="30"/>
+      <c r="B43" s="30"/>
       <c r="C43" s="34"/>
       <c r="D43" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="E43" s="38"/>
+      <c r="E43" s="32"/>
       <c r="F43" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="30"/>
+      <c r="B44" s="30"/>
       <c r="C44" s="34"/>
       <c r="D44" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="E44" s="38"/>
+      <c r="E44" s="32"/>
       <c r="F44" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
+      <c r="A45" s="30"/>
+      <c r="B45" s="30"/>
       <c r="C45" s="34"/>
       <c r="D45" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="E45" s="38"/>
+      <c r="E45" s="32"/>
       <c r="F45" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="36"/>
-      <c r="B46" s="36"/>
+      <c r="A46" s="30"/>
+      <c r="B46" s="30"/>
       <c r="C46" s="34"/>
       <c r="D46" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="E46" s="38"/>
+      <c r="E46" s="32"/>
       <c r="F46" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="36"/>
-      <c r="B47" s="36"/>
+      <c r="A47" s="30"/>
+      <c r="B47" s="30"/>
       <c r="C47" s="35"/>
       <c r="D47" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="E47" s="38"/>
+      <c r="E47" s="32"/>
       <c r="F47" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="36"/>
-      <c r="B48" s="36">
+      <c r="A48" s="30"/>
+      <c r="B48" s="30">
         <v>2527</v>
       </c>
-      <c r="C48" s="37">
+      <c r="C48" s="31">
         <v>32143454</v>
       </c>
       <c r="D48" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="E48" s="37" t="s">
+      <c r="E48" s="31" t="s">
         <v>97</v>
       </c>
       <c r="F48" s="8" t="s">
@@ -2747,99 +2747,99 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="36"/>
-      <c r="B49" s="36"/>
-      <c r="C49" s="37"/>
+      <c r="A49" s="30"/>
+      <c r="B49" s="30"/>
+      <c r="C49" s="31"/>
       <c r="D49" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="E49" s="37"/>
+      <c r="E49" s="31"/>
       <c r="F49" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="36"/>
-      <c r="B50" s="36"/>
-      <c r="C50" s="37"/>
+      <c r="A50" s="30"/>
+      <c r="B50" s="30"/>
+      <c r="C50" s="31"/>
       <c r="D50" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="E50" s="37"/>
+      <c r="E50" s="31"/>
       <c r="F50" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="36"/>
-      <c r="B51" s="36"/>
-      <c r="C51" s="37"/>
+      <c r="A51" s="30"/>
+      <c r="B51" s="30"/>
+      <c r="C51" s="31"/>
       <c r="D51" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="E51" s="37"/>
+      <c r="E51" s="31"/>
       <c r="F51" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="36"/>
-      <c r="B52" s="36"/>
-      <c r="C52" s="37"/>
+      <c r="A52" s="30"/>
+      <c r="B52" s="30"/>
+      <c r="C52" s="31"/>
       <c r="D52" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="E52" s="37"/>
+      <c r="E52" s="31"/>
       <c r="F52" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="36"/>
-      <c r="B53" s="36"/>
-      <c r="C53" s="37"/>
+      <c r="A53" s="30"/>
+      <c r="B53" s="30"/>
+      <c r="C53" s="31"/>
       <c r="D53" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="E53" s="37"/>
+      <c r="E53" s="31"/>
       <c r="F53" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="36"/>
-      <c r="B54" s="36"/>
-      <c r="C54" s="37"/>
+      <c r="A54" s="30"/>
+      <c r="B54" s="30"/>
+      <c r="C54" s="31"/>
       <c r="D54" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="E54" s="37"/>
+      <c r="E54" s="31"/>
       <c r="F54" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="36"/>
-      <c r="B55" s="36"/>
-      <c r="C55" s="37"/>
+      <c r="A55" s="30"/>
+      <c r="B55" s="30"/>
+      <c r="C55" s="31"/>
       <c r="D55" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="E55" s="37"/>
+      <c r="E55" s="31"/>
       <c r="F55" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="36"/>
-      <c r="B56" s="36"/>
-      <c r="C56" s="37">
+      <c r="A56" s="30"/>
+      <c r="B56" s="30"/>
+      <c r="C56" s="31">
         <v>42790786</v>
       </c>
       <c r="D56" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="E56" s="37" t="s">
+      <c r="E56" s="31" t="s">
         <v>98</v>
       </c>
       <c r="F56" s="8" t="s">
@@ -2847,91 +2847,91 @@
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="36"/>
-      <c r="B57" s="36"/>
-      <c r="C57" s="37"/>
+      <c r="A57" s="30"/>
+      <c r="B57" s="30"/>
+      <c r="C57" s="31"/>
       <c r="D57" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="E57" s="37"/>
+      <c r="E57" s="31"/>
       <c r="F57" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="36"/>
-      <c r="B58" s="36"/>
-      <c r="C58" s="37"/>
+      <c r="A58" s="30"/>
+      <c r="B58" s="30"/>
+      <c r="C58" s="31"/>
       <c r="D58" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="E58" s="37"/>
+      <c r="E58" s="31"/>
       <c r="F58" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="36"/>
-      <c r="B59" s="36"/>
-      <c r="C59" s="37"/>
+      <c r="A59" s="30"/>
+      <c r="B59" s="30"/>
+      <c r="C59" s="31"/>
       <c r="D59" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="E59" s="37"/>
+      <c r="E59" s="31"/>
       <c r="F59" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="36"/>
-      <c r="B60" s="36"/>
-      <c r="C60" s="37"/>
+      <c r="A60" s="30"/>
+      <c r="B60" s="30"/>
+      <c r="C60" s="31"/>
       <c r="D60" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="E60" s="37"/>
+      <c r="E60" s="31"/>
       <c r="F60" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="36"/>
-      <c r="B61" s="36"/>
-      <c r="C61" s="37"/>
+      <c r="A61" s="30"/>
+      <c r="B61" s="30"/>
+      <c r="C61" s="31"/>
       <c r="D61" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="E61" s="37"/>
+      <c r="E61" s="31"/>
       <c r="F61" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="36"/>
-      <c r="B62" s="36"/>
-      <c r="C62" s="37"/>
+      <c r="A62" s="30"/>
+      <c r="B62" s="30"/>
+      <c r="C62" s="31"/>
       <c r="D62" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="E62" s="37"/>
+      <c r="E62" s="31"/>
       <c r="F62" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="36"/>
-      <c r="B63" s="36"/>
-      <c r="C63" s="37"/>
+      <c r="A63" s="30"/>
+      <c r="B63" s="30"/>
+      <c r="C63" s="31"/>
       <c r="D63" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="E63" s="37"/>
+      <c r="E63" s="31"/>
       <c r="F63" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="36" t="s">
+      <c r="A64" s="30" t="s">
         <v>34</v>
       </c>
       <c r="B64" s="4">
@@ -2951,7 +2951,7 @@
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="36"/>
+      <c r="A65" s="30"/>
       <c r="B65" s="4">
         <v>2527</v>
       </c>
@@ -2969,10 +2969,10 @@
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="36" t="s">
+      <c r="A66" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="B66" s="36" t="s">
+      <c r="B66" s="30" t="s">
         <v>51</v>
       </c>
       <c r="C66" s="8" t="s">
@@ -2989,8 +2989,8 @@
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="36"/>
-      <c r="B67" s="36"/>
+      <c r="A67" s="30"/>
+      <c r="B67" s="30"/>
       <c r="C67" s="8" t="s">
         <v>117</v>
       </c>
@@ -3005,8 +3005,8 @@
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="36"/>
-      <c r="B68" s="36"/>
+      <c r="A68" s="30"/>
+      <c r="B68" s="30"/>
       <c r="C68" s="8" t="s">
         <v>118</v>
       </c>
@@ -3021,8 +3021,8 @@
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="36"/>
-      <c r="B69" s="36"/>
+      <c r="A69" s="30"/>
+      <c r="B69" s="30"/>
       <c r="C69" s="8" t="s">
         <v>119</v>
       </c>
@@ -3037,8 +3037,8 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="36"/>
-      <c r="B70" s="36"/>
+      <c r="A70" s="30"/>
+      <c r="B70" s="30"/>
       <c r="C70" s="8" t="s">
         <v>120</v>
       </c>
@@ -3053,8 +3053,8 @@
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="36"/>
-      <c r="B71" s="36"/>
+      <c r="A71" s="30"/>
+      <c r="B71" s="30"/>
       <c r="C71" s="8" t="s">
         <v>121</v>
       </c>
@@ -3069,8 +3069,8 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="36"/>
-      <c r="B72" s="36"/>
+      <c r="A72" s="30"/>
+      <c r="B72" s="30"/>
       <c r="C72" s="8" t="s">
         <v>122</v>
       </c>
@@ -3085,8 +3085,8 @@
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="36"/>
-      <c r="B73" s="36"/>
+      <c r="A73" s="30"/>
+      <c r="B73" s="30"/>
       <c r="C73" s="8" t="s">
         <v>123</v>
       </c>
@@ -3101,8 +3101,8 @@
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="36"/>
-      <c r="B74" s="36"/>
+      <c r="A74" s="30"/>
+      <c r="B74" s="30"/>
       <c r="C74" s="8" t="s">
         <v>124</v>
       </c>
@@ -3117,8 +3117,8 @@
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="36"/>
-      <c r="B75" s="36"/>
+      <c r="A75" s="30"/>
+      <c r="B75" s="30"/>
       <c r="C75" s="8" t="s">
         <v>125</v>
       </c>
@@ -3133,8 +3133,8 @@
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="36"/>
-      <c r="B76" s="36"/>
+      <c r="A76" s="30"/>
+      <c r="B76" s="30"/>
       <c r="C76" s="8" t="s">
         <v>126</v>
       </c>
@@ -3149,8 +3149,8 @@
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="36"/>
-      <c r="B77" s="36"/>
+      <c r="A77" s="30"/>
+      <c r="B77" s="30"/>
       <c r="C77" s="8" t="s">
         <v>127</v>
       </c>
@@ -3165,8 +3165,8 @@
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="36"/>
-      <c r="B78" s="36"/>
+      <c r="A78" s="30"/>
+      <c r="B78" s="30"/>
       <c r="C78" s="8" t="s">
         <v>128</v>
       </c>
@@ -3181,10 +3181,10 @@
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="36" t="s">
+      <c r="A79" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="B79" s="36">
+      <c r="B79" s="30">
         <v>4029</v>
       </c>
       <c r="C79" s="8" t="s">
@@ -3201,8 +3201,8 @@
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="36"/>
-      <c r="B80" s="36"/>
+      <c r="A80" s="30"/>
+      <c r="B80" s="30"/>
       <c r="C80" s="8" t="s">
         <v>146</v>
       </c>
@@ -3217,8 +3217,8 @@
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="36"/>
-      <c r="B81" s="36"/>
+      <c r="A81" s="30"/>
+      <c r="B81" s="30"/>
       <c r="C81" s="8" t="s">
         <v>147</v>
       </c>
@@ -3233,8 +3233,8 @@
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="36"/>
-      <c r="B82" s="36"/>
+      <c r="A82" s="30"/>
+      <c r="B82" s="30"/>
       <c r="C82" s="8" t="s">
         <v>148</v>
       </c>
@@ -3249,8 +3249,8 @@
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="36"/>
-      <c r="B83" s="36"/>
+      <c r="A83" s="30"/>
+      <c r="B83" s="30"/>
       <c r="C83" s="8" t="s">
         <v>149</v>
       </c>
@@ -3265,8 +3265,8 @@
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="36"/>
-      <c r="B84" s="36"/>
+      <c r="A84" s="30"/>
+      <c r="B84" s="30"/>
       <c r="C84" s="8" t="s">
         <v>150</v>
       </c>
@@ -3281,8 +3281,8 @@
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="36"/>
-      <c r="B85" s="36"/>
+      <c r="A85" s="30"/>
+      <c r="B85" s="30"/>
       <c r="C85" s="8" t="s">
         <v>151</v>
       </c>
@@ -3297,7 +3297,7 @@
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="36" t="s">
+      <c r="A86" s="30" t="s">
         <v>37</v>
       </c>
       <c r="B86" s="4">
@@ -3317,7 +3317,7 @@
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="36"/>
+      <c r="A87" s="30"/>
       <c r="B87" s="4">
         <v>3108</v>
       </c>
@@ -3335,7 +3335,7 @@
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="36" t="s">
+      <c r="A88" s="30" t="s">
         <v>39</v>
       </c>
       <c r="B88" s="4">
@@ -3355,7 +3355,7 @@
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="36"/>
+      <c r="A89" s="30"/>
       <c r="B89" s="4">
         <v>3152</v>
       </c>
@@ -3373,7 +3373,7 @@
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="36"/>
+      <c r="A90" s="30"/>
       <c r="B90" s="4">
         <v>3152</v>
       </c>
@@ -3391,7 +3391,7 @@
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="36" t="s">
+      <c r="A91" s="30" t="s">
         <v>38</v>
       </c>
       <c r="B91" s="4">
@@ -3411,7 +3411,7 @@
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="36"/>
+      <c r="A92" s="30"/>
       <c r="B92" s="4">
         <v>3152</v>
       </c>
@@ -3429,7 +3429,7 @@
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="36"/>
+      <c r="A93" s="30"/>
       <c r="B93" s="4">
         <v>3152</v>
       </c>
@@ -3447,7 +3447,7 @@
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="36"/>
+      <c r="A94" s="30"/>
       <c r="B94" s="4">
         <v>3152</v>
       </c>
@@ -3465,7 +3465,7 @@
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="36"/>
+      <c r="A95" s="30"/>
       <c r="B95" s="4">
         <v>3152</v>
       </c>
@@ -3483,7 +3483,7 @@
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="36"/>
+      <c r="A96" s="30"/>
       <c r="B96" s="4">
         <v>3152</v>
       </c>
@@ -3501,7 +3501,7 @@
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="36"/>
+      <c r="A97" s="30"/>
       <c r="B97" s="4">
         <v>3152</v>
       </c>
@@ -3519,7 +3519,7 @@
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="36"/>
+      <c r="A98" s="30"/>
       <c r="B98" s="4">
         <v>3152</v>
       </c>
@@ -3537,7 +3537,7 @@
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="36"/>
+      <c r="A99" s="30"/>
       <c r="B99" s="4">
         <v>3152</v>
       </c>
@@ -3555,7 +3555,7 @@
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="36"/>
+      <c r="A100" s="30"/>
       <c r="B100" s="4">
         <v>3152</v>
       </c>
@@ -3573,7 +3573,7 @@
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="36"/>
+      <c r="A101" s="30"/>
       <c r="B101" s="4">
         <v>3152</v>
       </c>
@@ -3591,7 +3591,7 @@
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" s="36"/>
+      <c r="A102" s="30"/>
       <c r="B102" s="4">
         <v>3152</v>
       </c>
@@ -3609,7 +3609,7 @@
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="36"/>
+      <c r="A103" s="30"/>
       <c r="B103" s="4">
         <v>3108</v>
       </c>
@@ -3627,7 +3627,7 @@
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" s="36"/>
+      <c r="A104" s="30"/>
       <c r="B104" s="4">
         <v>3108</v>
       </c>
@@ -3645,7 +3645,7 @@
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="36"/>
+      <c r="A105" s="30"/>
       <c r="B105" s="4">
         <v>3108</v>
       </c>
@@ -3663,7 +3663,7 @@
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" s="36"/>
+      <c r="A106" s="30"/>
       <c r="B106" s="4">
         <v>3108</v>
       </c>
@@ -3681,7 +3681,7 @@
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107" s="36"/>
+      <c r="A107" s="30"/>
       <c r="B107" s="4">
         <v>3108</v>
       </c>
@@ -3699,7 +3699,7 @@
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A108" s="36"/>
+      <c r="A108" s="30"/>
       <c r="B108" s="4">
         <v>3108</v>
       </c>
@@ -3723,7 +3723,7 @@
       <c r="B109" s="33">
         <v>4029</v>
       </c>
-      <c r="C109" s="30">
+      <c r="C109" s="36">
         <v>1128271593</v>
       </c>
       <c r="D109" s="4" t="s">
@@ -3739,7 +3739,7 @@
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="34"/>
       <c r="B110" s="34"/>
-      <c r="C110" s="31"/>
+      <c r="C110" s="37"/>
       <c r="D110" s="4" t="s">
         <v>189</v>
       </c>
@@ -3753,7 +3753,7 @@
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="34"/>
       <c r="B111" s="34"/>
-      <c r="C111" s="31"/>
+      <c r="C111" s="37"/>
       <c r="D111" s="4" t="s">
         <v>190</v>
       </c>
@@ -3767,7 +3767,7 @@
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="34"/>
       <c r="B112" s="34"/>
-      <c r="C112" s="31"/>
+      <c r="C112" s="37"/>
       <c r="D112" s="4" t="s">
         <v>191</v>
       </c>
@@ -3781,7 +3781,7 @@
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="34"/>
       <c r="B113" s="34"/>
-      <c r="C113" s="31"/>
+      <c r="C113" s="37"/>
       <c r="D113" s="4" t="s">
         <v>192</v>
       </c>
@@ -3795,7 +3795,7 @@
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="34"/>
       <c r="B114" s="34"/>
-      <c r="C114" s="31"/>
+      <c r="C114" s="37"/>
       <c r="D114" s="4" t="s">
         <v>193</v>
       </c>
@@ -3809,7 +3809,7 @@
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="34"/>
       <c r="B115" s="34"/>
-      <c r="C115" s="31"/>
+      <c r="C115" s="37"/>
       <c r="D115" s="4" t="s">
         <v>194</v>
       </c>
@@ -3823,7 +3823,7 @@
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="34"/>
       <c r="B116" s="34"/>
-      <c r="C116" s="31"/>
+      <c r="C116" s="37"/>
       <c r="D116" s="4" t="s">
         <v>195</v>
       </c>
@@ -3837,7 +3837,7 @@
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="34"/>
       <c r="B117" s="34"/>
-      <c r="C117" s="31"/>
+      <c r="C117" s="37"/>
       <c r="D117" s="4" t="s">
         <v>196</v>
       </c>
@@ -3851,7 +3851,7 @@
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="34"/>
       <c r="B118" s="34"/>
-      <c r="C118" s="32"/>
+      <c r="C118" s="38"/>
       <c r="D118" s="4" t="s">
         <v>197</v>
       </c>
@@ -4094,6 +4094,31 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="C109:C118"/>
+    <mergeCell ref="B109:B126"/>
+    <mergeCell ref="C119:C126"/>
+    <mergeCell ref="C127:C134"/>
+    <mergeCell ref="B127:B134"/>
+    <mergeCell ref="A109:A134"/>
+    <mergeCell ref="A79:A85"/>
+    <mergeCell ref="B79:B85"/>
+    <mergeCell ref="A86:A87"/>
+    <mergeCell ref="A88:A90"/>
+    <mergeCell ref="A91:A108"/>
+    <mergeCell ref="A64:A65"/>
+    <mergeCell ref="A66:A78"/>
+    <mergeCell ref="B66:B78"/>
+    <mergeCell ref="A8:A63"/>
+    <mergeCell ref="C56:C63"/>
+    <mergeCell ref="B48:B63"/>
+    <mergeCell ref="C8:C15"/>
+    <mergeCell ref="E56:E63"/>
+    <mergeCell ref="C32:C39"/>
+    <mergeCell ref="E32:E39"/>
+    <mergeCell ref="C40:C47"/>
+    <mergeCell ref="E40:E47"/>
+    <mergeCell ref="C48:C55"/>
+    <mergeCell ref="E48:E55"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="A2:A7"/>
@@ -4103,31 +4128,6 @@
     <mergeCell ref="E16:E23"/>
     <mergeCell ref="C24:C31"/>
     <mergeCell ref="E24:E31"/>
-    <mergeCell ref="E56:E63"/>
-    <mergeCell ref="C32:C39"/>
-    <mergeCell ref="E32:E39"/>
-    <mergeCell ref="C40:C47"/>
-    <mergeCell ref="E40:E47"/>
-    <mergeCell ref="C48:C55"/>
-    <mergeCell ref="E48:E55"/>
-    <mergeCell ref="A64:A65"/>
-    <mergeCell ref="A66:A78"/>
-    <mergeCell ref="B66:B78"/>
-    <mergeCell ref="A8:A63"/>
-    <mergeCell ref="C56:C63"/>
-    <mergeCell ref="B48:B63"/>
-    <mergeCell ref="C8:C15"/>
-    <mergeCell ref="A109:A134"/>
-    <mergeCell ref="A79:A85"/>
-    <mergeCell ref="B79:B85"/>
-    <mergeCell ref="A86:A87"/>
-    <mergeCell ref="A88:A90"/>
-    <mergeCell ref="A91:A108"/>
-    <mergeCell ref="C109:C118"/>
-    <mergeCell ref="B109:B126"/>
-    <mergeCell ref="C119:C126"/>
-    <mergeCell ref="C127:C134"/>
-    <mergeCell ref="B127:B134"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4139,8 +4139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B74" workbookViewId="0">
-      <selection activeCell="B95" sqref="B77:D95"/>
+    <sheetView tabSelected="1" topLeftCell="B80" workbookViewId="0">
+      <selection activeCell="D95" sqref="D95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Se modifica metodo plan de trabajo para el modelo de autorizaciones
</commit_message>
<xml_diff>
--- a/src/test/resources/data_driven/EstructuraServicio.xlsx
+++ b/src/test/resources/data_driven/EstructuraServicio.xlsx
@@ -380,7 +380,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1202" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1202" uniqueCount="300">
   <si>
     <t>Buscar Auxiliares de expedición asociados al parámetro + Su ubicación física de acuerdo al código de oficina</t>
   </si>
@@ -1283,6 +1283,9 @@
   </si>
   <si>
     <t xml:space="preserve"> jimecame</t>
+  </si>
+  <si>
+    <t>La fecha inicio de vigencia no cumple con el parámetro de retroactividad definido (60 dias)</t>
   </si>
 </sst>
 </file>
@@ -4139,8 +4142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B74" workbookViewId="0">
-      <selection activeCell="C88" sqref="C88"/>
+    <sheetView tabSelected="1" topLeftCell="A147" workbookViewId="0">
+      <selection activeCell="A161" sqref="A161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6351,13 +6354,13 @@
     </row>
     <row r="158" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A158" s="22" t="s">
-        <v>248</v>
+        <v>299</v>
       </c>
       <c r="B158" s="23" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="C158" s="24" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D158" s="17" t="s">
         <v>215</v>
@@ -6368,10 +6371,10 @@
         <v>249</v>
       </c>
       <c r="B159" s="23" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="C159" s="24" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D159" s="17" t="s">
         <v>215</v>

</xml_diff>

<commit_message>
Ajustes modelo de autorizaciones
</commit_message>
<xml_diff>
--- a/src/test/resources/data_driven/EstructuraServicio.xlsx
+++ b/src/test/resources/data_driven/EstructuraServicio.xlsx
@@ -380,7 +380,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1202" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1262" uniqueCount="299">
   <si>
     <t>Buscar Auxiliares de expedición asociados al parámetro + Su ubicación física de acuerdo al código de oficina</t>
   </si>
@@ -1283,9 +1283,6 @@
   </si>
   <si>
     <t xml:space="preserve"> jimecame</t>
-  </si>
-  <si>
-    <t>La fecha inicio de vigencia no cumple con el parámetro de retroactividad definido (60 dias)</t>
   </si>
 </sst>
 </file>
@@ -1362,7 +1359,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1378,6 +1375,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1456,7 +1459,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1511,6 +1514,22 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1868,28 +1887,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="28"/>
+      <c r="F1" s="36"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
       <c r="E2" s="2" t="s">
         <v>27</v>
       </c>
@@ -2132,10 +2151,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="36">
+      <c r="B2" s="44">
         <v>4029</v>
       </c>
       <c r="C2" s="6">
@@ -2152,8 +2171,8 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="37"/>
-      <c r="B3" s="36"/>
+      <c r="A3" s="45"/>
+      <c r="B3" s="44"/>
       <c r="C3" s="6">
         <v>70129463</v>
       </c>
@@ -2168,8 +2187,8 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="37"/>
-      <c r="B4" s="36"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="44"/>
       <c r="C4" s="6">
         <v>43596238</v>
       </c>
@@ -2184,8 +2203,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="37"/>
-      <c r="B5" s="36">
+      <c r="A5" s="45"/>
+      <c r="B5" s="44">
         <v>2527</v>
       </c>
       <c r="C5" s="8">
@@ -2200,8 +2219,8 @@
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="37"/>
-      <c r="B6" s="36"/>
+      <c r="A6" s="45"/>
+      <c r="B6" s="44"/>
       <c r="C6" s="8">
         <v>71526214</v>
       </c>
@@ -2214,8 +2233,8 @@
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="37"/>
-      <c r="B7" s="36"/>
+      <c r="A7" s="45"/>
+      <c r="B7" s="44"/>
       <c r="C7" s="8">
         <v>43287144</v>
       </c>
@@ -2228,19 +2247,19 @@
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="36">
+      <c r="B8" s="44">
         <v>4029</v>
       </c>
-      <c r="C8" s="33">
+      <c r="C8" s="41">
         <v>43628391</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="38" t="s">
+      <c r="E8" s="46" t="s">
         <v>52</v>
       </c>
       <c r="F8" s="8" t="s">
@@ -2248,99 +2267,99 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="36"/>
-      <c r="B9" s="36"/>
-      <c r="C9" s="34"/>
+      <c r="A9" s="44"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="42"/>
       <c r="D9" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="E9" s="38"/>
+      <c r="E9" s="46"/>
       <c r="F9" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="36"/>
-      <c r="B10" s="36"/>
-      <c r="C10" s="34"/>
+      <c r="A10" s="44"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="42"/>
       <c r="D10" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="38"/>
+      <c r="E10" s="46"/>
       <c r="F10" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="36"/>
-      <c r="B11" s="36"/>
-      <c r="C11" s="34"/>
+      <c r="A11" s="44"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="42"/>
       <c r="D11" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="E11" s="38"/>
+      <c r="E11" s="46"/>
       <c r="F11" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="36"/>
-      <c r="B12" s="36"/>
-      <c r="C12" s="34"/>
+      <c r="A12" s="44"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="42"/>
       <c r="D12" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="E12" s="38"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="36"/>
-      <c r="B13" s="36"/>
-      <c r="C13" s="34"/>
+      <c r="A13" s="44"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="42"/>
       <c r="D13" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="E13" s="38"/>
+      <c r="E13" s="46"/>
       <c r="F13" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="36"/>
-      <c r="B14" s="36"/>
-      <c r="C14" s="34"/>
+      <c r="A14" s="44"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="42"/>
       <c r="D14" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="E14" s="38"/>
+      <c r="E14" s="46"/>
       <c r="F14" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="36"/>
-      <c r="B15" s="36"/>
-      <c r="C15" s="35"/>
+      <c r="A15" s="44"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="43"/>
       <c r="D15" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="E15" s="38"/>
+      <c r="E15" s="46"/>
       <c r="F15" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="36"/>
-      <c r="B16" s="36"/>
-      <c r="C16" s="33">
+      <c r="A16" s="44"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="41">
         <v>43618716</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="E16" s="38" t="s">
+      <c r="E16" s="46" t="s">
         <v>53</v>
       </c>
       <c r="F16" s="8" t="s">
@@ -2348,99 +2367,99 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="36"/>
-      <c r="B17" s="36"/>
-      <c r="C17" s="34"/>
+      <c r="A17" s="44"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="42"/>
       <c r="D17" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="E17" s="38"/>
+      <c r="E17" s="46"/>
       <c r="F17" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="36"/>
-      <c r="B18" s="36"/>
-      <c r="C18" s="34"/>
+      <c r="A18" s="44"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="42"/>
       <c r="D18" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="E18" s="38"/>
+      <c r="E18" s="46"/>
       <c r="F18" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
-      <c r="C19" s="34"/>
+      <c r="A19" s="44"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="42"/>
       <c r="D19" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="38"/>
+      <c r="E19" s="46"/>
       <c r="F19" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="36"/>
-      <c r="B20" s="36"/>
-      <c r="C20" s="34"/>
+      <c r="A20" s="44"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="42"/>
       <c r="D20" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="E20" s="38"/>
+      <c r="E20" s="46"/>
       <c r="F20" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="36"/>
-      <c r="B21" s="36"/>
-      <c r="C21" s="34"/>
+      <c r="A21" s="44"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="42"/>
       <c r="D21" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="E21" s="38"/>
+      <c r="E21" s="46"/>
       <c r="F21" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="36"/>
-      <c r="B22" s="36"/>
-      <c r="C22" s="34"/>
+      <c r="A22" s="44"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="42"/>
       <c r="D22" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="E22" s="38"/>
+      <c r="E22" s="46"/>
       <c r="F22" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="36"/>
-      <c r="B23" s="36"/>
-      <c r="C23" s="35"/>
+      <c r="A23" s="44"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="43"/>
       <c r="D23" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="E23" s="38"/>
+      <c r="E23" s="46"/>
       <c r="F23" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="36"/>
-      <c r="B24" s="36"/>
-      <c r="C24" s="33">
+      <c r="A24" s="44"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="41">
         <v>71698481</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="E24" s="38" t="s">
+      <c r="E24" s="46" t="s">
         <v>54</v>
       </c>
       <c r="F24" s="8" t="s">
@@ -2448,99 +2467,99 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="36"/>
-      <c r="B25" s="36"/>
-      <c r="C25" s="34"/>
+      <c r="A25" s="44"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="42"/>
       <c r="D25" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="E25" s="38"/>
+      <c r="E25" s="46"/>
       <c r="F25" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="36"/>
-      <c r="B26" s="36"/>
-      <c r="C26" s="34"/>
+      <c r="A26" s="44"/>
+      <c r="B26" s="44"/>
+      <c r="C26" s="42"/>
       <c r="D26" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="E26" s="38"/>
+      <c r="E26" s="46"/>
       <c r="F26" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="36"/>
-      <c r="B27" s="36"/>
-      <c r="C27" s="34"/>
+      <c r="A27" s="44"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="42"/>
       <c r="D27" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="E27" s="38"/>
+      <c r="E27" s="46"/>
       <c r="F27" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="36"/>
-      <c r="B28" s="36"/>
-      <c r="C28" s="34"/>
+      <c r="A28" s="44"/>
+      <c r="B28" s="44"/>
+      <c r="C28" s="42"/>
       <c r="D28" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="E28" s="38"/>
+      <c r="E28" s="46"/>
       <c r="F28" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="36"/>
-      <c r="B29" s="36"/>
-      <c r="C29" s="34"/>
+      <c r="A29" s="44"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="42"/>
       <c r="D29" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="E29" s="38"/>
+      <c r="E29" s="46"/>
       <c r="F29" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="36"/>
-      <c r="B30" s="36"/>
-      <c r="C30" s="34"/>
+      <c r="A30" s="44"/>
+      <c r="B30" s="44"/>
+      <c r="C30" s="42"/>
       <c r="D30" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="E30" s="38"/>
+      <c r="E30" s="46"/>
       <c r="F30" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="36"/>
-      <c r="B31" s="36"/>
-      <c r="C31" s="35"/>
+      <c r="A31" s="44"/>
+      <c r="B31" s="44"/>
+      <c r="C31" s="43"/>
       <c r="D31" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="E31" s="38"/>
+      <c r="E31" s="46"/>
       <c r="F31" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="36"/>
-      <c r="B32" s="36"/>
-      <c r="C32" s="33">
+      <c r="A32" s="44"/>
+      <c r="B32" s="44"/>
+      <c r="C32" s="41">
         <v>43520997</v>
       </c>
       <c r="D32" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="E32" s="38" t="s">
+      <c r="E32" s="46" t="s">
         <v>55</v>
       </c>
       <c r="F32" s="8" t="s">
@@ -2548,99 +2567,99 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="36"/>
-      <c r="B33" s="36"/>
-      <c r="C33" s="34"/>
+      <c r="A33" s="44"/>
+      <c r="B33" s="44"/>
+      <c r="C33" s="42"/>
       <c r="D33" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="E33" s="38"/>
+      <c r="E33" s="46"/>
       <c r="F33" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="36"/>
-      <c r="B34" s="36"/>
-      <c r="C34" s="34"/>
+      <c r="A34" s="44"/>
+      <c r="B34" s="44"/>
+      <c r="C34" s="42"/>
       <c r="D34" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="E34" s="38"/>
+      <c r="E34" s="46"/>
       <c r="F34" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="36"/>
-      <c r="B35" s="36"/>
-      <c r="C35" s="34"/>
+      <c r="A35" s="44"/>
+      <c r="B35" s="44"/>
+      <c r="C35" s="42"/>
       <c r="D35" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="E35" s="38"/>
+      <c r="E35" s="46"/>
       <c r="F35" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="36"/>
-      <c r="B36" s="36"/>
-      <c r="C36" s="34"/>
+      <c r="A36" s="44"/>
+      <c r="B36" s="44"/>
+      <c r="C36" s="42"/>
       <c r="D36" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="E36" s="38"/>
+      <c r="E36" s="46"/>
       <c r="F36" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="36"/>
-      <c r="B37" s="36"/>
-      <c r="C37" s="34"/>
+      <c r="A37" s="44"/>
+      <c r="B37" s="44"/>
+      <c r="C37" s="42"/>
       <c r="D37" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E37" s="38"/>
+      <c r="E37" s="46"/>
       <c r="F37" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="36"/>
-      <c r="B38" s="36"/>
-      <c r="C38" s="34"/>
+      <c r="A38" s="44"/>
+      <c r="B38" s="44"/>
+      <c r="C38" s="42"/>
       <c r="D38" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="E38" s="38"/>
+      <c r="E38" s="46"/>
       <c r="F38" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="36"/>
-      <c r="B39" s="36"/>
-      <c r="C39" s="35"/>
+      <c r="A39" s="44"/>
+      <c r="B39" s="44"/>
+      <c r="C39" s="43"/>
       <c r="D39" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="E39" s="38"/>
+      <c r="E39" s="46"/>
       <c r="F39" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="36"/>
-      <c r="B40" s="36"/>
-      <c r="C40" s="33">
+      <c r="A40" s="44"/>
+      <c r="B40" s="44"/>
+      <c r="C40" s="41">
         <v>43527460</v>
       </c>
       <c r="D40" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="E40" s="38" t="s">
+      <c r="E40" s="46" t="s">
         <v>56</v>
       </c>
       <c r="F40" s="8" t="s">
@@ -2648,101 +2667,101 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="36"/>
-      <c r="B41" s="36"/>
-      <c r="C41" s="34"/>
+      <c r="A41" s="44"/>
+      <c r="B41" s="44"/>
+      <c r="C41" s="42"/>
       <c r="D41" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="E41" s="38"/>
+      <c r="E41" s="46"/>
       <c r="F41" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="36"/>
-      <c r="B42" s="36"/>
-      <c r="C42" s="34"/>
+      <c r="A42" s="44"/>
+      <c r="B42" s="44"/>
+      <c r="C42" s="42"/>
       <c r="D42" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="E42" s="38"/>
+      <c r="E42" s="46"/>
       <c r="F42" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="36"/>
-      <c r="B43" s="36"/>
-      <c r="C43" s="34"/>
+      <c r="A43" s="44"/>
+      <c r="B43" s="44"/>
+      <c r="C43" s="42"/>
       <c r="D43" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="E43" s="38"/>
+      <c r="E43" s="46"/>
       <c r="F43" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
-      <c r="C44" s="34"/>
+      <c r="A44" s="44"/>
+      <c r="B44" s="44"/>
+      <c r="C44" s="42"/>
       <c r="D44" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="E44" s="38"/>
+      <c r="E44" s="46"/>
       <c r="F44" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
-      <c r="C45" s="34"/>
+      <c r="A45" s="44"/>
+      <c r="B45" s="44"/>
+      <c r="C45" s="42"/>
       <c r="D45" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="E45" s="38"/>
+      <c r="E45" s="46"/>
       <c r="F45" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="36"/>
-      <c r="B46" s="36"/>
-      <c r="C46" s="34"/>
+      <c r="A46" s="44"/>
+      <c r="B46" s="44"/>
+      <c r="C46" s="42"/>
       <c r="D46" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="E46" s="38"/>
+      <c r="E46" s="46"/>
       <c r="F46" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="36"/>
-      <c r="B47" s="36"/>
-      <c r="C47" s="35"/>
+      <c r="A47" s="44"/>
+      <c r="B47" s="44"/>
+      <c r="C47" s="43"/>
       <c r="D47" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="E47" s="38"/>
+      <c r="E47" s="46"/>
       <c r="F47" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="36"/>
-      <c r="B48" s="36">
+      <c r="A48" s="44"/>
+      <c r="B48" s="44">
         <v>2527</v>
       </c>
-      <c r="C48" s="37">
+      <c r="C48" s="45">
         <v>32143454</v>
       </c>
       <c r="D48" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="E48" s="37" t="s">
+      <c r="E48" s="45" t="s">
         <v>97</v>
       </c>
       <c r="F48" s="8" t="s">
@@ -2750,99 +2769,99 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="36"/>
-      <c r="B49" s="36"/>
-      <c r="C49" s="37"/>
+      <c r="A49" s="44"/>
+      <c r="B49" s="44"/>
+      <c r="C49" s="45"/>
       <c r="D49" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="E49" s="37"/>
+      <c r="E49" s="45"/>
       <c r="F49" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="36"/>
-      <c r="B50" s="36"/>
-      <c r="C50" s="37"/>
+      <c r="A50" s="44"/>
+      <c r="B50" s="44"/>
+      <c r="C50" s="45"/>
       <c r="D50" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="E50" s="37"/>
+      <c r="E50" s="45"/>
       <c r="F50" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="36"/>
-      <c r="B51" s="36"/>
-      <c r="C51" s="37"/>
+      <c r="A51" s="44"/>
+      <c r="B51" s="44"/>
+      <c r="C51" s="45"/>
       <c r="D51" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="E51" s="37"/>
+      <c r="E51" s="45"/>
       <c r="F51" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="36"/>
-      <c r="B52" s="36"/>
-      <c r="C52" s="37"/>
+      <c r="A52" s="44"/>
+      <c r="B52" s="44"/>
+      <c r="C52" s="45"/>
       <c r="D52" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="E52" s="37"/>
+      <c r="E52" s="45"/>
       <c r="F52" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="36"/>
-      <c r="B53" s="36"/>
-      <c r="C53" s="37"/>
+      <c r="A53" s="44"/>
+      <c r="B53" s="44"/>
+      <c r="C53" s="45"/>
       <c r="D53" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="E53" s="37"/>
+      <c r="E53" s="45"/>
       <c r="F53" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="36"/>
-      <c r="B54" s="36"/>
-      <c r="C54" s="37"/>
+      <c r="A54" s="44"/>
+      <c r="B54" s="44"/>
+      <c r="C54" s="45"/>
       <c r="D54" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="E54" s="37"/>
+      <c r="E54" s="45"/>
       <c r="F54" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="36"/>
-      <c r="B55" s="36"/>
-      <c r="C55" s="37"/>
+      <c r="A55" s="44"/>
+      <c r="B55" s="44"/>
+      <c r="C55" s="45"/>
       <c r="D55" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="E55" s="37"/>
+      <c r="E55" s="45"/>
       <c r="F55" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="36"/>
-      <c r="B56" s="36"/>
-      <c r="C56" s="37">
+      <c r="A56" s="44"/>
+      <c r="B56" s="44"/>
+      <c r="C56" s="45">
         <v>42790786</v>
       </c>
       <c r="D56" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="E56" s="37" t="s">
+      <c r="E56" s="45" t="s">
         <v>98</v>
       </c>
       <c r="F56" s="8" t="s">
@@ -2850,91 +2869,91 @@
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="36"/>
-      <c r="B57" s="36"/>
-      <c r="C57" s="37"/>
+      <c r="A57" s="44"/>
+      <c r="B57" s="44"/>
+      <c r="C57" s="45"/>
       <c r="D57" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="E57" s="37"/>
+      <c r="E57" s="45"/>
       <c r="F57" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="36"/>
-      <c r="B58" s="36"/>
-      <c r="C58" s="37"/>
+      <c r="A58" s="44"/>
+      <c r="B58" s="44"/>
+      <c r="C58" s="45"/>
       <c r="D58" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="E58" s="37"/>
+      <c r="E58" s="45"/>
       <c r="F58" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="36"/>
-      <c r="B59" s="36"/>
-      <c r="C59" s="37"/>
+      <c r="A59" s="44"/>
+      <c r="B59" s="44"/>
+      <c r="C59" s="45"/>
       <c r="D59" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="E59" s="37"/>
+      <c r="E59" s="45"/>
       <c r="F59" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="36"/>
-      <c r="B60" s="36"/>
-      <c r="C60" s="37"/>
+      <c r="A60" s="44"/>
+      <c r="B60" s="44"/>
+      <c r="C60" s="45"/>
       <c r="D60" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="E60" s="37"/>
+      <c r="E60" s="45"/>
       <c r="F60" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="36"/>
-      <c r="B61" s="36"/>
-      <c r="C61" s="37"/>
+      <c r="A61" s="44"/>
+      <c r="B61" s="44"/>
+      <c r="C61" s="45"/>
       <c r="D61" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="E61" s="37"/>
+      <c r="E61" s="45"/>
       <c r="F61" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="36"/>
-      <c r="B62" s="36"/>
-      <c r="C62" s="37"/>
+      <c r="A62" s="44"/>
+      <c r="B62" s="44"/>
+      <c r="C62" s="45"/>
       <c r="D62" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="E62" s="37"/>
+      <c r="E62" s="45"/>
       <c r="F62" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="36"/>
-      <c r="B63" s="36"/>
-      <c r="C63" s="37"/>
+      <c r="A63" s="44"/>
+      <c r="B63" s="44"/>
+      <c r="C63" s="45"/>
       <c r="D63" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="E63" s="37"/>
+      <c r="E63" s="45"/>
       <c r="F63" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="36" t="s">
+      <c r="A64" s="44" t="s">
         <v>34</v>
       </c>
       <c r="B64" s="4">
@@ -2954,7 +2973,7 @@
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="36"/>
+      <c r="A65" s="44"/>
       <c r="B65" s="4">
         <v>2527</v>
       </c>
@@ -2972,10 +2991,10 @@
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="36" t="s">
+      <c r="A66" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="B66" s="36" t="s">
+      <c r="B66" s="44" t="s">
         <v>51</v>
       </c>
       <c r="C66" s="8" t="s">
@@ -2992,8 +3011,8 @@
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="36"/>
-      <c r="B67" s="36"/>
+      <c r="A67" s="44"/>
+      <c r="B67" s="44"/>
       <c r="C67" s="8" t="s">
         <v>117</v>
       </c>
@@ -3008,8 +3027,8 @@
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="36"/>
-      <c r="B68" s="36"/>
+      <c r="A68" s="44"/>
+      <c r="B68" s="44"/>
       <c r="C68" s="8" t="s">
         <v>118</v>
       </c>
@@ -3024,8 +3043,8 @@
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="36"/>
-      <c r="B69" s="36"/>
+      <c r="A69" s="44"/>
+      <c r="B69" s="44"/>
       <c r="C69" s="8" t="s">
         <v>119</v>
       </c>
@@ -3040,8 +3059,8 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="36"/>
-      <c r="B70" s="36"/>
+      <c r="A70" s="44"/>
+      <c r="B70" s="44"/>
       <c r="C70" s="8" t="s">
         <v>120</v>
       </c>
@@ -3056,8 +3075,8 @@
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="36"/>
-      <c r="B71" s="36"/>
+      <c r="A71" s="44"/>
+      <c r="B71" s="44"/>
       <c r="C71" s="8" t="s">
         <v>121</v>
       </c>
@@ -3072,8 +3091,8 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="36"/>
-      <c r="B72" s="36"/>
+      <c r="A72" s="44"/>
+      <c r="B72" s="44"/>
       <c r="C72" s="8" t="s">
         <v>122</v>
       </c>
@@ -3088,8 +3107,8 @@
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="36"/>
-      <c r="B73" s="36"/>
+      <c r="A73" s="44"/>
+      <c r="B73" s="44"/>
       <c r="C73" s="8" t="s">
         <v>123</v>
       </c>
@@ -3104,8 +3123,8 @@
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="36"/>
-      <c r="B74" s="36"/>
+      <c r="A74" s="44"/>
+      <c r="B74" s="44"/>
       <c r="C74" s="8" t="s">
         <v>124</v>
       </c>
@@ -3120,8 +3139,8 @@
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="36"/>
-      <c r="B75" s="36"/>
+      <c r="A75" s="44"/>
+      <c r="B75" s="44"/>
       <c r="C75" s="8" t="s">
         <v>125</v>
       </c>
@@ -3136,8 +3155,8 @@
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="36"/>
-      <c r="B76" s="36"/>
+      <c r="A76" s="44"/>
+      <c r="B76" s="44"/>
       <c r="C76" s="8" t="s">
         <v>126</v>
       </c>
@@ -3152,8 +3171,8 @@
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="36"/>
-      <c r="B77" s="36"/>
+      <c r="A77" s="44"/>
+      <c r="B77" s="44"/>
       <c r="C77" s="8" t="s">
         <v>127</v>
       </c>
@@ -3168,8 +3187,8 @@
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="36"/>
-      <c r="B78" s="36"/>
+      <c r="A78" s="44"/>
+      <c r="B78" s="44"/>
       <c r="C78" s="8" t="s">
         <v>128</v>
       </c>
@@ -3184,10 +3203,10 @@
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="36" t="s">
+      <c r="A79" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="B79" s="36">
+      <c r="B79" s="44">
         <v>4029</v>
       </c>
       <c r="C79" s="8" t="s">
@@ -3204,8 +3223,8 @@
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="36"/>
-      <c r="B80" s="36"/>
+      <c r="A80" s="44"/>
+      <c r="B80" s="44"/>
       <c r="C80" s="8" t="s">
         <v>146</v>
       </c>
@@ -3220,8 +3239,8 @@
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="36"/>
-      <c r="B81" s="36"/>
+      <c r="A81" s="44"/>
+      <c r="B81" s="44"/>
       <c r="C81" s="8" t="s">
         <v>147</v>
       </c>
@@ -3236,8 +3255,8 @@
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="36"/>
-      <c r="B82" s="36"/>
+      <c r="A82" s="44"/>
+      <c r="B82" s="44"/>
       <c r="C82" s="8" t="s">
         <v>148</v>
       </c>
@@ -3252,8 +3271,8 @@
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="36"/>
-      <c r="B83" s="36"/>
+      <c r="A83" s="44"/>
+      <c r="B83" s="44"/>
       <c r="C83" s="8" t="s">
         <v>149</v>
       </c>
@@ -3268,8 +3287,8 @@
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="36"/>
-      <c r="B84" s="36"/>
+      <c r="A84" s="44"/>
+      <c r="B84" s="44"/>
       <c r="C84" s="8" t="s">
         <v>150</v>
       </c>
@@ -3284,8 +3303,8 @@
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="36"/>
-      <c r="B85" s="36"/>
+      <c r="A85" s="44"/>
+      <c r="B85" s="44"/>
       <c r="C85" s="8" t="s">
         <v>151</v>
       </c>
@@ -3300,7 +3319,7 @@
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="36" t="s">
+      <c r="A86" s="44" t="s">
         <v>37</v>
       </c>
       <c r="B86" s="4">
@@ -3320,7 +3339,7 @@
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="36"/>
+      <c r="A87" s="44"/>
       <c r="B87" s="4">
         <v>3108</v>
       </c>
@@ -3338,7 +3357,7 @@
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="36" t="s">
+      <c r="A88" s="44" t="s">
         <v>39</v>
       </c>
       <c r="B88" s="4">
@@ -3358,7 +3377,7 @@
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="36"/>
+      <c r="A89" s="44"/>
       <c r="B89" s="4">
         <v>3152</v>
       </c>
@@ -3376,7 +3395,7 @@
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="36"/>
+      <c r="A90" s="44"/>
       <c r="B90" s="4">
         <v>3152</v>
       </c>
@@ -3394,7 +3413,7 @@
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="36" t="s">
+      <c r="A91" s="44" t="s">
         <v>38</v>
       </c>
       <c r="B91" s="4">
@@ -3414,7 +3433,7 @@
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="36"/>
+      <c r="A92" s="44"/>
       <c r="B92" s="4">
         <v>3152</v>
       </c>
@@ -3432,7 +3451,7 @@
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="36"/>
+      <c r="A93" s="44"/>
       <c r="B93" s="4">
         <v>3152</v>
       </c>
@@ -3450,7 +3469,7 @@
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="36"/>
+      <c r="A94" s="44"/>
       <c r="B94" s="4">
         <v>3152</v>
       </c>
@@ -3468,7 +3487,7 @@
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="36"/>
+      <c r="A95" s="44"/>
       <c r="B95" s="4">
         <v>3152</v>
       </c>
@@ -3486,7 +3505,7 @@
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="36"/>
+      <c r="A96" s="44"/>
       <c r="B96" s="4">
         <v>3152</v>
       </c>
@@ -3504,7 +3523,7 @@
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="36"/>
+      <c r="A97" s="44"/>
       <c r="B97" s="4">
         <v>3152</v>
       </c>
@@ -3522,7 +3541,7 @@
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="36"/>
+      <c r="A98" s="44"/>
       <c r="B98" s="4">
         <v>3152</v>
       </c>
@@ -3540,7 +3559,7 @@
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="36"/>
+      <c r="A99" s="44"/>
       <c r="B99" s="4">
         <v>3152</v>
       </c>
@@ -3558,7 +3577,7 @@
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="36"/>
+      <c r="A100" s="44"/>
       <c r="B100" s="4">
         <v>3152</v>
       </c>
@@ -3576,7 +3595,7 @@
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="36"/>
+      <c r="A101" s="44"/>
       <c r="B101" s="4">
         <v>3152</v>
       </c>
@@ -3594,7 +3613,7 @@
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" s="36"/>
+      <c r="A102" s="44"/>
       <c r="B102" s="4">
         <v>3152</v>
       </c>
@@ -3612,7 +3631,7 @@
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="36"/>
+      <c r="A103" s="44"/>
       <c r="B103" s="4">
         <v>3108</v>
       </c>
@@ -3630,7 +3649,7 @@
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" s="36"/>
+      <c r="A104" s="44"/>
       <c r="B104" s="4">
         <v>3108</v>
       </c>
@@ -3648,7 +3667,7 @@
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="36"/>
+      <c r="A105" s="44"/>
       <c r="B105" s="4">
         <v>3108</v>
       </c>
@@ -3666,7 +3685,7 @@
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" s="36"/>
+      <c r="A106" s="44"/>
       <c r="B106" s="4">
         <v>3108</v>
       </c>
@@ -3684,7 +3703,7 @@
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107" s="36"/>
+      <c r="A107" s="44"/>
       <c r="B107" s="4">
         <v>3108</v>
       </c>
@@ -3702,7 +3721,7 @@
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A108" s="36"/>
+      <c r="A108" s="44"/>
       <c r="B108" s="4">
         <v>3108</v>
       </c>
@@ -3720,13 +3739,13 @@
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109" s="33" t="s">
+      <c r="A109" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="B109" s="33">
+      <c r="B109" s="41">
         <v>4029</v>
       </c>
-      <c r="C109" s="30">
+      <c r="C109" s="38">
         <v>1128271593</v>
       </c>
       <c r="D109" s="4" t="s">
@@ -3740,9 +3759,9 @@
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A110" s="34"/>
-      <c r="B110" s="34"/>
-      <c r="C110" s="31"/>
+      <c r="A110" s="42"/>
+      <c r="B110" s="42"/>
+      <c r="C110" s="39"/>
       <c r="D110" s="4" t="s">
         <v>189</v>
       </c>
@@ -3754,9 +3773,9 @@
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A111" s="34"/>
-      <c r="B111" s="34"/>
-      <c r="C111" s="31"/>
+      <c r="A111" s="42"/>
+      <c r="B111" s="42"/>
+      <c r="C111" s="39"/>
       <c r="D111" s="4" t="s">
         <v>190</v>
       </c>
@@ -3768,9 +3787,9 @@
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A112" s="34"/>
-      <c r="B112" s="34"/>
-      <c r="C112" s="31"/>
+      <c r="A112" s="42"/>
+      <c r="B112" s="42"/>
+      <c r="C112" s="39"/>
       <c r="D112" s="4" t="s">
         <v>191</v>
       </c>
@@ -3782,9 +3801,9 @@
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A113" s="34"/>
-      <c r="B113" s="34"/>
-      <c r="C113" s="31"/>
+      <c r="A113" s="42"/>
+      <c r="B113" s="42"/>
+      <c r="C113" s="39"/>
       <c r="D113" s="4" t="s">
         <v>192</v>
       </c>
@@ -3796,9 +3815,9 @@
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A114" s="34"/>
-      <c r="B114" s="34"/>
-      <c r="C114" s="31"/>
+      <c r="A114" s="42"/>
+      <c r="B114" s="42"/>
+      <c r="C114" s="39"/>
       <c r="D114" s="4" t="s">
         <v>193</v>
       </c>
@@ -3810,9 +3829,9 @@
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A115" s="34"/>
-      <c r="B115" s="34"/>
-      <c r="C115" s="31"/>
+      <c r="A115" s="42"/>
+      <c r="B115" s="42"/>
+      <c r="C115" s="39"/>
       <c r="D115" s="4" t="s">
         <v>194</v>
       </c>
@@ -3824,9 +3843,9 @@
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A116" s="34"/>
-      <c r="B116" s="34"/>
-      <c r="C116" s="31"/>
+      <c r="A116" s="42"/>
+      <c r="B116" s="42"/>
+      <c r="C116" s="39"/>
       <c r="D116" s="4" t="s">
         <v>195</v>
       </c>
@@ -3838,9 +3857,9 @@
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A117" s="34"/>
-      <c r="B117" s="34"/>
-      <c r="C117" s="31"/>
+      <c r="A117" s="42"/>
+      <c r="B117" s="42"/>
+      <c r="C117" s="39"/>
       <c r="D117" s="4" t="s">
         <v>196</v>
       </c>
@@ -3852,9 +3871,9 @@
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A118" s="34"/>
-      <c r="B118" s="34"/>
-      <c r="C118" s="32"/>
+      <c r="A118" s="42"/>
+      <c r="B118" s="42"/>
+      <c r="C118" s="40"/>
       <c r="D118" s="4" t="s">
         <v>197</v>
       </c>
@@ -3866,9 +3885,9 @@
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A119" s="34"/>
-      <c r="B119" s="34"/>
-      <c r="C119" s="33">
+      <c r="A119" s="42"/>
+      <c r="B119" s="42"/>
+      <c r="C119" s="41">
         <v>43504265</v>
       </c>
       <c r="D119" s="4" t="s">
@@ -3882,9 +3901,9 @@
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A120" s="34"/>
-      <c r="B120" s="34"/>
-      <c r="C120" s="34"/>
+      <c r="A120" s="42"/>
+      <c r="B120" s="42"/>
+      <c r="C120" s="42"/>
       <c r="D120" s="4" t="s">
         <v>199</v>
       </c>
@@ -3896,9 +3915,9 @@
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A121" s="34"/>
-      <c r="B121" s="34"/>
-      <c r="C121" s="34"/>
+      <c r="A121" s="42"/>
+      <c r="B121" s="42"/>
+      <c r="C121" s="42"/>
       <c r="D121" s="4" t="s">
         <v>70</v>
       </c>
@@ -3910,9 +3929,9 @@
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A122" s="34"/>
-      <c r="B122" s="34"/>
-      <c r="C122" s="34"/>
+      <c r="A122" s="42"/>
+      <c r="B122" s="42"/>
+      <c r="C122" s="42"/>
       <c r="D122" s="4" t="s">
         <v>200</v>
       </c>
@@ -3924,9 +3943,9 @@
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A123" s="34"/>
-      <c r="B123" s="34"/>
-      <c r="C123" s="34"/>
+      <c r="A123" s="42"/>
+      <c r="B123" s="42"/>
+      <c r="C123" s="42"/>
       <c r="D123" s="4" t="s">
         <v>71</v>
       </c>
@@ -3938,9 +3957,9 @@
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A124" s="34"/>
-      <c r="B124" s="34"/>
-      <c r="C124" s="34"/>
+      <c r="A124" s="42"/>
+      <c r="B124" s="42"/>
+      <c r="C124" s="42"/>
       <c r="D124" s="4" t="s">
         <v>201</v>
       </c>
@@ -3952,9 +3971,9 @@
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A125" s="34"/>
-      <c r="B125" s="34"/>
-      <c r="C125" s="34"/>
+      <c r="A125" s="42"/>
+      <c r="B125" s="42"/>
+      <c r="C125" s="42"/>
       <c r="D125" s="4" t="s">
         <v>202</v>
       </c>
@@ -3966,9 +3985,9 @@
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A126" s="34"/>
-      <c r="B126" s="35"/>
-      <c r="C126" s="35"/>
+      <c r="A126" s="42"/>
+      <c r="B126" s="43"/>
+      <c r="C126" s="43"/>
       <c r="D126" s="4" t="s">
         <v>72</v>
       </c>
@@ -3980,11 +3999,11 @@
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A127" s="34"/>
-      <c r="B127" s="33">
+      <c r="A127" s="42"/>
+      <c r="B127" s="41">
         <v>2597</v>
       </c>
-      <c r="C127" s="33">
+      <c r="C127" s="41">
         <v>1128278017</v>
       </c>
       <c r="D127" s="4" t="s">
@@ -3998,9 +4017,9 @@
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A128" s="34"/>
-      <c r="B128" s="34"/>
-      <c r="C128" s="34"/>
+      <c r="A128" s="42"/>
+      <c r="B128" s="42"/>
+      <c r="C128" s="42"/>
       <c r="D128" s="4" t="s">
         <v>109</v>
       </c>
@@ -4012,9 +4031,9 @@
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A129" s="34"/>
-      <c r="B129" s="34"/>
-      <c r="C129" s="34"/>
+      <c r="A129" s="42"/>
+      <c r="B129" s="42"/>
+      <c r="C129" s="42"/>
       <c r="D129" s="4" t="s">
         <v>110</v>
       </c>
@@ -4026,9 +4045,9 @@
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A130" s="34"/>
-      <c r="B130" s="34"/>
-      <c r="C130" s="34"/>
+      <c r="A130" s="42"/>
+      <c r="B130" s="42"/>
+      <c r="C130" s="42"/>
       <c r="D130" s="4" t="s">
         <v>203</v>
       </c>
@@ -4040,9 +4059,9 @@
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A131" s="34"/>
-      <c r="B131" s="34"/>
-      <c r="C131" s="34"/>
+      <c r="A131" s="42"/>
+      <c r="B131" s="42"/>
+      <c r="C131" s="42"/>
       <c r="D131" s="4" t="s">
         <v>111</v>
       </c>
@@ -4054,9 +4073,9 @@
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A132" s="34"/>
-      <c r="B132" s="34"/>
-      <c r="C132" s="34"/>
+      <c r="A132" s="42"/>
+      <c r="B132" s="42"/>
+      <c r="C132" s="42"/>
       <c r="D132" s="4" t="s">
         <v>112</v>
       </c>
@@ -4068,9 +4087,9 @@
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A133" s="34"/>
-      <c r="B133" s="34"/>
-      <c r="C133" s="34"/>
+      <c r="A133" s="42"/>
+      <c r="B133" s="42"/>
+      <c r="C133" s="42"/>
       <c r="D133" s="4" t="s">
         <v>113</v>
       </c>
@@ -4082,9 +4101,9 @@
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A134" s="35"/>
-      <c r="B134" s="35"/>
-      <c r="C134" s="35"/>
+      <c r="A134" s="43"/>
+      <c r="B134" s="43"/>
+      <c r="C134" s="43"/>
       <c r="D134" s="4" t="s">
         <v>114</v>
       </c>
@@ -4140,10 +4159,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D185"/>
+  <dimension ref="A1:D200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A147" workbookViewId="0">
-      <selection activeCell="A161" sqref="A161"/>
+    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
+      <selection activeCell="A160" sqref="A160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5554,241 +5573,241 @@
         <v>215</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
+    <row r="101" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="28" t="s">
         <v>233</v>
       </c>
-      <c r="B101" s="19" t="s">
+      <c r="B101" s="29" t="s">
         <v>255</v>
       </c>
-      <c r="C101" s="20" t="s">
+      <c r="C101" s="30" t="s">
         <v>273</v>
       </c>
-      <c r="D101" s="17" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
+      <c r="D101" s="31" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="28" t="s">
         <v>233</v>
       </c>
-      <c r="B102" s="19" t="s">
+      <c r="B102" s="29" t="s">
         <v>263</v>
       </c>
-      <c r="C102" s="20" t="s">
+      <c r="C102" s="30" t="s">
         <v>280</v>
       </c>
-      <c r="D102" s="17" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
+      <c r="D102" s="31" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="28" t="s">
         <v>233</v>
       </c>
-      <c r="B103" s="19" t="s">
+      <c r="B103" s="29" t="s">
         <v>218</v>
       </c>
-      <c r="C103" s="20" t="s">
+      <c r="C103" s="30" t="s">
         <v>227</v>
       </c>
-      <c r="D103" s="17" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
+      <c r="D103" s="31" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="28" t="s">
         <v>233</v>
       </c>
-      <c r="B104" s="19" t="s">
+      <c r="B104" s="29" t="s">
         <v>296</v>
       </c>
-      <c r="C104" s="20" t="s">
+      <c r="C104" s="30" t="s">
         <v>228</v>
       </c>
-      <c r="D104" s="17" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
+      <c r="D104" s="31" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="28" t="s">
         <v>233</v>
       </c>
-      <c r="B105" s="19" t="s">
+      <c r="B105" s="29" t="s">
         <v>271</v>
       </c>
-      <c r="C105" s="20" t="s">
+      <c r="C105" s="30" t="s">
         <v>287</v>
       </c>
-      <c r="D105" s="17" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="1" t="s">
+      <c r="D105" s="31" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="28" t="s">
         <v>233</v>
       </c>
-      <c r="B106" s="19" t="s">
+      <c r="B106" s="29" t="s">
         <v>213</v>
       </c>
-      <c r="C106" s="20" t="s">
+      <c r="C106" s="30" t="s">
         <v>229</v>
       </c>
-      <c r="D106" s="17" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
+      <c r="D106" s="31" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="28" t="s">
         <v>233</v>
       </c>
-      <c r="B107" s="19" t="s">
+      <c r="B107" s="29" t="s">
         <v>256</v>
       </c>
-      <c r="C107" s="20" t="s">
+      <c r="C107" s="30" t="s">
         <v>157</v>
       </c>
-      <c r="D107" s="17" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
+      <c r="D107" s="31" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="28" t="s">
         <v>233</v>
       </c>
-      <c r="B108" s="19" t="s">
+      <c r="B108" s="29" t="s">
         <v>270</v>
       </c>
-      <c r="C108" s="20" t="s">
+      <c r="C108" s="30" t="s">
         <v>156</v>
       </c>
-      <c r="D108" s="17" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
+      <c r="D108" s="31" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="28" t="s">
         <v>233</v>
       </c>
-      <c r="B109" s="19" t="s">
+      <c r="B109" s="29" t="s">
         <v>265</v>
       </c>
-      <c r="C109" s="20" t="s">
+      <c r="C109" s="30" t="s">
         <v>241</v>
       </c>
-      <c r="D109" s="17" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
+      <c r="D109" s="31" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="28" t="s">
         <v>233</v>
       </c>
-      <c r="B110" s="19" t="s">
+      <c r="B110" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="C110" s="20" t="s">
+      <c r="C110" s="30" t="s">
         <v>279</v>
       </c>
-      <c r="D110" s="17" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
+      <c r="D110" s="31" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="28" t="s">
         <v>233</v>
       </c>
-      <c r="B111" s="19" t="s">
+      <c r="B111" s="29" t="s">
         <v>297</v>
       </c>
-      <c r="C111" s="27" t="s">
+      <c r="C111" s="33" t="s">
         <v>298</v>
       </c>
-      <c r="D111" s="17" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="1" t="s">
+      <c r="D111" s="31" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="28" t="s">
         <v>233</v>
       </c>
-      <c r="B112" s="19" t="s">
+      <c r="B112" s="29" t="s">
         <v>210</v>
       </c>
-      <c r="C112" s="20" t="s">
+      <c r="C112" s="30" t="s">
         <v>225</v>
       </c>
-      <c r="D112" s="17" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A113" s="18" t="s">
+      <c r="D112" s="31" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A113" s="34" t="s">
         <v>234</v>
       </c>
-      <c r="B113" s="26" t="s">
+      <c r="B113" s="35" t="s">
         <v>206</v>
       </c>
-      <c r="C113" s="17" t="s">
+      <c r="C113" s="31" t="s">
         <v>228</v>
       </c>
-      <c r="D113" s="17" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A114" s="18" t="s">
+      <c r="D113" s="31" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A114" s="34" t="s">
         <v>234</v>
       </c>
-      <c r="B114" s="17" t="s">
+      <c r="B114" s="31" t="s">
         <v>219</v>
       </c>
-      <c r="C114" s="17" t="s">
+      <c r="C114" s="31" t="s">
         <v>224</v>
       </c>
-      <c r="D114" s="17" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="18" t="s">
+      <c r="D114" s="31" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" s="32" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="34" t="s">
         <v>234</v>
       </c>
-      <c r="B115" s="17" t="s">
+      <c r="B115" s="31" t="s">
         <v>216</v>
       </c>
-      <c r="C115" s="17" t="s">
+      <c r="C115" s="31" t="s">
         <v>230</v>
       </c>
-      <c r="D115" s="17" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A116" s="18" t="s">
+      <c r="D115" s="31" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A116" s="34" t="s">
         <v>234</v>
       </c>
-      <c r="B116" s="17" t="s">
+      <c r="B116" s="31" t="s">
         <v>214</v>
       </c>
-      <c r="C116" s="17" t="s">
+      <c r="C116" s="31" t="s">
         <v>226</v>
       </c>
-      <c r="D116" s="17" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A117" s="18" t="s">
+      <c r="D116" s="31" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A117" s="34" t="s">
         <v>234</v>
       </c>
-      <c r="B117" s="19" t="s">
+      <c r="B117" s="29" t="s">
         <v>255</v>
       </c>
-      <c r="C117" s="20" t="s">
+      <c r="C117" s="30" t="s">
         <v>273</v>
       </c>
-      <c r="D117" s="17" t="s">
+      <c r="D117" s="31" t="s">
         <v>215</v>
       </c>
     </row>
@@ -6354,7 +6373,7 @@
     </row>
     <row r="158" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A158" s="22" t="s">
-        <v>299</v>
+        <v>248</v>
       </c>
       <c r="B158" s="23" t="s">
         <v>219</v>
@@ -6366,227 +6385,227 @@
         <v>215</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="B159" s="29" t="s">
+        <v>263</v>
+      </c>
+      <c r="C159" s="30" t="s">
+        <v>280</v>
+      </c>
+      <c r="D159" s="31" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="B160" s="29" t="s">
+        <v>218</v>
+      </c>
+      <c r="C160" s="30" t="s">
+        <v>227</v>
+      </c>
+      <c r="D160" s="31" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="B161" s="29" t="s">
+        <v>296</v>
+      </c>
+      <c r="C161" s="30" t="s">
+        <v>228</v>
+      </c>
+      <c r="D161" s="31" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="B162" s="29" t="s">
+        <v>271</v>
+      </c>
+      <c r="C162" s="30" t="s">
+        <v>287</v>
+      </c>
+      <c r="D162" s="31" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="B163" s="29" t="s">
+        <v>213</v>
+      </c>
+      <c r="C163" s="30" t="s">
+        <v>229</v>
+      </c>
+      <c r="D163" s="31" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="B164" s="29" t="s">
+        <v>256</v>
+      </c>
+      <c r="C164" s="30" t="s">
+        <v>157</v>
+      </c>
+      <c r="D164" s="31" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="B165" s="29" t="s">
+        <v>270</v>
+      </c>
+      <c r="C165" s="30" t="s">
+        <v>156</v>
+      </c>
+      <c r="D165" s="31" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="B166" s="29" t="s">
+        <v>265</v>
+      </c>
+      <c r="C166" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="D166" s="31" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="B167" s="29" t="s">
+        <v>262</v>
+      </c>
+      <c r="C167" s="30" t="s">
+        <v>279</v>
+      </c>
+      <c r="D167" s="31" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="B168" s="29" t="s">
+        <v>297</v>
+      </c>
+      <c r="C168" s="33" t="s">
+        <v>298</v>
+      </c>
+      <c r="D168" s="31" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="B169" s="29" t="s">
+        <v>210</v>
+      </c>
+      <c r="C169" s="30" t="s">
+        <v>225</v>
+      </c>
+      <c r="D169" s="31" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="B170" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="C170" s="31" t="s">
+        <v>228</v>
+      </c>
+      <c r="D170" s="31" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="B171" s="31" t="s">
+        <v>219</v>
+      </c>
+      <c r="C171" s="31" t="s">
+        <v>224</v>
+      </c>
+      <c r="D171" s="31" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="B172" s="31" t="s">
+        <v>216</v>
+      </c>
+      <c r="C172" s="31" t="s">
+        <v>230</v>
+      </c>
+      <c r="D172" s="31" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="B173" s="31" t="s">
+        <v>214</v>
+      </c>
+      <c r="C173" s="31" t="s">
+        <v>226</v>
+      </c>
+      <c r="D173" s="31" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A174" s="22" t="s">
         <v>249</v>
       </c>
-      <c r="B159" s="23" t="s">
-        <v>219</v>
-      </c>
-      <c r="C159" s="24" t="s">
-        <v>224</v>
-      </c>
-      <c r="D159" s="17" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
-        <v>252</v>
-      </c>
-      <c r="B160" s="12" t="s">
-        <v>264</v>
-      </c>
-      <c r="C160" s="7" t="s">
-        <v>281</v>
-      </c>
-      <c r="D160" s="17" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
-        <v>252</v>
-      </c>
-      <c r="B161" s="12" t="s">
-        <v>240</v>
-      </c>
-      <c r="C161" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="D161" s="17" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A162" t="s">
-        <v>252</v>
-      </c>
-      <c r="B162" s="25" t="s">
-        <v>288</v>
-      </c>
-      <c r="C162" s="18" t="s">
-        <v>272</v>
-      </c>
-      <c r="D162" s="17" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A163" t="s">
-        <v>252</v>
-      </c>
-      <c r="B163" s="25" t="s">
-        <v>289</v>
-      </c>
-      <c r="C163" s="18" t="s">
-        <v>294</v>
-      </c>
-      <c r="D163" s="17" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A164" t="s">
-        <v>252</v>
-      </c>
-      <c r="B164" s="21" t="s">
-        <v>269</v>
-      </c>
-      <c r="C164" s="18" t="s">
-        <v>286</v>
-      </c>
-      <c r="D164" s="17" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
-        <v>252</v>
-      </c>
-      <c r="B165" s="12" t="s">
-        <v>258</v>
-      </c>
-      <c r="C165" s="7" t="s">
-        <v>275</v>
-      </c>
-      <c r="D165" s="17" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
-        <v>252</v>
-      </c>
-      <c r="B166" s="16" t="s">
-        <v>290</v>
-      </c>
-      <c r="C166" s="7" t="s">
-        <v>295</v>
-      </c>
-      <c r="D166" s="17" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A167" t="s">
-        <v>252</v>
-      </c>
-      <c r="B167" s="25" t="s">
-        <v>291</v>
-      </c>
-      <c r="C167" s="18" t="s">
-        <v>239</v>
-      </c>
-      <c r="D167" s="17" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A168" t="s">
-        <v>252</v>
-      </c>
-      <c r="B168" s="21" t="s">
-        <v>250</v>
-      </c>
-      <c r="C168" s="18" t="s">
-        <v>251</v>
-      </c>
-      <c r="D168" s="17" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A169" t="s">
-        <v>252</v>
-      </c>
-      <c r="B169" s="21" t="s">
-        <v>266</v>
-      </c>
-      <c r="C169" s="18" t="s">
-        <v>283</v>
-      </c>
-      <c r="D169" s="17" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
-        <v>252</v>
-      </c>
-      <c r="B170" s="12" t="s">
-        <v>260</v>
-      </c>
-      <c r="C170" s="7" t="s">
-        <v>277</v>
-      </c>
-      <c r="D170" s="17" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
-        <v>252</v>
-      </c>
-      <c r="B171" s="12" t="s">
-        <v>268</v>
-      </c>
-      <c r="C171" s="7" t="s">
-        <v>285</v>
-      </c>
-      <c r="D171" s="17" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="172" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A172" t="s">
-        <v>252</v>
-      </c>
-      <c r="B172" s="25" t="s">
-        <v>292</v>
-      </c>
-      <c r="C172" s="18" t="s">
-        <v>276</v>
-      </c>
-      <c r="D172" s="17" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="173" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A173" t="s">
-        <v>252</v>
-      </c>
-      <c r="B173" s="21" t="s">
-        <v>242</v>
-      </c>
-      <c r="C173" s="18" t="s">
-        <v>243</v>
-      </c>
-      <c r="D173" s="17" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
-        <v>252</v>
-      </c>
-      <c r="B174" s="12" t="s">
-        <v>257</v>
-      </c>
-      <c r="C174" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="D174" s="17" t="s">
+      <c r="B174" s="29" t="s">
+        <v>255</v>
+      </c>
+      <c r="C174" s="30" t="s">
+        <v>273</v>
+      </c>
+      <c r="D174" s="31" t="s">
         <v>215</v>
       </c>
     </row>
@@ -6595,24 +6614,24 @@
         <v>252</v>
       </c>
       <c r="B175" s="12" t="s">
-        <v>246</v>
+        <v>264</v>
       </c>
       <c r="C175" s="7" t="s">
-        <v>241</v>
+        <v>281</v>
       </c>
       <c r="D175" s="17" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="176" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>252</v>
       </c>
-      <c r="B176" s="25" t="s">
-        <v>293</v>
-      </c>
-      <c r="C176" s="18" t="s">
-        <v>243</v>
+      <c r="B176" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="C176" s="7" t="s">
+        <v>241</v>
       </c>
       <c r="D176" s="17" t="s">
         <v>215</v>
@@ -6622,11 +6641,11 @@
       <c r="A177" t="s">
         <v>252</v>
       </c>
-      <c r="B177" s="21" t="s">
-        <v>242</v>
+      <c r="B177" s="25" t="s">
+        <v>288</v>
       </c>
       <c r="C177" s="18" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="D177" s="17" t="s">
         <v>215</v>
@@ -6636,95 +6655,95 @@
       <c r="A178" t="s">
         <v>252</v>
       </c>
-      <c r="B178" s="21" t="s">
-        <v>267</v>
+      <c r="B178" s="25" t="s">
+        <v>289</v>
       </c>
       <c r="C178" s="18" t="s">
-        <v>284</v>
+        <v>294</v>
       </c>
       <c r="D178" s="17" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="179" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A179" s="22" t="s">
-        <v>248</v>
-      </c>
-      <c r="B179" s="23" t="s">
-        <v>208</v>
-      </c>
-      <c r="C179" s="24" t="s">
-        <v>223</v>
+      <c r="A179" t="s">
+        <v>252</v>
+      </c>
+      <c r="B179" s="21" t="s">
+        <v>269</v>
+      </c>
+      <c r="C179" s="18" t="s">
+        <v>286</v>
       </c>
       <c r="D179" s="17" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="180" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A180" s="22" t="s">
-        <v>253</v>
-      </c>
-      <c r="B180" s="23" t="s">
-        <v>240</v>
-      </c>
-      <c r="C180" s="24" t="s">
-        <v>241</v>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>252</v>
+      </c>
+      <c r="B180" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="C180" s="7" t="s">
+        <v>275</v>
       </c>
       <c r="D180" s="17" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="181" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A181" s="22" t="s">
-        <v>253</v>
-      </c>
-      <c r="B181" s="23" t="s">
-        <v>232</v>
-      </c>
-      <c r="C181" s="24" t="s">
-        <v>220</v>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>252</v>
+      </c>
+      <c r="B181" s="16" t="s">
+        <v>290</v>
+      </c>
+      <c r="C181" s="7" t="s">
+        <v>295</v>
       </c>
       <c r="D181" s="17" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="182" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A182" s="22" t="s">
-        <v>253</v>
-      </c>
-      <c r="B182" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C182" s="24" t="s">
-        <v>247</v>
+      <c r="A182" t="s">
+        <v>252</v>
+      </c>
+      <c r="B182" s="25" t="s">
+        <v>291</v>
+      </c>
+      <c r="C182" s="18" t="s">
+        <v>239</v>
       </c>
       <c r="D182" s="17" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="183" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A183" s="22" t="s">
-        <v>253</v>
-      </c>
-      <c r="B183" s="23" t="s">
-        <v>242</v>
-      </c>
-      <c r="C183" s="24" t="s">
-        <v>243</v>
+      <c r="A183" t="s">
+        <v>252</v>
+      </c>
+      <c r="B183" s="21" t="s">
+        <v>250</v>
+      </c>
+      <c r="C183" s="18" t="s">
+        <v>251</v>
       </c>
       <c r="D183" s="17" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="184" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A184" s="22" t="s">
-        <v>253</v>
-      </c>
-      <c r="B184" s="23" t="s">
-        <v>244</v>
-      </c>
-      <c r="C184" s="24" t="s">
-        <v>245</v>
+      <c r="A184" t="s">
+        <v>252</v>
+      </c>
+      <c r="B184" s="21" t="s">
+        <v>266</v>
+      </c>
+      <c r="C184" s="18" t="s">
+        <v>283</v>
       </c>
       <c r="D184" s="17" t="s">
         <v>215</v>
@@ -6732,6 +6751,216 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
+        <v>252</v>
+      </c>
+      <c r="B185" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="C185" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="D185" s="17" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>252</v>
+      </c>
+      <c r="B186" s="12" t="s">
+        <v>268</v>
+      </c>
+      <c r="C186" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="D186" s="17" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A187" t="s">
+        <v>252</v>
+      </c>
+      <c r="B187" s="25" t="s">
+        <v>292</v>
+      </c>
+      <c r="C187" s="18" t="s">
+        <v>276</v>
+      </c>
+      <c r="D187" s="17" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A188" t="s">
+        <v>252</v>
+      </c>
+      <c r="B188" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="C188" s="18" t="s">
+        <v>243</v>
+      </c>
+      <c r="D188" s="17" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>252</v>
+      </c>
+      <c r="B189" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C189" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="D189" s="17" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>252</v>
+      </c>
+      <c r="B190" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="C190" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="D190" s="17" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A191" t="s">
+        <v>252</v>
+      </c>
+      <c r="B191" s="25" t="s">
+        <v>293</v>
+      </c>
+      <c r="C191" s="18" t="s">
+        <v>243</v>
+      </c>
+      <c r="D191" s="17" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A192" t="s">
+        <v>252</v>
+      </c>
+      <c r="B192" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="C192" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="D192" s="17" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A193" t="s">
+        <v>252</v>
+      </c>
+      <c r="B193" s="21" t="s">
+        <v>267</v>
+      </c>
+      <c r="C193" s="18" t="s">
+        <v>284</v>
+      </c>
+      <c r="D193" s="17" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A194" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="B194" s="23" t="s">
+        <v>208</v>
+      </c>
+      <c r="C194" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="D194" s="17" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A195" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="B195" s="23" t="s">
+        <v>240</v>
+      </c>
+      <c r="C195" s="24" t="s">
+        <v>241</v>
+      </c>
+      <c r="D195" s="17" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A196" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="B196" s="23" t="s">
+        <v>232</v>
+      </c>
+      <c r="C196" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="D196" s="17" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A197" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="B197" s="23" t="s">
+        <v>246</v>
+      </c>
+      <c r="C197" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="D197" s="17" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A198" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="B198" s="23" t="s">
+        <v>242</v>
+      </c>
+      <c r="C198" s="24" t="s">
+        <v>243</v>
+      </c>
+      <c r="D198" s="17" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A199" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="B199" s="23" t="s">
+        <v>244</v>
+      </c>
+      <c r="C199" s="24" t="s">
+        <v>245</v>
+      </c>
+      <c r="D199" s="17" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
         <v>249</v>
       </c>
     </row>

</xml_diff>